<commit_message>
added new icons for recent requests
</commit_message>
<xml_diff>
--- a/assets/icons/bowtie.xlsx
+++ b/assets/icons/bowtie.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2642" uniqueCount="1059">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2741" uniqueCount="1158">
   <si>
     <t>uE709-edit-outline.svg</t>
   </si>
@@ -3197,6 +3197,303 @@
   </si>
   <si>
     <t>current filename cw</t>
+  </si>
+  <si>
+    <t>watch-eye-fill.svg</t>
+  </si>
+  <si>
+    <t>blur.svg</t>
+  </si>
+  <si>
+    <t>camera.svg</t>
+  </si>
+  <si>
+    <t>test-user.svg</t>
+  </si>
+  <si>
+    <t>trigger.svg</t>
+  </si>
+  <si>
+    <t>trigger-auto.svg</t>
+  </si>
+  <si>
+    <t>trigger-user.svg</t>
+  </si>
+  <si>
+    <t>variable.svg</t>
+  </si>
+  <si>
+    <t>test-fill.svg</t>
+  </si>
+  <si>
+    <t>devices.svg</t>
+  </si>
+  <si>
+    <t>format-font.svg</t>
+  </si>
+  <si>
+    <t>merge-duplicate.svg</t>
+  </si>
+  <si>
+    <t>deploy.svg</t>
+  </si>
+  <si>
+    <t>redeploy.svg</t>
+  </si>
+  <si>
+    <t>step.svg</t>
+  </si>
+  <si>
+    <t>robot.svg</t>
+  </si>
+  <si>
+    <t>log.svg</t>
+  </si>
+  <si>
+    <t>server.svg</t>
+  </si>
+  <si>
+    <t>environment.svg</t>
+  </si>
+  <si>
+    <t>test.svg</t>
+  </si>
+  <si>
+    <t>test-auto.svg</t>
+  </si>
+  <si>
+    <t>test-auto-fill.svg</t>
+  </si>
+  <si>
+    <t>test-user-fill.svg</t>
+  </si>
+  <si>
+    <t>test-explore-fill.svg</t>
+  </si>
+  <si>
+    <t>brand-mtm.svg</t>
+  </si>
+  <si>
+    <t>print.svg</t>
+  </si>
+  <si>
+    <t>arrow-open.svg</t>
+  </si>
+  <si>
+    <t>save-all.svg</t>
+  </si>
+  <si>
+    <t>step-shared.svg</t>
+  </si>
+  <si>
+    <t>group-rows.svg</t>
+  </si>
+  <si>
+    <t>arrow-export.svg</t>
+  </si>
+  <si>
+    <t>toggle-tree-expanded-outline.svg</t>
+  </si>
+  <si>
+    <t>video.svg</t>
+  </si>
+  <si>
+    <t>uEA62-watch-eye-fill.svg</t>
+  </si>
+  <si>
+    <t>uEA63-blur.svg</t>
+  </si>
+  <si>
+    <t>uEA64-camera.svg</t>
+  </si>
+  <si>
+    <t>uEA65-test-user.svg</t>
+  </si>
+  <si>
+    <t>uEA66-trigger.svg</t>
+  </si>
+  <si>
+    <t>uEA67-trigger-auto.svg</t>
+  </si>
+  <si>
+    <t>uEA68-trigger-user.svg</t>
+  </si>
+  <si>
+    <t>uEA69-variable.svg</t>
+  </si>
+  <si>
+    <t>uEA6A-test-fill.svg</t>
+  </si>
+  <si>
+    <t>uEA6B-devices.svg</t>
+  </si>
+  <si>
+    <t>uEA6C-format-font.svg</t>
+  </si>
+  <si>
+    <t>uEA6D-merge-duplicate.svg</t>
+  </si>
+  <si>
+    <t>uEA6E-deploy.svg</t>
+  </si>
+  <si>
+    <t>uEA6F-redeploy.svg</t>
+  </si>
+  <si>
+    <t>uEA70-step.svg</t>
+  </si>
+  <si>
+    <t>uEA71-robot.svg</t>
+  </si>
+  <si>
+    <t>uEA72-log.svg</t>
+  </si>
+  <si>
+    <t>uEA73-server.svg</t>
+  </si>
+  <si>
+    <t>uEA74-environment.svg</t>
+  </si>
+  <si>
+    <t>uEA75-test.svg</t>
+  </si>
+  <si>
+    <t>uEA76-test-auto.svg</t>
+  </si>
+  <si>
+    <t>uEA77-test-auto-fill.svg</t>
+  </si>
+  <si>
+    <t>uEA78-test-user-fill.svg</t>
+  </si>
+  <si>
+    <t>uEA79-test-explore-fill.svg</t>
+  </si>
+  <si>
+    <t>uEA7A-brand-mtm.svg</t>
+  </si>
+  <si>
+    <t>uEA7B-print.svg</t>
+  </si>
+  <si>
+    <t>uEA7C-arrow-open.svg</t>
+  </si>
+  <si>
+    <t>uEA7D-save-all.svg</t>
+  </si>
+  <si>
+    <t>uEA7E-step-shared.svg</t>
+  </si>
+  <si>
+    <t>uEA7F-group-rows.svg</t>
+  </si>
+  <si>
+    <t>uEA80-arrow-export.svg</t>
+  </si>
+  <si>
+    <t>uEA81-toggle-tree-expanded-outline.svg</t>
+  </si>
+  <si>
+    <t>uEA82-video.svg</t>
+  </si>
+  <si>
+    <t>uEA62</t>
+  </si>
+  <si>
+    <t>uEA63</t>
+  </si>
+  <si>
+    <t>uEA64</t>
+  </si>
+  <si>
+    <t>uEA65</t>
+  </si>
+  <si>
+    <t>uEA66</t>
+  </si>
+  <si>
+    <t>uEA67</t>
+  </si>
+  <si>
+    <t>uEA68</t>
+  </si>
+  <si>
+    <t>uEA69</t>
+  </si>
+  <si>
+    <t>uEA6A</t>
+  </si>
+  <si>
+    <t>uEA6B</t>
+  </si>
+  <si>
+    <t>uEA6C</t>
+  </si>
+  <si>
+    <t>uEA6D</t>
+  </si>
+  <si>
+    <t>uEA6E</t>
+  </si>
+  <si>
+    <t>uEA6F</t>
+  </si>
+  <si>
+    <t>uEA70</t>
+  </si>
+  <si>
+    <t>uEA71</t>
+  </si>
+  <si>
+    <t>uEA72</t>
+  </si>
+  <si>
+    <t>uEA73</t>
+  </si>
+  <si>
+    <t>uEA74</t>
+  </si>
+  <si>
+    <t>uEA75</t>
+  </si>
+  <si>
+    <t>uEA76</t>
+  </si>
+  <si>
+    <t>uEA77</t>
+  </si>
+  <si>
+    <t>uEA78</t>
+  </si>
+  <si>
+    <t>uEA79</t>
+  </si>
+  <si>
+    <t>uEA7A</t>
+  </si>
+  <si>
+    <t>uEA7B</t>
+  </si>
+  <si>
+    <t>uEA7C</t>
+  </si>
+  <si>
+    <t>uEA7D</t>
+  </si>
+  <si>
+    <t>uEA7E</t>
+  </si>
+  <si>
+    <t>uEA7F</t>
+  </si>
+  <si>
+    <t>uEA80</t>
+  </si>
+  <si>
+    <t>uEA81</t>
+  </si>
+  <si>
+    <t>uEA82</t>
   </si>
 </sst>
 </file>
@@ -3245,12 +3542,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -31117,22 +31415,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K263"/>
+  <dimension ref="A1:K296"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A254" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G259" sqref="G259"/>
+      <pane ySplit="1" topLeftCell="A258" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G262" sqref="G262"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="5" width="15" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15" style="4" customWidth="1"/>
+    <col min="5" max="5" width="15" style="1" customWidth="1"/>
     <col min="6" max="6" width="15.42578125" style="1" customWidth="1"/>
     <col min="7" max="7" width="17.85546875" style="1" customWidth="1"/>
     <col min="8" max="8" width="15.5703125" style="1" customWidth="1"/>
     <col min="9" max="9" width="21.42578125" customWidth="1"/>
     <col min="10" max="10" width="24" customWidth="1"/>
     <col min="11" max="11" width="13.7109375" customWidth="1"/>
+    <col min="14" max="14" width="29.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="2" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -31145,7 +31445,7 @@
       <c r="C1" s="2" t="s">
         <v>793</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="5" t="s">
         <v>794</v>
       </c>
       <c r="E1" s="3" t="s">
@@ -31177,7 +31477,7 @@
       <c r="C2" t="s">
         <v>519</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="4">
         <v>1795</v>
       </c>
       <c r="E2" s="4" t="s">
@@ -31206,7 +31506,7 @@
       <c r="C3" t="s">
         <v>521</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="4">
         <v>1797</v>
       </c>
       <c r="E3" s="4" t="s">
@@ -31235,7 +31535,7 @@
       <c r="C4" t="s">
         <v>425</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="4">
         <v>1539</v>
       </c>
       <c r="E4" s="4" t="s">
@@ -31264,7 +31564,7 @@
       <c r="C5" t="s">
         <v>426</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="4">
         <v>1540</v>
       </c>
       <c r="E5" s="4" t="s">
@@ -31293,7 +31593,7 @@
       <c r="C6" t="s">
         <v>427</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="4">
         <v>1541</v>
       </c>
       <c r="E6" s="4" t="s">
@@ -31322,7 +31622,7 @@
       <c r="C7" t="s">
         <v>520</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="4">
         <v>1796</v>
       </c>
       <c r="E7" s="4" t="s">
@@ -31351,7 +31651,7 @@
       <c r="C8" t="s">
         <v>518</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="4">
         <v>1794</v>
       </c>
       <c r="E8" s="4" t="s">
@@ -31380,7 +31680,7 @@
       <c r="C9" t="s">
         <v>428</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="4">
         <v>1542</v>
       </c>
       <c r="E9" s="4" t="s">
@@ -31409,7 +31709,7 @@
       <c r="C10" t="s">
         <v>422</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="4">
         <v>1536</v>
       </c>
       <c r="E10" s="4" t="s">
@@ -31438,7 +31738,7 @@
       <c r="C11" t="s">
         <v>423</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="4">
         <v>1537</v>
       </c>
       <c r="E11" s="4" t="s">
@@ -31467,7 +31767,7 @@
       <c r="C12" t="s">
         <v>424</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="4">
         <v>1538</v>
       </c>
       <c r="E12" s="4" t="s">
@@ -31496,7 +31796,7 @@
       <c r="C13" t="s">
         <v>429</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13" s="4">
         <v>1543</v>
       </c>
       <c r="E13" s="4" t="s">
@@ -31525,7 +31825,7 @@
       <c r="C14" t="s">
         <v>326</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14" s="4">
         <v>1753</v>
       </c>
       <c r="E14" s="4" t="s">
@@ -31554,7 +31854,7 @@
       <c r="C15" t="s">
         <v>430</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15" s="4">
         <v>1544</v>
       </c>
       <c r="E15" s="4" t="s">
@@ -31583,7 +31883,7 @@
       <c r="C16" t="s">
         <v>431</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16" s="4">
         <v>1545</v>
       </c>
       <c r="E16" s="4" t="s">
@@ -31612,7 +31912,7 @@
       <c r="C17" t="s">
         <v>275</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D17" s="4">
         <v>1700</v>
       </c>
       <c r="E17" s="4" t="s">
@@ -31641,7 +31941,7 @@
       <c r="C18" t="s">
         <v>276</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D18" s="4">
         <v>1701</v>
       </c>
       <c r="E18" s="4" t="s">
@@ -31670,7 +31970,7 @@
       <c r="C19" t="s">
         <v>277</v>
       </c>
-      <c r="D19" s="1">
+      <c r="D19" s="4">
         <v>1702</v>
       </c>
       <c r="E19" s="4" t="s">
@@ -31699,7 +31999,7 @@
       <c r="C20" t="s">
         <v>278</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D20" s="4">
         <v>1703</v>
       </c>
       <c r="E20" s="4" t="s">
@@ -31728,7 +32028,7 @@
       <c r="C21" t="s">
         <v>298</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D21" s="4">
         <v>1725</v>
       </c>
       <c r="E21" s="4" t="s">
@@ -31757,7 +32057,7 @@
       <c r="C22" t="s">
         <v>296</v>
       </c>
-      <c r="D22" s="1">
+      <c r="D22" s="4">
         <v>1723</v>
       </c>
       <c r="E22" s="4" t="s">
@@ -31786,7 +32086,7 @@
       <c r="C23" t="s">
         <v>279</v>
       </c>
-      <c r="D23" s="1">
+      <c r="D23" s="4">
         <v>1704</v>
       </c>
       <c r="E23" s="4" t="s">
@@ -31815,7 +32115,7 @@
       <c r="C24" t="s">
         <v>280</v>
       </c>
-      <c r="D24" s="1">
+      <c r="D24" s="4">
         <v>1705</v>
       </c>
       <c r="E24" s="4" t="s">
@@ -31844,7 +32144,7 @@
       <c r="C25" t="s">
         <v>281</v>
       </c>
-      <c r="D25" s="1">
+      <c r="D25" s="4">
         <v>1706</v>
       </c>
       <c r="E25" s="4" t="s">
@@ -31873,7 +32173,7 @@
       <c r="C26" t="s">
         <v>282</v>
       </c>
-      <c r="D26" s="1">
+      <c r="D26" s="4">
         <v>1707</v>
       </c>
       <c r="E26" s="4" t="s">
@@ -31902,7 +32202,7 @@
       <c r="C27" t="s">
         <v>283</v>
       </c>
-      <c r="D27" s="1">
+      <c r="D27" s="4">
         <v>1708</v>
       </c>
       <c r="E27" s="4" t="s">
@@ -31931,7 +32231,7 @@
       <c r="C28" t="s">
         <v>365</v>
       </c>
-      <c r="D28" s="1">
+      <c r="D28" s="4">
         <v>1548</v>
       </c>
       <c r="E28" s="4" t="s">
@@ -31960,7 +32260,7 @@
       <c r="C29" t="s">
         <v>364</v>
       </c>
-      <c r="D29" s="1">
+      <c r="D29" s="4">
         <v>1547</v>
       </c>
       <c r="E29" s="4" t="s">
@@ -31989,7 +32289,7 @@
       <c r="C30" t="s">
         <v>366</v>
       </c>
-      <c r="D30" s="1">
+      <c r="D30" s="4">
         <v>1549</v>
       </c>
       <c r="E30" s="4" t="s">
@@ -32018,7 +32318,7 @@
       <c r="C31" t="s">
         <v>363</v>
       </c>
-      <c r="D31" s="1">
+      <c r="D31" s="4">
         <v>1546</v>
       </c>
       <c r="E31" s="4" t="s">
@@ -32047,7 +32347,7 @@
       <c r="C32" t="s">
         <v>284</v>
       </c>
-      <c r="D32" s="1">
+      <c r="D32" s="4">
         <v>1709</v>
       </c>
       <c r="E32" s="4" t="s">
@@ -32076,7 +32376,7 @@
       <c r="C33" t="s">
         <v>367</v>
       </c>
-      <c r="D33" s="1">
+      <c r="D33" s="4">
         <v>1550</v>
       </c>
       <c r="E33" s="4" t="s">
@@ -32105,7 +32405,7 @@
       <c r="C34" t="s">
         <v>338</v>
       </c>
-      <c r="D34" s="1">
+      <c r="D34" s="4">
         <v>1765</v>
       </c>
       <c r="E34" s="4" t="s">
@@ -32134,7 +32434,7 @@
       <c r="C35" t="s">
         <v>329</v>
       </c>
-      <c r="D35" s="1">
+      <c r="D35" s="4">
         <v>1756</v>
       </c>
       <c r="E35" s="4" t="s">
@@ -32163,7 +32463,7 @@
       <c r="C36" t="s">
         <v>330</v>
       </c>
-      <c r="D36" s="1">
+      <c r="D36" s="4">
         <v>1757</v>
       </c>
       <c r="E36" s="4" t="s">
@@ -32192,7 +32492,7 @@
       <c r="C37" t="s">
         <v>328</v>
       </c>
-      <c r="D37" s="1">
+      <c r="D37" s="4">
         <v>1755</v>
       </c>
       <c r="E37" s="4" t="s">
@@ -32221,7 +32521,7 @@
       <c r="C38" t="s">
         <v>337</v>
       </c>
-      <c r="D38" s="1">
+      <c r="D38" s="4">
         <v>1764</v>
       </c>
       <c r="E38" s="4" t="s">
@@ -32250,7 +32550,7 @@
       <c r="C39" t="s">
         <v>342</v>
       </c>
-      <c r="D39" s="1">
+      <c r="D39" s="4">
         <v>1769</v>
       </c>
       <c r="E39" s="4" t="s">
@@ -32279,7 +32579,7 @@
       <c r="C40" t="s">
         <v>332</v>
       </c>
-      <c r="D40" s="1">
+      <c r="D40" s="4">
         <v>1759</v>
       </c>
       <c r="E40" s="4" t="s">
@@ -32308,7 +32608,7 @@
       <c r="C41" t="s">
         <v>339</v>
       </c>
-      <c r="D41" s="1">
+      <c r="D41" s="4">
         <v>1766</v>
       </c>
       <c r="E41" s="4" t="s">
@@ -32337,7 +32637,7 @@
       <c r="C42" t="s">
         <v>285</v>
       </c>
-      <c r="D42" s="1">
+      <c r="D42" s="4">
         <v>1710</v>
       </c>
       <c r="E42" s="4" t="s">
@@ -32366,7 +32666,7 @@
       <c r="C43" t="s">
         <v>368</v>
       </c>
-      <c r="D43" s="1">
+      <c r="D43" s="4">
         <v>1551</v>
       </c>
       <c r="E43" s="4" t="s">
@@ -32395,7 +32695,7 @@
       <c r="C44" t="s">
         <v>267</v>
       </c>
-      <c r="D44" s="1">
+      <c r="D44" s="4">
         <v>1711</v>
       </c>
       <c r="E44" s="4" t="s">
@@ -32424,7 +32724,7 @@
       <c r="C45" t="s">
         <v>268</v>
       </c>
-      <c r="D45" s="1">
+      <c r="D45" s="4">
         <v>1712</v>
       </c>
       <c r="E45" s="4" t="s">
@@ -32453,7 +32753,7 @@
       <c r="C46" t="s">
         <v>432</v>
       </c>
-      <c r="D46" s="1">
+      <c r="D46" s="4">
         <v>1552</v>
       </c>
       <c r="E46" s="4" t="s">
@@ -32482,7 +32782,7 @@
       <c r="C47" t="s">
         <v>433</v>
       </c>
-      <c r="D47" s="1">
+      <c r="D47" s="4">
         <v>1553</v>
       </c>
       <c r="E47" s="4" t="s">
@@ -32511,7 +32811,7 @@
       <c r="C48" t="s">
         <v>434</v>
       </c>
-      <c r="D48" s="1">
+      <c r="D48" s="4">
         <v>1554</v>
       </c>
       <c r="E48" s="4" t="s">
@@ -32540,7 +32840,7 @@
       <c r="C49" t="s">
         <v>435</v>
       </c>
-      <c r="D49" s="1">
+      <c r="D49" s="4">
         <v>1555</v>
       </c>
       <c r="E49" s="4" t="s">
@@ -32569,7 +32869,7 @@
       <c r="C50" t="s">
         <v>436</v>
       </c>
-      <c r="D50" s="1">
+      <c r="D50" s="4">
         <v>1556</v>
       </c>
       <c r="E50" s="4" t="s">
@@ -32598,7 +32898,7 @@
       <c r="C51" t="s">
         <v>437</v>
       </c>
-      <c r="D51" s="1">
+      <c r="D51" s="4">
         <v>1557</v>
       </c>
       <c r="E51" s="4" t="s">
@@ -32627,7 +32927,7 @@
       <c r="C52" t="s">
         <v>438</v>
       </c>
-      <c r="D52" s="1">
+      <c r="D52" s="4">
         <v>1558</v>
       </c>
       <c r="E52" s="4" t="s">
@@ -32656,7 +32956,7 @@
       <c r="C53" t="s">
         <v>439</v>
       </c>
-      <c r="D53" s="1">
+      <c r="D53" s="4">
         <v>1559</v>
       </c>
       <c r="E53" s="4" t="s">
@@ -32685,7 +32985,7 @@
       <c r="C54" t="s">
         <v>440</v>
       </c>
-      <c r="D54" s="1">
+      <c r="D54" s="4">
         <v>1560</v>
       </c>
       <c r="E54" s="4" t="s">
@@ -32714,7 +33014,7 @@
       <c r="C55" t="s">
         <v>441</v>
       </c>
-      <c r="D55" s="1">
+      <c r="D55" s="4">
         <v>1561</v>
       </c>
       <c r="E55" s="4" t="s">
@@ -32743,7 +33043,7 @@
       <c r="C56" t="s">
         <v>286</v>
       </c>
-      <c r="D56" s="1">
+      <c r="D56" s="4">
         <v>1713</v>
       </c>
       <c r="E56" s="4" t="s">
@@ -32772,7 +33072,7 @@
       <c r="C57" t="s">
         <v>369</v>
       </c>
-      <c r="D57" s="1">
+      <c r="D57" s="4">
         <v>1562</v>
       </c>
       <c r="E57" s="4" t="s">
@@ -32801,7 +33101,7 @@
       <c r="C58" t="s">
         <v>371</v>
       </c>
-      <c r="D58" s="1">
+      <c r="D58" s="4">
         <v>1564</v>
       </c>
       <c r="E58" s="4" t="s">
@@ -32830,7 +33130,7 @@
       <c r="C59" t="s">
         <v>372</v>
       </c>
-      <c r="D59" s="1">
+      <c r="D59" s="4">
         <v>1565</v>
       </c>
       <c r="E59" s="4" t="s">
@@ -32859,7 +33159,7 @@
       <c r="C60" t="s">
         <v>373</v>
       </c>
-      <c r="D60" s="1">
+      <c r="D60" s="4">
         <v>1566</v>
       </c>
       <c r="E60" s="4" t="s">
@@ -32888,7 +33188,7 @@
       <c r="C61" t="s">
         <v>374</v>
       </c>
-      <c r="D61" s="1">
+      <c r="D61" s="4">
         <v>1567</v>
       </c>
       <c r="E61" s="4" t="s">
@@ -32917,7 +33217,7 @@
       <c r="C62" t="s">
         <v>442</v>
       </c>
-      <c r="D62" s="1">
+      <c r="D62" s="4">
         <v>1568</v>
       </c>
       <c r="E62" s="4" t="s">
@@ -32946,7 +33246,7 @@
       <c r="C63" t="s">
         <v>443</v>
       </c>
-      <c r="D63" s="1">
+      <c r="D63" s="4">
         <v>1569</v>
       </c>
       <c r="E63" s="4" t="s">
@@ -32975,7 +33275,7 @@
       <c r="C64" t="s">
         <v>444</v>
       </c>
-      <c r="D64" s="1">
+      <c r="D64" s="4">
         <v>1570</v>
       </c>
       <c r="E64" s="4" t="s">
@@ -33004,7 +33304,7 @@
       <c r="C65" t="s">
         <v>370</v>
       </c>
-      <c r="D65" s="1">
+      <c r="D65" s="4">
         <v>1563</v>
       </c>
       <c r="E65" s="4" t="s">
@@ -33033,7 +33333,7 @@
       <c r="C66" t="s">
         <v>287</v>
       </c>
-      <c r="D66" s="1">
+      <c r="D66" s="4">
         <v>1714</v>
       </c>
       <c r="E66" s="4" t="s">
@@ -33062,7 +33362,7 @@
       <c r="C67" t="s">
         <v>288</v>
       </c>
-      <c r="D67" s="1">
+      <c r="D67" s="4">
         <v>1715</v>
       </c>
       <c r="E67" s="4" t="s">
@@ -33091,7 +33391,7 @@
       <c r="C68" t="s">
         <v>289</v>
       </c>
-      <c r="D68" s="1">
+      <c r="D68" s="4">
         <v>1716</v>
       </c>
       <c r="E68" s="4" t="s">
@@ -33120,7 +33420,7 @@
       <c r="C69" t="s">
         <v>445</v>
       </c>
-      <c r="D69" s="1">
+      <c r="D69" s="4">
         <v>1571</v>
       </c>
       <c r="E69" s="4" t="s">
@@ -33149,7 +33449,7 @@
       <c r="C70" t="s">
         <v>446</v>
       </c>
-      <c r="D70" s="1">
+      <c r="D70" s="4">
         <v>1572</v>
       </c>
       <c r="E70" s="4" t="s">
@@ -33178,7 +33478,7 @@
       <c r="C71" t="s">
         <v>303</v>
       </c>
-      <c r="D71" s="1">
+      <c r="D71" s="4">
         <v>1730</v>
       </c>
       <c r="E71" s="4" t="s">
@@ -33207,7 +33507,7 @@
       <c r="C72" t="s">
         <v>447</v>
       </c>
-      <c r="D72" s="1">
+      <c r="D72" s="4">
         <v>1573</v>
       </c>
       <c r="E72" s="4" t="s">
@@ -33236,7 +33536,7 @@
       <c r="C73" t="s">
         <v>448</v>
       </c>
-      <c r="D73" s="1">
+      <c r="D73" s="4">
         <v>1574</v>
       </c>
       <c r="E73" s="4" t="s">
@@ -33265,7 +33565,7 @@
       <c r="C74" t="s">
         <v>449</v>
       </c>
-      <c r="D74" s="1">
+      <c r="D74" s="4">
         <v>1575</v>
       </c>
       <c r="E74" s="4" t="s">
@@ -33294,7 +33594,7 @@
       <c r="C75" t="s">
         <v>450</v>
       </c>
-      <c r="D75" s="1">
+      <c r="D75" s="4">
         <v>1576</v>
       </c>
       <c r="E75" s="4" t="s">
@@ -33323,7 +33623,7 @@
       <c r="C76" t="s">
         <v>451</v>
       </c>
-      <c r="D76" s="1">
+      <c r="D76" s="4">
         <v>1577</v>
       </c>
       <c r="E76" s="4" t="s">
@@ -33352,7 +33652,7 @@
       <c r="C77" t="s">
         <v>375</v>
       </c>
-      <c r="D77" s="1">
+      <c r="D77" s="4">
         <v>1578</v>
       </c>
       <c r="E77" s="4" t="s">
@@ -33381,7 +33681,7 @@
       <c r="C78" t="s">
         <v>377</v>
       </c>
-      <c r="D78" s="1">
+      <c r="D78" s="4">
         <v>1580</v>
       </c>
       <c r="E78" s="4" t="s">
@@ -33410,7 +33710,7 @@
       <c r="C79" t="s">
         <v>378</v>
       </c>
-      <c r="D79" s="1">
+      <c r="D79" s="4">
         <v>1581</v>
       </c>
       <c r="E79" s="4" t="s">
@@ -33439,7 +33739,7 @@
       <c r="C80" t="s">
         <v>517</v>
       </c>
-      <c r="D80" s="1">
+      <c r="D80" s="4">
         <v>1793</v>
       </c>
       <c r="E80" s="4" t="s">
@@ -33468,7 +33768,7 @@
       <c r="C81" t="s">
         <v>263</v>
       </c>
-      <c r="D81" s="1">
+      <c r="D81" s="4">
         <v>1801</v>
       </c>
       <c r="E81" s="4" t="s">
@@ -33497,7 +33797,7 @@
       <c r="C82" t="s">
         <v>380</v>
       </c>
-      <c r="D82" s="1">
+      <c r="D82" s="4">
         <v>1583</v>
       </c>
       <c r="E82" s="4" t="s">
@@ -33526,7 +33826,7 @@
       <c r="C83" t="s">
         <v>452</v>
       </c>
-      <c r="D83" s="1">
+      <c r="D83" s="4">
         <v>1584</v>
       </c>
       <c r="E83" s="4" t="s">
@@ -33555,7 +33855,7 @@
       <c r="C84" t="s">
         <v>453</v>
       </c>
-      <c r="D84" s="1">
+      <c r="D84" s="4">
         <v>1585</v>
       </c>
       <c r="E84" s="4" t="s">
@@ -33584,7 +33884,7 @@
       <c r="C85" t="s">
         <v>454</v>
       </c>
-      <c r="D85" s="1">
+      <c r="D85" s="4">
         <v>1586</v>
       </c>
       <c r="E85" s="4" t="s">
@@ -33613,7 +33913,7 @@
       <c r="C86" t="s">
         <v>455</v>
       </c>
-      <c r="D86" s="1">
+      <c r="D86" s="4">
         <v>1587</v>
       </c>
       <c r="E86" s="4" t="s">
@@ -33642,7 +33942,7 @@
       <c r="C87" t="s">
         <v>376</v>
       </c>
-      <c r="D87" s="1">
+      <c r="D87" s="4">
         <v>1579</v>
       </c>
       <c r="E87" s="4" t="s">
@@ -33671,7 +33971,7 @@
       <c r="C88" t="s">
         <v>456</v>
       </c>
-      <c r="D88" s="1">
+      <c r="D88" s="4">
         <v>1588</v>
       </c>
       <c r="E88" s="4" t="s">
@@ -33700,7 +34000,7 @@
       <c r="C89" t="s">
         <v>266</v>
       </c>
-      <c r="D89" s="1">
+      <c r="D89" s="4">
         <v>1590</v>
       </c>
       <c r="E89" s="4" t="s">
@@ -33729,7 +34029,7 @@
       <c r="C90" t="s">
         <v>265</v>
       </c>
-      <c r="D90" s="1">
+      <c r="D90" s="4">
         <v>1589</v>
       </c>
       <c r="E90" s="4" t="s">
@@ -33758,7 +34058,7 @@
       <c r="C91" t="s">
         <v>457</v>
       </c>
-      <c r="D91" s="1">
+      <c r="D91" s="4">
         <v>1591</v>
       </c>
       <c r="E91" s="4" t="s">
@@ -33787,7 +34087,7 @@
       <c r="C92" t="s">
         <v>458</v>
       </c>
-      <c r="D92" s="1">
+      <c r="D92" s="4">
         <v>1592</v>
       </c>
       <c r="E92" s="4" t="s">
@@ -33816,7 +34116,7 @@
       <c r="C93" t="s">
         <v>295</v>
       </c>
-      <c r="D93" s="1">
+      <c r="D93" s="4">
         <v>1722</v>
       </c>
       <c r="E93" s="4" t="s">
@@ -33845,7 +34145,7 @@
       <c r="C94" t="s">
         <v>459</v>
       </c>
-      <c r="D94" s="1">
+      <c r="D94" s="4">
         <v>1593</v>
       </c>
       <c r="E94" s="4" t="s">
@@ -33874,7 +34174,7 @@
       <c r="C95" t="s">
         <v>381</v>
       </c>
-      <c r="D95" s="1">
+      <c r="D95" s="4">
         <v>1594</v>
       </c>
       <c r="E95" s="4" t="s">
@@ -33903,7 +34203,7 @@
       <c r="C96" t="s">
         <v>383</v>
       </c>
-      <c r="D96" s="1">
+      <c r="D96" s="4">
         <v>1596</v>
       </c>
       <c r="E96" s="4" t="s">
@@ -33932,7 +34232,7 @@
       <c r="C97" t="s">
         <v>384</v>
       </c>
-      <c r="D97" s="1">
+      <c r="D97" s="4">
         <v>1597</v>
       </c>
       <c r="E97" s="4" t="s">
@@ -33961,7 +34261,7 @@
       <c r="C98" t="s">
         <v>385</v>
       </c>
-      <c r="D98" s="1">
+      <c r="D98" s="4">
         <v>1598</v>
       </c>
       <c r="E98" s="4" t="s">
@@ -33990,7 +34290,7 @@
       <c r="C99" t="s">
         <v>386</v>
       </c>
-      <c r="D99" s="1">
+      <c r="D99" s="4">
         <v>1599</v>
       </c>
       <c r="E99" s="4" t="s">
@@ -34019,7 +34319,7 @@
       <c r="C100" t="s">
         <v>460</v>
       </c>
-      <c r="D100" s="1">
+      <c r="D100" s="4">
         <v>1600</v>
       </c>
       <c r="E100" s="4" t="s">
@@ -34048,7 +34348,7 @@
       <c r="C101" t="s">
         <v>461</v>
       </c>
-      <c r="D101" s="1">
+      <c r="D101" s="4">
         <v>1601</v>
       </c>
       <c r="E101" s="4" t="s">
@@ -34077,7 +34377,7 @@
       <c r="C102" t="s">
         <v>382</v>
       </c>
-      <c r="D102" s="1">
+      <c r="D102" s="4">
         <v>1595</v>
       </c>
       <c r="E102" s="4" t="s">
@@ -34106,7 +34406,7 @@
       <c r="C103" t="s">
         <v>462</v>
       </c>
-      <c r="D103" s="1">
+      <c r="D103" s="4">
         <v>1602</v>
       </c>
       <c r="E103" s="4" t="s">
@@ -34135,7 +34435,7 @@
       <c r="C104" t="s">
         <v>463</v>
       </c>
-      <c r="D104" s="1">
+      <c r="D104" s="4">
         <v>1603</v>
       </c>
       <c r="E104" s="4" t="s">
@@ -34164,7 +34464,7 @@
       <c r="C105" t="s">
         <v>464</v>
       </c>
-      <c r="D105" s="1">
+      <c r="D105" s="4">
         <v>1604</v>
       </c>
       <c r="E105" s="4" t="s">
@@ -34193,7 +34493,7 @@
       <c r="C106" t="s">
         <v>335</v>
       </c>
-      <c r="D106" s="1">
+      <c r="D106" s="4">
         <v>1762</v>
       </c>
       <c r="E106" s="4" t="s">
@@ -34222,7 +34522,7 @@
       <c r="C107" t="s">
         <v>349</v>
       </c>
-      <c r="D107" s="1">
+      <c r="D107" s="4">
         <v>1776</v>
       </c>
       <c r="E107" s="4" t="s">
@@ -34251,7 +34551,7 @@
       <c r="C108" t="s">
         <v>355</v>
       </c>
-      <c r="D108" s="1">
+      <c r="D108" s="4">
         <v>1782</v>
       </c>
       <c r="E108" s="4" t="s">
@@ -34280,7 +34580,7 @@
       <c r="C109" t="s">
         <v>356</v>
       </c>
-      <c r="D109" s="1">
+      <c r="D109" s="4">
         <v>1783</v>
       </c>
       <c r="E109" s="4" t="s">
@@ -34309,7 +34609,7 @@
       <c r="C110" t="s">
         <v>357</v>
       </c>
-      <c r="D110" s="1">
+      <c r="D110" s="4">
         <v>1784</v>
       </c>
       <c r="E110" s="4" t="s">
@@ -34338,7 +34638,7 @@
       <c r="C111" t="s">
         <v>358</v>
       </c>
-      <c r="D111" s="1">
+      <c r="D111" s="4">
         <v>1785</v>
       </c>
       <c r="E111" s="4" t="s">
@@ -34367,7 +34667,7 @@
       <c r="C112" t="s">
         <v>359</v>
       </c>
-      <c r="D112" s="1">
+      <c r="D112" s="4">
         <v>1786</v>
       </c>
       <c r="E112" s="4" t="s">
@@ -34396,7 +34696,7 @@
       <c r="C113" t="s">
         <v>360</v>
       </c>
-      <c r="D113" s="1">
+      <c r="D113" s="4">
         <v>1787</v>
       </c>
       <c r="E113" s="4" t="s">
@@ -34425,7 +34725,7 @@
       <c r="C114" t="s">
         <v>361</v>
       </c>
-      <c r="D114" s="1">
+      <c r="D114" s="4">
         <v>1788</v>
       </c>
       <c r="E114" s="4" t="s">
@@ -34454,7 +34754,7 @@
       <c r="C115" t="s">
         <v>362</v>
       </c>
-      <c r="D115" s="1">
+      <c r="D115" s="4">
         <v>1789</v>
       </c>
       <c r="E115" s="4" t="s">
@@ -34483,7 +34783,7 @@
       <c r="C116" t="s">
         <v>465</v>
       </c>
-      <c r="D116" s="1">
+      <c r="D116" s="4">
         <v>1605</v>
       </c>
       <c r="E116" s="4" t="s">
@@ -34512,7 +34812,7 @@
       <c r="C117" t="s">
         <v>300</v>
       </c>
-      <c r="D117" s="1">
+      <c r="D117" s="4">
         <v>1727</v>
       </c>
       <c r="E117" s="4" t="s">
@@ -34541,7 +34841,7 @@
       <c r="C118" t="s">
         <v>301</v>
       </c>
-      <c r="D118" s="1">
+      <c r="D118" s="4">
         <v>1728</v>
       </c>
       <c r="E118" s="4" t="s">
@@ -34570,7 +34870,7 @@
       <c r="C119" t="s">
         <v>302</v>
       </c>
-      <c r="D119" s="1">
+      <c r="D119" s="4">
         <v>1729</v>
       </c>
       <c r="E119" s="4" t="s">
@@ -34599,7 +34899,7 @@
       <c r="C120" t="s">
         <v>466</v>
       </c>
-      <c r="D120" s="1">
+      <c r="D120" s="4">
         <v>1606</v>
       </c>
       <c r="E120" s="4" t="s">
@@ -34628,7 +34928,7 @@
       <c r="C121" t="s">
         <v>304</v>
       </c>
-      <c r="D121" s="1">
+      <c r="D121" s="4">
         <v>1731</v>
       </c>
       <c r="E121" s="4" t="s">
@@ -34657,7 +34957,7 @@
       <c r="C122" t="s">
         <v>467</v>
       </c>
-      <c r="D122" s="1">
+      <c r="D122" s="4">
         <v>1607</v>
       </c>
       <c r="E122" s="4" t="s">
@@ -34686,7 +34986,7 @@
       <c r="C123" t="s">
         <v>468</v>
       </c>
-      <c r="D123" s="1">
+      <c r="D123" s="4">
         <v>1608</v>
       </c>
       <c r="E123" s="4" t="s">
@@ -34715,7 +35015,7 @@
       <c r="C124" t="s">
         <v>469</v>
       </c>
-      <c r="D124" s="1">
+      <c r="D124" s="4">
         <v>1609</v>
       </c>
       <c r="E124" s="4" t="s">
@@ -34744,7 +35044,7 @@
       <c r="C125" t="s">
         <v>305</v>
       </c>
-      <c r="D125" s="1">
+      <c r="D125" s="4">
         <v>1732</v>
       </c>
       <c r="E125" s="4" t="s">
@@ -34773,7 +35073,7 @@
       <c r="C126" t="s">
         <v>387</v>
       </c>
-      <c r="D126" s="1">
+      <c r="D126" s="4">
         <v>1611</v>
       </c>
       <c r="E126" s="4" t="s">
@@ -34802,7 +35102,7 @@
       <c r="C127" t="s">
         <v>271</v>
       </c>
-      <c r="D127" s="1">
+      <c r="D127" s="4">
         <v>1790</v>
       </c>
       <c r="E127" s="4" t="s">
@@ -34831,7 +35131,7 @@
       <c r="C128" t="s">
         <v>389</v>
       </c>
-      <c r="D128" s="1">
+      <c r="D128" s="4">
         <v>1613</v>
       </c>
       <c r="E128" s="4" t="s">
@@ -34860,7 +35160,7 @@
       <c r="C129" t="s">
         <v>306</v>
       </c>
-      <c r="D129" s="1">
+      <c r="D129" s="4">
         <v>1733</v>
       </c>
       <c r="E129" s="4" t="s">
@@ -34889,7 +35189,7 @@
       <c r="C130" t="s">
         <v>390</v>
       </c>
-      <c r="D130" s="1">
+      <c r="D130" s="4">
         <v>1614</v>
       </c>
       <c r="E130" s="4" t="s">
@@ -34918,7 +35218,7 @@
       <c r="C131" t="s">
         <v>307</v>
       </c>
-      <c r="D131" s="1">
+      <c r="D131" s="4">
         <v>1734</v>
       </c>
       <c r="E131" s="4" t="s">
@@ -34947,7 +35247,7 @@
       <c r="C132" t="s">
         <v>388</v>
       </c>
-      <c r="D132" s="1">
+      <c r="D132" s="4">
         <v>1612</v>
       </c>
       <c r="E132" s="4" t="s">
@@ -34976,7 +35276,7 @@
       <c r="C133" t="s">
         <v>270</v>
       </c>
-      <c r="D133" s="1">
+      <c r="D133" s="4">
         <v>1791</v>
       </c>
       <c r="E133" s="4" t="s">
@@ -35005,7 +35305,7 @@
       <c r="C134" t="s">
         <v>308</v>
       </c>
-      <c r="D134" s="1">
+      <c r="D134" s="4">
         <v>1735</v>
       </c>
       <c r="E134" s="4" t="s">
@@ -35034,7 +35334,7 @@
       <c r="C135" t="s">
         <v>309</v>
       </c>
-      <c r="D135" s="1">
+      <c r="D135" s="4">
         <v>1736</v>
       </c>
       <c r="E135" s="4" t="s">
@@ -35063,7 +35363,7 @@
       <c r="C136" t="s">
         <v>310</v>
       </c>
-      <c r="D136" s="1">
+      <c r="D136" s="4">
         <v>1737</v>
       </c>
       <c r="E136" s="4" t="s">
@@ -35092,7 +35392,7 @@
       <c r="C137" t="s">
         <v>391</v>
       </c>
-      <c r="D137" s="1">
+      <c r="D137" s="4">
         <v>1615</v>
       </c>
       <c r="E137" s="4" t="s">
@@ -35121,7 +35421,7 @@
       <c r="C138" t="s">
         <v>269</v>
       </c>
-      <c r="D138" s="1">
+      <c r="D138" s="4">
         <v>1792</v>
       </c>
       <c r="E138" s="4" t="s">
@@ -35150,7 +35450,7 @@
       <c r="C139" t="s">
         <v>470</v>
       </c>
-      <c r="D139" s="1">
+      <c r="D139" s="4">
         <v>1616</v>
       </c>
       <c r="E139" s="4" t="s">
@@ -35179,7 +35479,7 @@
       <c r="C140" t="s">
         <v>311</v>
       </c>
-      <c r="D140" s="1">
+      <c r="D140" s="4">
         <v>1738</v>
       </c>
       <c r="E140" s="4" t="s">
@@ -35208,7 +35508,7 @@
       <c r="C141" t="s">
         <v>471</v>
       </c>
-      <c r="D141" s="1">
+      <c r="D141" s="4">
         <v>1617</v>
       </c>
       <c r="E141" s="4" t="s">
@@ -35237,7 +35537,7 @@
       <c r="C142" t="s">
         <v>472</v>
       </c>
-      <c r="D142" s="1">
+      <c r="D142" s="4">
         <v>1618</v>
       </c>
       <c r="E142" s="4" t="s">
@@ -35266,7 +35566,7 @@
       <c r="C143" t="s">
         <v>312</v>
       </c>
-      <c r="D143" s="1">
+      <c r="D143" s="4">
         <v>1739</v>
       </c>
       <c r="E143" s="4" t="s">
@@ -35295,7 +35595,7 @@
       <c r="C144" t="s">
         <v>473</v>
       </c>
-      <c r="D144" s="1">
+      <c r="D144" s="4">
         <v>1619</v>
       </c>
       <c r="E144" s="4" t="s">
@@ -35324,7 +35624,7 @@
       <c r="C145" t="s">
         <v>313</v>
       </c>
-      <c r="D145" s="1">
+      <c r="D145" s="4">
         <v>1740</v>
       </c>
       <c r="E145" s="4" t="s">
@@ -35353,7 +35653,7 @@
       <c r="C146" t="s">
         <v>474</v>
       </c>
-      <c r="D146" s="1">
+      <c r="D146" s="4">
         <v>1620</v>
       </c>
       <c r="E146" s="4" t="s">
@@ -35382,7 +35682,7 @@
       <c r="C147" t="s">
         <v>475</v>
       </c>
-      <c r="D147" s="1">
+      <c r="D147" s="4">
         <v>1621</v>
       </c>
       <c r="E147" s="4" t="s">
@@ -35411,7 +35711,7 @@
       <c r="C148" t="s">
         <v>476</v>
       </c>
-      <c r="D148" s="1">
+      <c r="D148" s="4">
         <v>1622</v>
       </c>
       <c r="E148" s="4" t="s">
@@ -35440,7 +35740,7 @@
       <c r="C149" t="s">
         <v>477</v>
       </c>
-      <c r="D149" s="1">
+      <c r="D149" s="4">
         <v>1623</v>
       </c>
       <c r="E149" s="4" t="s">
@@ -35469,7 +35769,7 @@
       <c r="C150" t="s">
         <v>478</v>
       </c>
-      <c r="D150" s="1">
+      <c r="D150" s="4">
         <v>1624</v>
       </c>
       <c r="E150" s="4" t="s">
@@ -35498,7 +35798,7 @@
       <c r="C151" t="s">
         <v>479</v>
       </c>
-      <c r="D151" s="1">
+      <c r="D151" s="4">
         <v>1625</v>
       </c>
       <c r="E151" s="4" t="s">
@@ -35527,7 +35827,7 @@
       <c r="C152" t="s">
         <v>392</v>
       </c>
-      <c r="D152" s="1">
+      <c r="D152" s="4">
         <v>1626</v>
       </c>
       <c r="E152" s="4" t="s">
@@ -35556,7 +35856,7 @@
       <c r="C153" t="s">
         <v>393</v>
       </c>
-      <c r="D153" s="1">
+      <c r="D153" s="4">
         <v>1627</v>
       </c>
       <c r="E153" s="4" t="s">
@@ -35585,7 +35885,7 @@
       <c r="C154" t="s">
         <v>394</v>
       </c>
-      <c r="D154" s="1">
+      <c r="D154" s="4">
         <v>1628</v>
       </c>
       <c r="E154" s="4" t="s">
@@ -35614,7 +35914,7 @@
       <c r="C155" t="s">
         <v>395</v>
       </c>
-      <c r="D155" s="1">
+      <c r="D155" s="4">
         <v>1629</v>
       </c>
       <c r="E155" s="4" t="s">
@@ -35643,7 +35943,7 @@
       <c r="C156" t="s">
         <v>396</v>
       </c>
-      <c r="D156" s="1">
+      <c r="D156" s="4">
         <v>1630</v>
       </c>
       <c r="E156" s="4" t="s">
@@ -35672,7 +35972,7 @@
       <c r="C157" t="s">
         <v>314</v>
       </c>
-      <c r="D157" s="1">
+      <c r="D157" s="4">
         <v>1741</v>
       </c>
       <c r="E157" s="4" t="s">
@@ -35701,7 +36001,7 @@
       <c r="C158" t="s">
         <v>315</v>
       </c>
-      <c r="D158" s="1">
+      <c r="D158" s="4">
         <v>1742</v>
       </c>
       <c r="E158" s="4" t="s">
@@ -35730,7 +36030,7 @@
       <c r="C159" t="s">
         <v>397</v>
       </c>
-      <c r="D159" s="1">
+      <c r="D159" s="4">
         <v>1631</v>
       </c>
       <c r="E159" s="4" t="s">
@@ -35759,7 +36059,7 @@
       <c r="C160" t="s">
         <v>316</v>
       </c>
-      <c r="D160" s="1">
+      <c r="D160" s="4">
         <v>1743</v>
       </c>
       <c r="E160" s="4" t="s">
@@ -35788,7 +36088,7 @@
       <c r="C161" t="s">
         <v>317</v>
       </c>
-      <c r="D161" s="1">
+      <c r="D161" s="4">
         <v>1744</v>
       </c>
       <c r="E161" s="4" t="s">
@@ -35817,7 +36117,7 @@
       <c r="C162" t="s">
         <v>318</v>
       </c>
-      <c r="D162" s="1">
+      <c r="D162" s="4">
         <v>1745</v>
       </c>
       <c r="E162" s="4" t="s">
@@ -35846,7 +36146,7 @@
       <c r="C163" t="s">
         <v>319</v>
       </c>
-      <c r="D163" s="1">
+      <c r="D163" s="4">
         <v>1746</v>
       </c>
       <c r="E163" s="4" t="s">
@@ -35875,7 +36175,7 @@
       <c r="C164" t="s">
         <v>320</v>
       </c>
-      <c r="D164" s="1">
+      <c r="D164" s="4">
         <v>1747</v>
       </c>
       <c r="E164" s="4" t="s">
@@ -35904,7 +36204,7 @@
       <c r="C165" t="s">
         <v>480</v>
       </c>
-      <c r="D165" s="1">
+      <c r="D165" s="4">
         <v>1632</v>
       </c>
       <c r="E165" s="4" t="s">
@@ -35933,7 +36233,7 @@
       <c r="C166" t="s">
         <v>524</v>
       </c>
-      <c r="D166" s="1">
+      <c r="D166" s="4">
         <v>1800</v>
       </c>
       <c r="E166" s="4" t="s">
@@ -35962,7 +36262,7 @@
       <c r="C167" t="s">
         <v>321</v>
       </c>
-      <c r="D167" s="1">
+      <c r="D167" s="4">
         <v>1748</v>
       </c>
       <c r="E167" s="4" t="s">
@@ -35991,7 +36291,7 @@
       <c r="C168" t="s">
         <v>343</v>
       </c>
-      <c r="D168" s="1">
+      <c r="D168" s="4">
         <v>1770</v>
       </c>
       <c r="E168" s="4" t="s">
@@ -36020,7 +36320,7 @@
       <c r="C169" t="s">
         <v>322</v>
       </c>
-      <c r="D169" s="1">
+      <c r="D169" s="4">
         <v>1749</v>
       </c>
       <c r="E169" s="4" t="s">
@@ -36049,7 +36349,7 @@
       <c r="C170" t="s">
         <v>323</v>
       </c>
-      <c r="D170" s="1">
+      <c r="D170" s="4">
         <v>1750</v>
       </c>
       <c r="E170" s="4" t="s">
@@ -36078,7 +36378,7 @@
       <c r="C171" t="s">
         <v>331</v>
       </c>
-      <c r="D171" s="1">
+      <c r="D171" s="4">
         <v>1758</v>
       </c>
       <c r="E171" s="4" t="s">
@@ -36107,7 +36407,7 @@
       <c r="C172" t="s">
         <v>324</v>
       </c>
-      <c r="D172" s="1">
+      <c r="D172" s="4">
         <v>1751</v>
       </c>
       <c r="E172" s="4" t="s">
@@ -36136,7 +36436,7 @@
       <c r="C173" t="s">
         <v>346</v>
       </c>
-      <c r="D173" s="1">
+      <c r="D173" s="4">
         <v>1773</v>
       </c>
       <c r="E173" s="4" t="s">
@@ -36165,7 +36465,7 @@
       <c r="C174" t="s">
         <v>483</v>
       </c>
-      <c r="D174" s="1">
+      <c r="D174" s="4">
         <v>1635</v>
       </c>
       <c r="E174" s="4" t="s">
@@ -36194,7 +36494,7 @@
       <c r="C175" t="s">
         <v>481</v>
       </c>
-      <c r="D175" s="1">
+      <c r="D175" s="4">
         <v>1633</v>
       </c>
       <c r="E175" s="4" t="s">
@@ -36223,7 +36523,7 @@
       <c r="C176" t="s">
         <v>484</v>
       </c>
-      <c r="D176" s="1">
+      <c r="D176" s="4">
         <v>1636</v>
       </c>
       <c r="E176" s="4" t="s">
@@ -36252,7 +36552,7 @@
       <c r="C177" t="s">
         <v>482</v>
       </c>
-      <c r="D177" s="1">
+      <c r="D177" s="4">
         <v>1634</v>
       </c>
       <c r="E177" s="4" t="s">
@@ -36281,7 +36581,7 @@
       <c r="C178" t="s">
         <v>347</v>
       </c>
-      <c r="D178" s="1">
+      <c r="D178" s="4">
         <v>1774</v>
       </c>
       <c r="E178" s="4" t="s">
@@ -36310,7 +36610,7 @@
       <c r="C179" t="s">
         <v>485</v>
       </c>
-      <c r="D179" s="1">
+      <c r="D179" s="4">
         <v>1638</v>
       </c>
       <c r="E179" s="4" t="s">
@@ -36339,7 +36639,7 @@
       <c r="C180" t="s">
         <v>333</v>
       </c>
-      <c r="D180" s="1">
+      <c r="D180" s="4">
         <v>1760</v>
       </c>
       <c r="E180" s="4" t="s">
@@ -36368,7 +36668,7 @@
       <c r="C181" t="s">
         <v>486</v>
       </c>
-      <c r="D181" s="1">
+      <c r="D181" s="4">
         <v>1639</v>
       </c>
       <c r="E181" s="4" t="s">
@@ -36397,7 +36697,7 @@
       <c r="C182" t="s">
         <v>487</v>
       </c>
-      <c r="D182" s="1">
+      <c r="D182" s="4">
         <v>1640</v>
       </c>
       <c r="E182" s="4" t="s">
@@ -36426,7 +36726,7 @@
       <c r="C183" t="s">
         <v>398</v>
       </c>
-      <c r="D183" s="1">
+      <c r="D183" s="4">
         <v>1642</v>
       </c>
       <c r="E183" s="4" t="s">
@@ -36455,7 +36755,7 @@
       <c r="C184" t="s">
         <v>334</v>
       </c>
-      <c r="D184" s="1">
+      <c r="D184" s="4">
         <v>1761</v>
       </c>
       <c r="E184" s="4" t="s">
@@ -36484,7 +36784,7 @@
       <c r="C185" t="s">
         <v>399</v>
       </c>
-      <c r="D185" s="1">
+      <c r="D185" s="4">
         <v>1643</v>
       </c>
       <c r="E185" s="4" t="s">
@@ -36513,7 +36813,7 @@
       <c r="C186" t="s">
         <v>336</v>
       </c>
-      <c r="D186" s="1">
+      <c r="D186" s="4">
         <v>1763</v>
       </c>
       <c r="E186" s="4" t="s">
@@ -36542,7 +36842,7 @@
       <c r="C187" t="s">
         <v>400</v>
       </c>
-      <c r="D187" s="1">
+      <c r="D187" s="4">
         <v>1644</v>
       </c>
       <c r="E187" s="4" t="s">
@@ -36571,7 +36871,7 @@
       <c r="C188" t="s">
         <v>488</v>
       </c>
-      <c r="D188" s="1">
+      <c r="D188" s="4">
         <v>1641</v>
       </c>
       <c r="E188" s="4" t="s">
@@ -36600,7 +36900,7 @@
       <c r="C189" t="s">
         <v>401</v>
       </c>
-      <c r="D189" s="1">
+      <c r="D189" s="4">
         <v>1645</v>
       </c>
       <c r="E189" s="4" t="s">
@@ -36629,7 +36929,7 @@
       <c r="C190" t="s">
         <v>402</v>
       </c>
-      <c r="D190" s="1">
+      <c r="D190" s="4">
         <v>1646</v>
       </c>
       <c r="E190" s="4" t="s">
@@ -36658,7 +36958,7 @@
       <c r="C191" t="s">
         <v>403</v>
       </c>
-      <c r="D191" s="1">
+      <c r="D191" s="4">
         <v>1647</v>
       </c>
       <c r="E191" s="4" t="s">
@@ -36687,7 +36987,7 @@
       <c r="C192" t="s">
         <v>489</v>
       </c>
-      <c r="D192" s="1">
+      <c r="D192" s="4">
         <v>1648</v>
       </c>
       <c r="E192" s="4" t="s">
@@ -36716,7 +37016,7 @@
       <c r="C193" t="s">
         <v>353</v>
       </c>
-      <c r="D193" s="1">
+      <c r="D193" s="4">
         <v>1780</v>
       </c>
       <c r="E193" s="4" t="s">
@@ -36745,7 +37045,7 @@
       <c r="C194" t="s">
         <v>490</v>
       </c>
-      <c r="D194" s="1">
+      <c r="D194" s="4">
         <v>1649</v>
       </c>
       <c r="E194" s="4" t="s">
@@ -36774,7 +37074,7 @@
       <c r="C195" t="s">
         <v>491</v>
       </c>
-      <c r="D195" s="1">
+      <c r="D195" s="4">
         <v>1652</v>
       </c>
       <c r="E195" s="4" t="s">
@@ -36803,7 +37103,7 @@
       <c r="C196" t="s">
         <v>492</v>
       </c>
-      <c r="D196" s="1">
+      <c r="D196" s="4">
         <v>1653</v>
       </c>
       <c r="E196" s="4" t="s">
@@ -36832,7 +37132,7 @@
       <c r="C197" t="s">
         <v>340</v>
       </c>
-      <c r="D197" s="1">
+      <c r="D197" s="4">
         <v>1767</v>
       </c>
       <c r="E197" s="4" t="s">
@@ -36861,7 +37161,7 @@
       <c r="C198" t="s">
         <v>493</v>
       </c>
-      <c r="D198" s="1">
+      <c r="D198" s="4">
         <v>1654</v>
       </c>
       <c r="E198" s="4" t="s">
@@ -36890,7 +37190,7 @@
       <c r="C199" t="s">
         <v>341</v>
       </c>
-      <c r="D199" s="1">
+      <c r="D199" s="4">
         <v>1768</v>
       </c>
       <c r="E199" s="4" t="s">
@@ -36919,7 +37219,7 @@
       <c r="C200" t="s">
         <v>264</v>
       </c>
-      <c r="D200" s="1">
+      <c r="D200" s="4">
         <v>2657</v>
       </c>
       <c r="E200" s="4" t="s">
@@ -36948,7 +37248,7 @@
       <c r="C201" t="s">
         <v>494</v>
       </c>
-      <c r="D201" s="1">
+      <c r="D201" s="4">
         <v>1655</v>
       </c>
       <c r="E201" s="4" t="s">
@@ -36977,7 +37277,7 @@
       <c r="C202" t="s">
         <v>273</v>
       </c>
-      <c r="D202" s="1">
+      <c r="D202" s="4">
         <v>1698</v>
       </c>
       <c r="E202" s="4" t="s">
@@ -37006,7 +37306,7 @@
       <c r="C203" t="s">
         <v>495</v>
       </c>
-      <c r="D203" s="1">
+      <c r="D203" s="4">
         <v>1656</v>
       </c>
       <c r="E203" s="4" t="s">
@@ -37035,7 +37335,7 @@
       <c r="C204" t="s">
         <v>344</v>
       </c>
-      <c r="D204" s="1">
+      <c r="D204" s="4">
         <v>1771</v>
       </c>
       <c r="E204" s="4" t="s">
@@ -37064,7 +37364,7 @@
       <c r="C205" t="s">
         <v>496</v>
       </c>
-      <c r="D205" s="1">
+      <c r="D205" s="4">
         <v>1657</v>
       </c>
       <c r="E205" s="4" t="s">
@@ -37093,7 +37393,7 @@
       <c r="C206" t="s">
         <v>404</v>
       </c>
-      <c r="D206" s="1">
+      <c r="D206" s="4">
         <v>1658</v>
       </c>
       <c r="E206" s="4" t="s">
@@ -37122,7 +37422,7 @@
       <c r="C207" t="s">
         <v>405</v>
       </c>
-      <c r="D207" s="1">
+      <c r="D207" s="4">
         <v>1659</v>
       </c>
       <c r="E207" s="4" t="s">
@@ -37151,7 +37451,7 @@
       <c r="C208" t="s">
         <v>345</v>
       </c>
-      <c r="D208" s="1">
+      <c r="D208" s="4">
         <v>1772</v>
       </c>
       <c r="E208" s="4" t="s">
@@ -37180,7 +37480,7 @@
       <c r="C209" t="s">
         <v>290</v>
       </c>
-      <c r="D209" s="1">
+      <c r="D209" s="4">
         <v>1717</v>
       </c>
       <c r="E209" s="4" t="s">
@@ -37209,7 +37509,7 @@
       <c r="C210" t="s">
         <v>293</v>
       </c>
-      <c r="D210" s="1">
+      <c r="D210" s="4">
         <v>1720</v>
       </c>
       <c r="E210" s="4" t="s">
@@ -37238,7 +37538,7 @@
       <c r="C211" t="s">
         <v>292</v>
       </c>
-      <c r="D211" s="1">
+      <c r="D211" s="4">
         <v>1719</v>
       </c>
       <c r="E211" s="4" t="s">
@@ -37267,7 +37567,7 @@
       <c r="C212" t="s">
         <v>523</v>
       </c>
-      <c r="D212" s="1">
+      <c r="D212" s="4">
         <v>1799</v>
       </c>
       <c r="E212" s="4" t="s">
@@ -37296,7 +37596,7 @@
       <c r="C213" t="s">
         <v>522</v>
       </c>
-      <c r="D213" s="1">
+      <c r="D213" s="4">
         <v>1798</v>
       </c>
       <c r="E213" s="4" t="s">
@@ -37325,7 +37625,7 @@
       <c r="C214" t="s">
         <v>297</v>
       </c>
-      <c r="D214" s="1">
+      <c r="D214" s="4">
         <v>1724</v>
       </c>
       <c r="E214" s="4" t="s">
@@ -37354,7 +37654,7 @@
       <c r="C215" t="s">
         <v>294</v>
       </c>
-      <c r="D215" s="1">
+      <c r="D215" s="4">
         <v>1721</v>
       </c>
       <c r="E215" s="4" t="s">
@@ -37383,7 +37683,7 @@
       <c r="C216" t="s">
         <v>352</v>
       </c>
-      <c r="D216" s="1">
+      <c r="D216" s="4">
         <v>1779</v>
       </c>
       <c r="E216" s="4" t="s">
@@ -37412,7 +37712,7 @@
       <c r="C217" t="s">
         <v>274</v>
       </c>
-      <c r="D217" s="1">
+      <c r="D217" s="4">
         <v>1699</v>
       </c>
       <c r="E217" s="4" t="s">
@@ -37441,7 +37741,7 @@
       <c r="C218" t="s">
         <v>406</v>
       </c>
-      <c r="D218" s="1">
+      <c r="D218" s="4">
         <v>1660</v>
       </c>
       <c r="E218" s="4" t="s">
@@ -37470,7 +37770,7 @@
       <c r="C219" t="s">
         <v>299</v>
       </c>
-      <c r="D219" s="1">
+      <c r="D219" s="4">
         <v>1726</v>
       </c>
       <c r="E219" s="4" t="s">
@@ -37499,7 +37799,7 @@
       <c r="C220" t="s">
         <v>407</v>
       </c>
-      <c r="D220" s="1">
+      <c r="D220" s="4">
         <v>1661</v>
       </c>
       <c r="E220" s="4" t="s">
@@ -37528,7 +37828,7 @@
       <c r="C221" t="s">
         <v>291</v>
       </c>
-      <c r="D221" s="1">
+      <c r="D221" s="4">
         <v>1718</v>
       </c>
       <c r="E221" s="4" t="s">
@@ -37557,7 +37857,7 @@
       <c r="C222" t="s">
         <v>408</v>
       </c>
-      <c r="D222" s="1">
+      <c r="D222" s="4">
         <v>1662</v>
       </c>
       <c r="E222" s="4" t="s">
@@ -37586,7 +37886,7 @@
       <c r="C223" t="s">
         <v>327</v>
       </c>
-      <c r="D223" s="1">
+      <c r="D223" s="4">
         <v>1754</v>
       </c>
       <c r="E223" s="4" t="s">
@@ -37615,7 +37915,7 @@
       <c r="C224" t="s">
         <v>409</v>
       </c>
-      <c r="D224" s="1">
+      <c r="D224" s="4">
         <v>1663</v>
       </c>
       <c r="E224" s="4" t="s">
@@ -37644,7 +37944,7 @@
       <c r="C225" t="s">
         <v>350</v>
       </c>
-      <c r="D225" s="1">
+      <c r="D225" s="4">
         <v>1777</v>
       </c>
       <c r="E225" s="4" t="s">
@@ -37673,7 +37973,7 @@
       <c r="C226" t="s">
         <v>351</v>
       </c>
-      <c r="D226" s="1">
+      <c r="D226" s="4">
         <v>1778</v>
       </c>
       <c r="E226" s="4" t="s">
@@ -37702,7 +38002,7 @@
       <c r="C227" t="s">
         <v>497</v>
       </c>
-      <c r="D227" s="1">
+      <c r="D227" s="4">
         <v>1664</v>
       </c>
       <c r="E227" s="4" t="s">
@@ -37731,7 +38031,7 @@
       <c r="C228" t="s">
         <v>498</v>
       </c>
-      <c r="D228" s="1">
+      <c r="D228" s="4">
         <v>1665</v>
       </c>
       <c r="E228" s="4" t="s">
@@ -37760,7 +38060,7 @@
       <c r="C229" t="s">
         <v>499</v>
       </c>
-      <c r="D229" s="1">
+      <c r="D229" s="4">
         <v>1666</v>
       </c>
       <c r="E229" s="4" t="s">
@@ -37789,7 +38089,7 @@
       <c r="C230" t="s">
         <v>500</v>
       </c>
-      <c r="D230" s="1">
+      <c r="D230" s="4">
         <v>1667</v>
       </c>
       <c r="E230" s="4" t="s">
@@ -37818,7 +38118,7 @@
       <c r="C231" t="s">
         <v>501</v>
       </c>
-      <c r="D231" s="1">
+      <c r="D231" s="4">
         <v>1668</v>
       </c>
       <c r="E231" s="4" t="s">
@@ -37847,7 +38147,7 @@
       <c r="C232" t="s">
         <v>502</v>
       </c>
-      <c r="D232" s="1">
+      <c r="D232" s="4">
         <v>1669</v>
       </c>
       <c r="E232" s="4" t="s">
@@ -37876,7 +38176,7 @@
       <c r="C233" t="s">
         <v>354</v>
       </c>
-      <c r="D233" s="1">
+      <c r="D233" s="4">
         <v>1781</v>
       </c>
       <c r="E233" s="4" t="s">
@@ -37905,7 +38205,7 @@
       <c r="C234" t="s">
         <v>503</v>
       </c>
-      <c r="D234" s="1">
+      <c r="D234" s="4">
         <v>1670</v>
       </c>
       <c r="E234" s="4" t="s">
@@ -37934,7 +38234,7 @@
       <c r="C235" t="s">
         <v>504</v>
       </c>
-      <c r="D235" s="1">
+      <c r="D235" s="4">
         <v>1671</v>
       </c>
       <c r="E235" s="4" t="s">
@@ -37963,7 +38263,7 @@
       <c r="C236" t="s">
         <v>505</v>
       </c>
-      <c r="D236" s="1">
+      <c r="D236" s="4">
         <v>1672</v>
       </c>
       <c r="E236" s="4" t="s">
@@ -37992,7 +38292,7 @@
       <c r="C237" t="s">
         <v>506</v>
       </c>
-      <c r="D237" s="1">
+      <c r="D237" s="4">
         <v>1673</v>
       </c>
       <c r="E237" s="4" t="s">
@@ -38021,7 +38321,7 @@
       <c r="C238" t="s">
         <v>410</v>
       </c>
-      <c r="D238" s="1">
+      <c r="D238" s="4">
         <v>1674</v>
       </c>
       <c r="E238" s="4" t="s">
@@ -38050,7 +38350,7 @@
       <c r="C239" t="s">
         <v>411</v>
       </c>
-      <c r="D239" s="1">
+      <c r="D239" s="4">
         <v>1675</v>
       </c>
       <c r="E239" s="4" t="s">
@@ -38079,7 +38379,7 @@
       <c r="C240" t="s">
         <v>412</v>
       </c>
-      <c r="D240" s="1">
+      <c r="D240" s="4">
         <v>1676</v>
       </c>
       <c r="E240" s="4" t="s">
@@ -38108,7 +38408,7 @@
       <c r="C241" t="s">
         <v>413</v>
       </c>
-      <c r="D241" s="1">
+      <c r="D241" s="4">
         <v>1677</v>
       </c>
       <c r="E241" s="4" t="s">
@@ -38137,7 +38437,7 @@
       <c r="C242" t="s">
         <v>414</v>
       </c>
-      <c r="D242" s="1">
+      <c r="D242" s="4">
         <v>1678</v>
       </c>
       <c r="E242" s="4" t="s">
@@ -38166,7 +38466,7 @@
       <c r="C243" t="s">
         <v>415</v>
       </c>
-      <c r="D243" s="1">
+      <c r="D243" s="4">
         <v>1679</v>
       </c>
       <c r="E243" s="4" t="s">
@@ -38195,7 +38495,7 @@
       <c r="C244" t="s">
         <v>507</v>
       </c>
-      <c r="D244" s="1">
+      <c r="D244" s="4">
         <v>1680</v>
       </c>
       <c r="E244" s="4" t="s">
@@ -38224,7 +38524,7 @@
       <c r="C245" t="s">
         <v>508</v>
       </c>
-      <c r="D245" s="1">
+      <c r="D245" s="4">
         <v>1681</v>
       </c>
       <c r="E245" s="4" t="s">
@@ -38253,7 +38553,7 @@
       <c r="C246" t="s">
         <v>509</v>
       </c>
-      <c r="D246" s="1">
+      <c r="D246" s="4">
         <v>1682</v>
       </c>
       <c r="E246" s="4" t="s">
@@ -38282,7 +38582,7 @@
       <c r="C247" t="s">
         <v>379</v>
       </c>
-      <c r="D247" s="1">
+      <c r="D247" s="4">
         <v>1582</v>
       </c>
       <c r="E247" s="4" t="s">
@@ -38311,7 +38611,7 @@
       <c r="C248" t="s">
         <v>510</v>
       </c>
-      <c r="D248" s="1">
+      <c r="D248" s="4">
         <v>1683</v>
       </c>
       <c r="E248" s="4" t="s">
@@ -38340,7 +38640,7 @@
       <c r="C249" t="s">
         <v>511</v>
       </c>
-      <c r="D249" s="1">
+      <c r="D249" s="4">
         <v>1684</v>
       </c>
       <c r="E249" s="4" t="s">
@@ -38369,7 +38669,7 @@
       <c r="C250" t="s">
         <v>512</v>
       </c>
-      <c r="D250" s="1">
+      <c r="D250" s="4">
         <v>1685</v>
       </c>
       <c r="E250" s="4" t="s">
@@ -38398,7 +38698,7 @@
       <c r="C251" t="s">
         <v>513</v>
       </c>
-      <c r="D251" s="1">
+      <c r="D251" s="4">
         <v>1686</v>
       </c>
       <c r="E251" s="4" t="s">
@@ -38427,7 +38727,7 @@
       <c r="C252" t="s">
         <v>514</v>
       </c>
-      <c r="D252" s="1">
+      <c r="D252" s="4">
         <v>1687</v>
       </c>
       <c r="E252" s="4" t="s">
@@ -38456,7 +38756,7 @@
       <c r="C253" t="s">
         <v>515</v>
       </c>
-      <c r="D253" s="1">
+      <c r="D253" s="4">
         <v>1688</v>
       </c>
       <c r="E253" s="4" t="s">
@@ -38485,7 +38785,7 @@
       <c r="C254" t="s">
         <v>416</v>
       </c>
-      <c r="D254" s="1">
+      <c r="D254" s="4">
         <v>1690</v>
       </c>
       <c r="E254" s="4" t="s">
@@ -38514,7 +38814,7 @@
       <c r="C255" t="s">
         <v>516</v>
       </c>
-      <c r="D255" s="1">
+      <c r="D255" s="4">
         <v>1689</v>
       </c>
       <c r="E255" s="4" t="s">
@@ -38543,7 +38843,7 @@
       <c r="C256" t="s">
         <v>325</v>
       </c>
-      <c r="D256" s="1">
+      <c r="D256" s="4">
         <v>1752</v>
       </c>
       <c r="E256" s="4" t="s">
@@ -38572,7 +38872,7 @@
       <c r="C257" t="s">
         <v>417</v>
       </c>
-      <c r="D257" s="1">
+      <c r="D257" s="4">
         <v>1691</v>
       </c>
       <c r="E257" s="4" t="s">
@@ -38601,7 +38901,7 @@
       <c r="C258" t="s">
         <v>418</v>
       </c>
-      <c r="D258" s="1">
+      <c r="D258" s="4">
         <v>1692</v>
       </c>
       <c r="E258" s="4" t="s">
@@ -38630,7 +38930,7 @@
       <c r="C259" t="s">
         <v>419</v>
       </c>
-      <c r="D259" s="1">
+      <c r="D259" s="4">
         <v>1693</v>
       </c>
       <c r="E259" s="4" t="s">
@@ -38659,7 +38959,7 @@
       <c r="C260" t="s">
         <v>420</v>
       </c>
-      <c r="D260" s="1">
+      <c r="D260" s="4">
         <v>1694</v>
       </c>
       <c r="E260" s="4" t="s">
@@ -38688,7 +38988,7 @@
       <c r="C261" t="s">
         <v>272</v>
       </c>
-      <c r="D261" s="1">
+      <c r="D261" s="4">
         <v>1696</v>
       </c>
       <c r="E261" s="4" t="s">
@@ -38717,7 +39017,7 @@
       <c r="C262" t="s">
         <v>348</v>
       </c>
-      <c r="D262" s="1">
+      <c r="D262" s="4">
         <v>1775</v>
       </c>
       <c r="E262" s="4" t="s">
@@ -38746,7 +39046,7 @@
       <c r="C263" t="s">
         <v>421</v>
       </c>
-      <c r="D263" s="1">
+      <c r="D263" s="4">
         <v>1695</v>
       </c>
       <c r="E263" s="4" t="s">
@@ -38766,6 +39066,501 @@
       </c>
       <c r="J263" t="s">
         <v>158</v>
+      </c>
+    </row>
+    <row r="264" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C264" t="s">
+        <v>1125</v>
+      </c>
+      <c r="D264" s="4">
+        <f>HEX2DEC(REPLACE(C264,1,2,""))</f>
+        <v>2658</v>
+      </c>
+      <c r="I264" t="s">
+        <v>1059</v>
+      </c>
+      <c r="J264" t="s">
+        <v>1092</v>
+      </c>
+    </row>
+    <row r="265" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C265" t="s">
+        <v>1126</v>
+      </c>
+      <c r="D265" s="4">
+        <f t="shared" ref="D265:D296" si="0">HEX2DEC(REPLACE(C265,1,2,""))</f>
+        <v>2659</v>
+      </c>
+      <c r="I265" t="s">
+        <v>1060</v>
+      </c>
+      <c r="J265" t="s">
+        <v>1093</v>
+      </c>
+    </row>
+    <row r="266" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C266" t="s">
+        <v>1127</v>
+      </c>
+      <c r="D266" s="4">
+        <f t="shared" si="0"/>
+        <v>2660</v>
+      </c>
+      <c r="I266" t="s">
+        <v>1061</v>
+      </c>
+      <c r="J266" t="s">
+        <v>1094</v>
+      </c>
+    </row>
+    <row r="267" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C267" t="s">
+        <v>1128</v>
+      </c>
+      <c r="D267" s="4">
+        <f t="shared" si="0"/>
+        <v>2661</v>
+      </c>
+      <c r="I267" t="s">
+        <v>1062</v>
+      </c>
+      <c r="J267" t="s">
+        <v>1095</v>
+      </c>
+    </row>
+    <row r="268" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C268" t="s">
+        <v>1129</v>
+      </c>
+      <c r="D268" s="4">
+        <f t="shared" si="0"/>
+        <v>2662</v>
+      </c>
+      <c r="I268" t="s">
+        <v>1063</v>
+      </c>
+      <c r="J268" t="s">
+        <v>1096</v>
+      </c>
+    </row>
+    <row r="269" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C269" t="s">
+        <v>1130</v>
+      </c>
+      <c r="D269" s="4">
+        <f t="shared" si="0"/>
+        <v>2663</v>
+      </c>
+      <c r="I269" t="s">
+        <v>1064</v>
+      </c>
+      <c r="J269" t="s">
+        <v>1097</v>
+      </c>
+    </row>
+    <row r="270" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C270" t="s">
+        <v>1131</v>
+      </c>
+      <c r="D270" s="4">
+        <f t="shared" si="0"/>
+        <v>2664</v>
+      </c>
+      <c r="I270" t="s">
+        <v>1065</v>
+      </c>
+      <c r="J270" t="s">
+        <v>1098</v>
+      </c>
+    </row>
+    <row r="271" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C271" t="s">
+        <v>1132</v>
+      </c>
+      <c r="D271" s="4">
+        <f t="shared" si="0"/>
+        <v>2665</v>
+      </c>
+      <c r="I271" t="s">
+        <v>1066</v>
+      </c>
+      <c r="J271" t="s">
+        <v>1099</v>
+      </c>
+    </row>
+    <row r="272" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C272" t="s">
+        <v>1133</v>
+      </c>
+      <c r="D272" s="4">
+        <f t="shared" si="0"/>
+        <v>2666</v>
+      </c>
+      <c r="I272" t="s">
+        <v>1067</v>
+      </c>
+      <c r="J272" t="s">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="273" spans="3:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C273" t="s">
+        <v>1134</v>
+      </c>
+      <c r="D273" s="4">
+        <f t="shared" si="0"/>
+        <v>2667</v>
+      </c>
+      <c r="I273" t="s">
+        <v>1068</v>
+      </c>
+      <c r="J273" t="s">
+        <v>1101</v>
+      </c>
+    </row>
+    <row r="274" spans="3:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C274" t="s">
+        <v>1135</v>
+      </c>
+      <c r="D274" s="4">
+        <f t="shared" si="0"/>
+        <v>2668</v>
+      </c>
+      <c r="I274" t="s">
+        <v>1069</v>
+      </c>
+      <c r="J274" t="s">
+        <v>1102</v>
+      </c>
+    </row>
+    <row r="275" spans="3:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C275" t="s">
+        <v>1136</v>
+      </c>
+      <c r="D275" s="4">
+        <f t="shared" si="0"/>
+        <v>2669</v>
+      </c>
+      <c r="I275" t="s">
+        <v>1070</v>
+      </c>
+      <c r="J275" t="s">
+        <v>1103</v>
+      </c>
+    </row>
+    <row r="276" spans="3:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C276" t="s">
+        <v>1137</v>
+      </c>
+      <c r="D276" s="4">
+        <f t="shared" si="0"/>
+        <v>2670</v>
+      </c>
+      <c r="I276" t="s">
+        <v>1071</v>
+      </c>
+      <c r="J276" t="s">
+        <v>1104</v>
+      </c>
+    </row>
+    <row r="277" spans="3:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C277" t="s">
+        <v>1138</v>
+      </c>
+      <c r="D277" s="4">
+        <f t="shared" si="0"/>
+        <v>2671</v>
+      </c>
+      <c r="I277" t="s">
+        <v>1072</v>
+      </c>
+      <c r="J277" t="s">
+        <v>1105</v>
+      </c>
+    </row>
+    <row r="278" spans="3:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C278" t="s">
+        <v>1139</v>
+      </c>
+      <c r="D278" s="4">
+        <f t="shared" si="0"/>
+        <v>2672</v>
+      </c>
+      <c r="I278" t="s">
+        <v>1073</v>
+      </c>
+      <c r="J278" t="s">
+        <v>1106</v>
+      </c>
+    </row>
+    <row r="279" spans="3:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C279" t="s">
+        <v>1140</v>
+      </c>
+      <c r="D279" s="4">
+        <f t="shared" si="0"/>
+        <v>2673</v>
+      </c>
+      <c r="I279" t="s">
+        <v>1074</v>
+      </c>
+      <c r="J279" t="s">
+        <v>1107</v>
+      </c>
+    </row>
+    <row r="280" spans="3:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C280" t="s">
+        <v>1141</v>
+      </c>
+      <c r="D280" s="4">
+        <f t="shared" si="0"/>
+        <v>2674</v>
+      </c>
+      <c r="I280" t="s">
+        <v>1075</v>
+      </c>
+      <c r="J280" t="s">
+        <v>1108</v>
+      </c>
+    </row>
+    <row r="281" spans="3:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C281" t="s">
+        <v>1142</v>
+      </c>
+      <c r="D281" s="4">
+        <f t="shared" si="0"/>
+        <v>2675</v>
+      </c>
+      <c r="I281" t="s">
+        <v>1076</v>
+      </c>
+      <c r="J281" t="s">
+        <v>1109</v>
+      </c>
+    </row>
+    <row r="282" spans="3:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C282" t="s">
+        <v>1143</v>
+      </c>
+      <c r="D282" s="4">
+        <f t="shared" si="0"/>
+        <v>2676</v>
+      </c>
+      <c r="I282" t="s">
+        <v>1077</v>
+      </c>
+      <c r="J282" t="s">
+        <v>1110</v>
+      </c>
+    </row>
+    <row r="283" spans="3:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C283" t="s">
+        <v>1144</v>
+      </c>
+      <c r="D283" s="4">
+        <f t="shared" si="0"/>
+        <v>2677</v>
+      </c>
+      <c r="I283" t="s">
+        <v>1078</v>
+      </c>
+      <c r="J283" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="284" spans="3:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C284" t="s">
+        <v>1145</v>
+      </c>
+      <c r="D284" s="4">
+        <f t="shared" si="0"/>
+        <v>2678</v>
+      </c>
+      <c r="I284" t="s">
+        <v>1079</v>
+      </c>
+      <c r="J284" t="s">
+        <v>1112</v>
+      </c>
+    </row>
+    <row r="285" spans="3:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C285" t="s">
+        <v>1146</v>
+      </c>
+      <c r="D285" s="4">
+        <f t="shared" si="0"/>
+        <v>2679</v>
+      </c>
+      <c r="I285" t="s">
+        <v>1080</v>
+      </c>
+      <c r="J285" t="s">
+        <v>1113</v>
+      </c>
+    </row>
+    <row r="286" spans="3:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C286" t="s">
+        <v>1147</v>
+      </c>
+      <c r="D286" s="4">
+        <f t="shared" si="0"/>
+        <v>2680</v>
+      </c>
+      <c r="I286" t="s">
+        <v>1081</v>
+      </c>
+      <c r="J286" t="s">
+        <v>1114</v>
+      </c>
+    </row>
+    <row r="287" spans="3:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C287" t="s">
+        <v>1148</v>
+      </c>
+      <c r="D287" s="4">
+        <f t="shared" si="0"/>
+        <v>2681</v>
+      </c>
+      <c r="I287" t="s">
+        <v>1082</v>
+      </c>
+      <c r="J287" t="s">
+        <v>1115</v>
+      </c>
+    </row>
+    <row r="288" spans="3:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C288" t="s">
+        <v>1149</v>
+      </c>
+      <c r="D288" s="4">
+        <f t="shared" si="0"/>
+        <v>2682</v>
+      </c>
+      <c r="I288" t="s">
+        <v>1083</v>
+      </c>
+      <c r="J288" t="s">
+        <v>1116</v>
+      </c>
+    </row>
+    <row r="289" spans="3:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C289" t="s">
+        <v>1150</v>
+      </c>
+      <c r="D289" s="4">
+        <f t="shared" si="0"/>
+        <v>2683</v>
+      </c>
+      <c r="I289" t="s">
+        <v>1084</v>
+      </c>
+      <c r="J289" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="290" spans="3:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C290" t="s">
+        <v>1151</v>
+      </c>
+      <c r="D290" s="4">
+        <f t="shared" si="0"/>
+        <v>2684</v>
+      </c>
+      <c r="I290" t="s">
+        <v>1085</v>
+      </c>
+      <c r="J290" t="s">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="291" spans="3:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C291" t="s">
+        <v>1152</v>
+      </c>
+      <c r="D291" s="4">
+        <f t="shared" si="0"/>
+        <v>2685</v>
+      </c>
+      <c r="I291" t="s">
+        <v>1086</v>
+      </c>
+      <c r="J291" t="s">
+        <v>1119</v>
+      </c>
+    </row>
+    <row r="292" spans="3:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C292" t="s">
+        <v>1153</v>
+      </c>
+      <c r="D292" s="4">
+        <f t="shared" si="0"/>
+        <v>2686</v>
+      </c>
+      <c r="I292" t="s">
+        <v>1087</v>
+      </c>
+      <c r="J292" t="s">
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="293" spans="3:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C293" t="s">
+        <v>1154</v>
+      </c>
+      <c r="D293" s="4">
+        <f t="shared" si="0"/>
+        <v>2687</v>
+      </c>
+      <c r="I293" t="s">
+        <v>1088</v>
+      </c>
+      <c r="J293" t="s">
+        <v>1121</v>
+      </c>
+    </row>
+    <row r="294" spans="3:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C294" t="s">
+        <v>1155</v>
+      </c>
+      <c r="D294" s="4">
+        <f t="shared" si="0"/>
+        <v>2688</v>
+      </c>
+      <c r="I294" t="s">
+        <v>1089</v>
+      </c>
+      <c r="J294" t="s">
+        <v>1122</v>
+      </c>
+    </row>
+    <row r="295" spans="3:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C295" t="s">
+        <v>1156</v>
+      </c>
+      <c r="D295" s="4">
+        <f t="shared" si="0"/>
+        <v>2689</v>
+      </c>
+      <c r="I295" t="s">
+        <v>1090</v>
+      </c>
+      <c r="J295" t="s">
+        <v>1123</v>
+      </c>
+    </row>
+    <row r="296" spans="3:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C296" t="s">
+        <v>1157</v>
+      </c>
+      <c r="D296" s="4">
+        <f t="shared" si="0"/>
+        <v>2690</v>
+      </c>
+      <c r="I296" t="s">
+        <v>1091</v>
+      </c>
+      <c r="J296" t="s">
+        <v>1124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added some icons for chrome extension
</commit_message>
<xml_diff>
--- a/assets/icons/bowtie.xlsx
+++ b/assets/icons/bowtie.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
@@ -10,7 +10,7 @@
     <sheet name="Bowtie v1.0" sheetId="1" r:id="rId1"/>
     <sheet name="Bowtie v2.0" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2741" uniqueCount="1158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2819" uniqueCount="1236">
   <si>
     <t>uE709-edit-outline.svg</t>
   </si>
@@ -3494,12 +3494,246 @@
   </si>
   <si>
     <t>uEA82</t>
+  </si>
+  <si>
+    <t>uEA83-file-bug.svg</t>
+  </si>
+  <si>
+    <t>uEA84-chevron-up-all.svg</t>
+  </si>
+  <si>
+    <t>uEA85-chevron-down-all.svg</t>
+  </si>
+  <si>
+    <t>uEA86-chevron-left-all.svg</t>
+  </si>
+  <si>
+    <t>uEA87-chevron-right-all.svg</t>
+  </si>
+  <si>
+    <t>uEA83</t>
+  </si>
+  <si>
+    <t>uEA84</t>
+  </si>
+  <si>
+    <t>uEA85</t>
+  </si>
+  <si>
+    <t>uEA86</t>
+  </si>
+  <si>
+    <t>uEA87</t>
+  </si>
+  <si>
+    <t>file-bug.svg</t>
+  </si>
+  <si>
+    <t>chevron-up-all.svg</t>
+  </si>
+  <si>
+    <t>chevron-down-all.svg</t>
+  </si>
+  <si>
+    <t>chevron-left-all.svg</t>
+  </si>
+  <si>
+    <t>chevron-right-all.svg</t>
+  </si>
+  <si>
+    <t>uEA88</t>
+  </si>
+  <si>
+    <t>uEA89</t>
+  </si>
+  <si>
+    <t>uEA8A</t>
+  </si>
+  <si>
+    <t>uEA8B</t>
+  </si>
+  <si>
+    <t>uEA8C</t>
+  </si>
+  <si>
+    <t>uEA8D</t>
+  </si>
+  <si>
+    <t>uEA8E</t>
+  </si>
+  <si>
+    <t>uEA8F</t>
+  </si>
+  <si>
+    <t>uEA90</t>
+  </si>
+  <si>
+    <t>uEA91</t>
+  </si>
+  <si>
+    <t>uEA92</t>
+  </si>
+  <si>
+    <t>uEA93</t>
+  </si>
+  <si>
+    <t>uEA94</t>
+  </si>
+  <si>
+    <t>uEA95</t>
+  </si>
+  <si>
+    <t>uEA96</t>
+  </si>
+  <si>
+    <t>uEA97</t>
+  </si>
+  <si>
+    <t>uEA98</t>
+  </si>
+  <si>
+    <t>uEA99</t>
+  </si>
+  <si>
+    <t>uEA9A</t>
+  </si>
+  <si>
+    <t>uEA9B</t>
+  </si>
+  <si>
+    <t>uEA9C</t>
+  </si>
+  <si>
+    <t>uEA88-play-resume.svg</t>
+  </si>
+  <si>
+    <t>uEA89-play.svg</t>
+  </si>
+  <si>
+    <t>uEA8A-stop-fill.svg</t>
+  </si>
+  <si>
+    <t>uEA8B-stop.svg</t>
+  </si>
+  <si>
+    <t>uEA8C-record-fill.svg</t>
+  </si>
+  <si>
+    <t>uEA8D-fast-forward-fill.svg</t>
+  </si>
+  <si>
+    <t>uEA8E-fast-backward-fill.svg</t>
+  </si>
+  <si>
+    <t>uEA8F-previous-frame-fill.svg</t>
+  </si>
+  <si>
+    <t>uEA90-next-frame-fill.svg</t>
+  </si>
+  <si>
+    <t>uEA91-settings-gear-outline.svg</t>
+  </si>
+  <si>
+    <t>uEA92-play-fill.svg</t>
+  </si>
+  <si>
+    <t>uEA93-record.svg</t>
+  </si>
+  <si>
+    <t>uEA94-fast-forward.svg</t>
+  </si>
+  <si>
+    <t>uEA95-fast-backward.svg</t>
+  </si>
+  <si>
+    <t>uEA96-previous-frame.svg</t>
+  </si>
+  <si>
+    <t>uEA97-next-frame.svg</t>
+  </si>
+  <si>
+    <t>uEA98-pause.svg</t>
+  </si>
+  <si>
+    <t>uEA99-pause-fill.svg</t>
+  </si>
+  <si>
+    <t>uEA9A-play-resume-fill.svg</t>
+  </si>
+  <si>
+    <t>uEA9B-work-item-bug.svg</t>
+  </si>
+  <si>
+    <t>uEA9C-resize-grip.svg</t>
+  </si>
+  <si>
+    <t>play-resume.svg</t>
+  </si>
+  <si>
+    <t>play.svg</t>
+  </si>
+  <si>
+    <t>stop-fill.svg</t>
+  </si>
+  <si>
+    <t>stop.svg</t>
+  </si>
+  <si>
+    <t>record-fill.svg</t>
+  </si>
+  <si>
+    <t>fast-forward-fill.svg</t>
+  </si>
+  <si>
+    <t>fast-backward-fill.svg</t>
+  </si>
+  <si>
+    <t>previous-frame-fill.svg</t>
+  </si>
+  <si>
+    <t>next-frame-fill.svg</t>
+  </si>
+  <si>
+    <t>settings-gear-outline.svg</t>
+  </si>
+  <si>
+    <t>play-fill.svg</t>
+  </si>
+  <si>
+    <t>record.svg</t>
+  </si>
+  <si>
+    <t>fast-forward.svg</t>
+  </si>
+  <si>
+    <t>fast-backward.svg</t>
+  </si>
+  <si>
+    <t>previous-frame.svg</t>
+  </si>
+  <si>
+    <t>next-frame.svg</t>
+  </si>
+  <si>
+    <t>pause.svg</t>
+  </si>
+  <si>
+    <t>pause-fill.svg</t>
+  </si>
+  <si>
+    <t>play-resume-fill.svg</t>
+  </si>
+  <si>
+    <t>work-item-bug.svg</t>
+  </si>
+  <si>
+    <t>resize-grip.svg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -31415,11 +31649,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K296"/>
+  <dimension ref="A1:K322"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A258" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G262" sqref="G262"/>
+      <pane ySplit="1" topLeftCell="A297" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N306" sqref="N306"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -39563,6 +39797,370 @@
         <v>1124</v>
       </c>
     </row>
+    <row r="297" spans="3:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C297" t="s">
+        <v>1163</v>
+      </c>
+      <c r="D297" s="4">
+        <v>2691</v>
+      </c>
+      <c r="I297" t="s">
+        <v>1168</v>
+      </c>
+      <c r="J297" t="s">
+        <v>1158</v>
+      </c>
+    </row>
+    <row r="298" spans="3:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C298" t="s">
+        <v>1164</v>
+      </c>
+      <c r="D298" s="4">
+        <v>2692</v>
+      </c>
+      <c r="I298" t="s">
+        <v>1169</v>
+      </c>
+      <c r="J298" t="s">
+        <v>1159</v>
+      </c>
+    </row>
+    <row r="299" spans="3:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C299" t="s">
+        <v>1165</v>
+      </c>
+      <c r="D299" s="4">
+        <v>2693</v>
+      </c>
+      <c r="I299" t="s">
+        <v>1170</v>
+      </c>
+      <c r="J299" t="s">
+        <v>1160</v>
+      </c>
+    </row>
+    <row r="300" spans="3:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C300" t="s">
+        <v>1166</v>
+      </c>
+      <c r="D300" s="4">
+        <v>2694</v>
+      </c>
+      <c r="I300" t="s">
+        <v>1171</v>
+      </c>
+      <c r="J300" t="s">
+        <v>1161</v>
+      </c>
+    </row>
+    <row r="301" spans="3:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C301" t="s">
+        <v>1167</v>
+      </c>
+      <c r="D301" s="4">
+        <v>2695</v>
+      </c>
+      <c r="I301" t="s">
+        <v>1172</v>
+      </c>
+      <c r="J301" t="s">
+        <v>1162</v>
+      </c>
+    </row>
+    <row r="302" spans="3:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C302" t="s">
+        <v>1173</v>
+      </c>
+      <c r="D302" s="4">
+        <v>2696</v>
+      </c>
+      <c r="I302" t="s">
+        <v>1215</v>
+      </c>
+      <c r="J302" s="2" t="s">
+        <v>1194</v>
+      </c>
+    </row>
+    <row r="303" spans="3:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C303" t="s">
+        <v>1174</v>
+      </c>
+      <c r="D303" s="4">
+        <v>2697</v>
+      </c>
+      <c r="I303" t="s">
+        <v>1216</v>
+      </c>
+      <c r="J303" s="2" t="s">
+        <v>1195</v>
+      </c>
+    </row>
+    <row r="304" spans="3:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C304" t="s">
+        <v>1175</v>
+      </c>
+      <c r="D304" s="4">
+        <v>2698</v>
+      </c>
+      <c r="I304" t="s">
+        <v>1217</v>
+      </c>
+      <c r="J304" s="2" t="s">
+        <v>1196</v>
+      </c>
+    </row>
+    <row r="305" spans="3:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C305" t="s">
+        <v>1176</v>
+      </c>
+      <c r="D305" s="4">
+        <v>2699</v>
+      </c>
+      <c r="I305" t="s">
+        <v>1218</v>
+      </c>
+      <c r="J305" s="2" t="s">
+        <v>1197</v>
+      </c>
+    </row>
+    <row r="306" spans="3:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C306" t="s">
+        <v>1177</v>
+      </c>
+      <c r="D306" s="4">
+        <v>2700</v>
+      </c>
+      <c r="I306" t="s">
+        <v>1219</v>
+      </c>
+      <c r="J306" s="2" t="s">
+        <v>1198</v>
+      </c>
+    </row>
+    <row r="307" spans="3:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C307" t="s">
+        <v>1178</v>
+      </c>
+      <c r="D307" s="4">
+        <v>2701</v>
+      </c>
+      <c r="I307" t="s">
+        <v>1220</v>
+      </c>
+      <c r="J307" s="2" t="s">
+        <v>1199</v>
+      </c>
+    </row>
+    <row r="308" spans="3:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C308" t="s">
+        <v>1179</v>
+      </c>
+      <c r="D308" s="4">
+        <v>2702</v>
+      </c>
+      <c r="I308" t="s">
+        <v>1221</v>
+      </c>
+      <c r="J308" s="2" t="s">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="309" spans="3:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C309" t="s">
+        <v>1180</v>
+      </c>
+      <c r="D309" s="4">
+        <v>2703</v>
+      </c>
+      <c r="I309" t="s">
+        <v>1222</v>
+      </c>
+      <c r="J309" s="2" t="s">
+        <v>1201</v>
+      </c>
+    </row>
+    <row r="310" spans="3:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C310" t="s">
+        <v>1181</v>
+      </c>
+      <c r="D310" s="4">
+        <v>2704</v>
+      </c>
+      <c r="I310" t="s">
+        <v>1223</v>
+      </c>
+      <c r="J310" s="2" t="s">
+        <v>1202</v>
+      </c>
+    </row>
+    <row r="311" spans="3:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C311" t="s">
+        <v>1182</v>
+      </c>
+      <c r="D311" s="4">
+        <v>2705</v>
+      </c>
+      <c r="I311" t="s">
+        <v>1224</v>
+      </c>
+      <c r="J311" s="2" t="s">
+        <v>1203</v>
+      </c>
+    </row>
+    <row r="312" spans="3:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C312" t="s">
+        <v>1183</v>
+      </c>
+      <c r="D312" s="4">
+        <v>2706</v>
+      </c>
+      <c r="I312" t="s">
+        <v>1225</v>
+      </c>
+      <c r="J312" s="2" t="s">
+        <v>1204</v>
+      </c>
+    </row>
+    <row r="313" spans="3:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C313" t="s">
+        <v>1184</v>
+      </c>
+      <c r="D313" s="4">
+        <v>2707</v>
+      </c>
+      <c r="I313" t="s">
+        <v>1226</v>
+      </c>
+      <c r="J313" s="2" t="s">
+        <v>1205</v>
+      </c>
+    </row>
+    <row r="314" spans="3:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C314" t="s">
+        <v>1185</v>
+      </c>
+      <c r="D314" s="4">
+        <v>2708</v>
+      </c>
+      <c r="I314" t="s">
+        <v>1227</v>
+      </c>
+      <c r="J314" s="2" t="s">
+        <v>1206</v>
+      </c>
+    </row>
+    <row r="315" spans="3:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C315" t="s">
+        <v>1186</v>
+      </c>
+      <c r="D315" s="4">
+        <v>2709</v>
+      </c>
+      <c r="I315" t="s">
+        <v>1228</v>
+      </c>
+      <c r="J315" s="2" t="s">
+        <v>1207</v>
+      </c>
+    </row>
+    <row r="316" spans="3:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C316" t="s">
+        <v>1187</v>
+      </c>
+      <c r="D316" s="4">
+        <v>2710</v>
+      </c>
+      <c r="I316" t="s">
+        <v>1229</v>
+      </c>
+      <c r="J316" s="2" t="s">
+        <v>1208</v>
+      </c>
+    </row>
+    <row r="317" spans="3:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C317" t="s">
+        <v>1188</v>
+      </c>
+      <c r="D317" s="4">
+        <v>2711</v>
+      </c>
+      <c r="I317" t="s">
+        <v>1230</v>
+      </c>
+      <c r="J317" s="2" t="s">
+        <v>1209</v>
+      </c>
+    </row>
+    <row r="318" spans="3:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C318" t="s">
+        <v>1189</v>
+      </c>
+      <c r="D318" s="4">
+        <v>2712</v>
+      </c>
+      <c r="I318" t="s">
+        <v>1231</v>
+      </c>
+      <c r="J318" s="2" t="s">
+        <v>1210</v>
+      </c>
+    </row>
+    <row r="319" spans="3:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C319" t="s">
+        <v>1190</v>
+      </c>
+      <c r="D319" s="4">
+        <v>2713</v>
+      </c>
+      <c r="I319" t="s">
+        <v>1232</v>
+      </c>
+      <c r="J319" s="2" t="s">
+        <v>1211</v>
+      </c>
+    </row>
+    <row r="320" spans="3:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C320" t="s">
+        <v>1191</v>
+      </c>
+      <c r="D320" s="4">
+        <v>2714</v>
+      </c>
+      <c r="I320" t="s">
+        <v>1233</v>
+      </c>
+      <c r="J320" s="2" t="s">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="321" spans="3:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C321" t="s">
+        <v>1192</v>
+      </c>
+      <c r="D321" s="4">
+        <v>2715</v>
+      </c>
+      <c r="I321" t="s">
+        <v>1234</v>
+      </c>
+      <c r="J321" s="2" t="s">
+        <v>1213</v>
+      </c>
+    </row>
+    <row r="322" spans="3:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C322" t="s">
+        <v>1193</v>
+      </c>
+      <c r="D322" s="4">
+        <v>2716</v>
+      </c>
+      <c r="I322" t="s">
+        <v>1235</v>
+      </c>
+      <c r="J322" s="2" t="s">
+        <v>1214</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fix unicode in filename and regenerate files
</commit_message>
<xml_diff>
--- a/assets/icons/bowtie.xlsx
+++ b/assets/icons/bowtie.xlsx
@@ -31721,8 +31721,8 @@
   <dimension ref="A1:L326"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A311" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N318" sqref="N318"/>
+      <pane ySplit="1" topLeftCell="A293" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I299" sqref="I299"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -31798,10 +31798,6 @@
       <c r="J2" t="s">
         <v>256</v>
       </c>
-      <c r="K2" t="str">
-        <f>CONCATENATE(E2,"-",I2)</f>
-        <v>uE904-arrow-down-right.svg</v>
-      </c>
     </row>
     <row r="3" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -31825,10 +31821,6 @@
       <c r="J3" t="s">
         <v>258</v>
       </c>
-      <c r="K3" t="str">
-        <f t="shared" ref="K3:K66" si="0">CONCATENATE(E3,"-",I3)</f>
-        <v>uE903-arrow-down-left.svg</v>
-      </c>
     </row>
     <row r="4" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -31852,10 +31844,6 @@
       <c r="J4" t="s">
         <v>162</v>
       </c>
-      <c r="K4" t="str">
-        <f t="shared" si="0"/>
-        <v>uE905-arrow-down.svg</v>
-      </c>
     </row>
     <row r="5" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -31879,10 +31867,6 @@
       <c r="J5" t="s">
         <v>163</v>
       </c>
-      <c r="K5" t="str">
-        <f t="shared" si="0"/>
-        <v>uE906-arrow-left.svg</v>
-      </c>
     </row>
     <row r="6" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -31906,10 +31890,6 @@
       <c r="J6" t="s">
         <v>164</v>
       </c>
-      <c r="K6" t="str">
-        <f t="shared" si="0"/>
-        <v>uE907-arrow-right.svg</v>
-      </c>
     </row>
     <row r="7" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -31933,10 +31913,6 @@
       <c r="J7" t="s">
         <v>257</v>
       </c>
-      <c r="K7" t="str">
-        <f t="shared" si="0"/>
-        <v>uE908-arrow-up-left.svg</v>
-      </c>
     </row>
     <row r="8" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -31960,10 +31936,6 @@
       <c r="J8" t="s">
         <v>255</v>
       </c>
-      <c r="K8" t="str">
-        <f t="shared" si="0"/>
-        <v>uE909-arrow-up-right.svg</v>
-      </c>
     </row>
     <row r="9" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -31987,10 +31959,6 @@
       <c r="J9" t="s">
         <v>165</v>
       </c>
-      <c r="K9" t="str">
-        <f t="shared" si="0"/>
-        <v>uE90A-arrow-up.svg</v>
-      </c>
     </row>
     <row r="10" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -32014,10 +31982,6 @@
       <c r="J10" t="s">
         <v>159</v>
       </c>
-      <c r="K10" t="str">
-        <f t="shared" si="0"/>
-        <v>uE900-alert.svg</v>
-      </c>
     </row>
     <row r="11" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -32041,10 +32005,6 @@
       <c r="J11" t="s">
         <v>160</v>
       </c>
-      <c r="K11" t="str">
-        <f t="shared" si="0"/>
-        <v>uE901-approve.svg</v>
-      </c>
     </row>
     <row r="12" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -32068,10 +32028,6 @@
       <c r="J12" t="s">
         <v>161</v>
       </c>
-      <c r="K12" t="str">
-        <f t="shared" si="0"/>
-        <v>uE902-approve-disapprove.svg</v>
-      </c>
     </row>
     <row r="13" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -32095,10 +32051,6 @@
       <c r="J13" t="s">
         <v>166</v>
       </c>
-      <c r="K13" t="str">
-        <f t="shared" si="0"/>
-        <v>uE90B-attach.svg</v>
-      </c>
     </row>
     <row r="14" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -32122,10 +32074,6 @@
       <c r="J14" t="s">
         <v>63</v>
       </c>
-      <c r="K14" t="str">
-        <f t="shared" si="0"/>
-        <v>uE90B-auto-fill-template.svg</v>
-      </c>
     </row>
     <row r="15" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -32149,10 +32097,6 @@
       <c r="J15" t="s">
         <v>167</v>
       </c>
-      <c r="K15" t="str">
-        <f t="shared" si="0"/>
-        <v>uE90D-azure-api-management.svg</v>
-      </c>
     </row>
     <row r="16" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -32176,12 +32120,8 @@
       <c r="J16" t="s">
         <v>168</v>
       </c>
-      <c r="K16" t="str">
-        <f t="shared" si="0"/>
-        <v>uE90E-azure-service-endpoint.svg</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>160</v>
       </c>
@@ -32203,12 +32143,8 @@
       <c r="J17" t="s">
         <v>12</v>
       </c>
-      <c r="K17" t="str">
-        <f t="shared" si="0"/>
-        <v>uE90F-brand-android.svg</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>161</v>
       </c>
@@ -32230,12 +32166,8 @@
       <c r="J18" t="s">
         <v>13</v>
       </c>
-      <c r="K18" t="str">
-        <f t="shared" si="0"/>
-        <v>uE910-brand-facebook.svg</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>162</v>
       </c>
@@ -32257,12 +32189,8 @@
       <c r="J19" t="s">
         <v>14</v>
       </c>
-      <c r="K19" t="str">
-        <f t="shared" si="0"/>
-        <v>uE911-brand-git.svg</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>163</v>
       </c>
@@ -32284,12 +32212,8 @@
       <c r="J20" t="s">
         <v>15</v>
       </c>
-      <c r="K20" t="str">
-        <f t="shared" si="0"/>
-        <v>uE912-brand-github.svg</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>185</v>
       </c>
@@ -32311,12 +32235,8 @@
       <c r="J21" t="s">
         <v>35</v>
       </c>
-      <c r="K21" t="str">
-        <f t="shared" si="0"/>
-        <v>uE913-brand-maven.svg</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>183</v>
       </c>
@@ -32338,12 +32258,8 @@
       <c r="J22" t="s">
         <v>33</v>
       </c>
-      <c r="K22" t="str">
-        <f t="shared" si="0"/>
-        <v>uE914-brand-npm.svg</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>164</v>
       </c>
@@ -32365,12 +32281,8 @@
       <c r="J23" t="s">
         <v>16</v>
       </c>
-      <c r="K23" t="str">
-        <f t="shared" si="0"/>
-        <v>uE915-brand-nuget.svg</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>165</v>
       </c>
@@ -32392,12 +32304,8 @@
       <c r="J24" t="s">
         <v>17</v>
       </c>
-      <c r="K24" t="str">
-        <f t="shared" si="0"/>
-        <v>uE916-brand-tfvc.svg</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>166</v>
       </c>
@@ -32419,12 +32327,8 @@
       <c r="J25" t="s">
         <v>18</v>
       </c>
-      <c r="K25" t="str">
-        <f t="shared" si="0"/>
-        <v>uE917-brand-twitter.svg</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>167</v>
       </c>
@@ -32446,12 +32350,8 @@
       <c r="J26" t="s">
         <v>19</v>
       </c>
-      <c r="K26" t="str">
-        <f t="shared" si="0"/>
-        <v>uE918-brand-visualstudio.svg</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>168</v>
       </c>
@@ -32473,12 +32373,8 @@
       <c r="J27" t="s">
         <v>20</v>
       </c>
-      <c r="K27" t="str">
-        <f t="shared" si="0"/>
-        <v>uE919-brand-windows.svg</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>13</v>
       </c>
@@ -32500,12 +32396,8 @@
       <c r="J28" t="s">
         <v>102</v>
       </c>
-      <c r="K28" t="str">
-        <f t="shared" si="0"/>
-        <v>uE91A-build-qnew.svg</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>12</v>
       </c>
@@ -32527,12 +32419,8 @@
       <c r="J29" t="s">
         <v>101</v>
       </c>
-      <c r="K29" t="str">
-        <f t="shared" si="0"/>
-        <v>uE91B-build-queue.svg</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>14</v>
       </c>
@@ -32554,12 +32442,8 @@
       <c r="J30" t="s">
         <v>103</v>
       </c>
-      <c r="K30" t="str">
-        <f t="shared" si="0"/>
-        <v>uE91C-build-reason-checkin-shelveset.svg</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>11</v>
       </c>
@@ -32581,12 +32465,8 @@
       <c r="J31" t="s">
         <v>100</v>
       </c>
-      <c r="K31" t="str">
-        <f t="shared" si="0"/>
-        <v>uE91D-build.svg</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>169</v>
       </c>
@@ -32608,12 +32488,8 @@
       <c r="J32" t="s">
         <v>21</v>
       </c>
-      <c r="K32" t="str">
-        <f t="shared" si="0"/>
-        <v>uE91E-calendar-month.svg</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>15</v>
       </c>
@@ -32635,12 +32511,8 @@
       <c r="J33" t="s">
         <v>104</v>
       </c>
-      <c r="K33" t="str">
-        <f t="shared" si="0"/>
-        <v>uE91F-calendar.svg</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>225</v>
       </c>
@@ -32662,12 +32534,8 @@
       <c r="J34" t="s">
         <v>75</v>
       </c>
-      <c r="K34" t="str">
-        <f t="shared" si="0"/>
-        <v>uE920-chart-area.svg</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>216</v>
       </c>
@@ -32689,12 +32557,8 @@
       <c r="J35" t="s">
         <v>66</v>
       </c>
-      <c r="K35" t="str">
-        <f t="shared" si="0"/>
-        <v>uE921-chart-bar.svg</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>217</v>
       </c>
@@ -32716,12 +32580,8 @@
       <c r="J36" t="s">
         <v>67</v>
       </c>
-      <c r="K36" t="str">
-        <f t="shared" si="0"/>
-        <v>uE922-chart-column.svg</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>215</v>
       </c>
@@ -32743,12 +32603,8 @@
       <c r="J37" t="s">
         <v>65</v>
       </c>
-      <c r="K37" t="str">
-        <f t="shared" si="0"/>
-        <v>uE923-chart-pie.svg</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>224</v>
       </c>
@@ -32770,12 +32626,8 @@
       <c r="J38" t="s">
         <v>74</v>
       </c>
-      <c r="K38" t="str">
-        <f t="shared" si="0"/>
-        <v>uE924-chart-pivot.svg</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>229</v>
       </c>
@@ -32797,12 +32649,8 @@
       <c r="J39" t="s">
         <v>79</v>
       </c>
-      <c r="K39" t="str">
-        <f t="shared" si="0"/>
-        <v>uE925-chart-stacked-area.svg</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>219</v>
       </c>
@@ -32824,12 +32672,8 @@
       <c r="J40" t="s">
         <v>69</v>
       </c>
-      <c r="K40" t="str">
-        <f t="shared" si="0"/>
-        <v>uE926-chart-stacked-bar.svg</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>226</v>
       </c>
@@ -32851,12 +32695,8 @@
       <c r="J41" t="s">
         <v>76</v>
       </c>
-      <c r="K41" t="str">
-        <f t="shared" si="0"/>
-        <v>uE927-chart-stacked-line.svg</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>170</v>
       </c>
@@ -32878,12 +32718,8 @@
       <c r="J42" t="s">
         <v>22</v>
       </c>
-      <c r="K42" t="str">
-        <f t="shared" si="0"/>
-        <v>uE928-check-light.svg</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>16</v>
       </c>
@@ -32905,12 +32741,8 @@
       <c r="J43" t="s">
         <v>105</v>
       </c>
-      <c r="K43" t="str">
-        <f t="shared" si="0"/>
-        <v>uE929-check.svg</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>171</v>
       </c>
@@ -32932,12 +32764,8 @@
       <c r="J44" t="s">
         <v>4</v>
       </c>
-      <c r="K44" t="str">
-        <f t="shared" si="0"/>
-        <v>uE92A-checkbox-empty.svg</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>172</v>
       </c>
@@ -32959,12 +32787,8 @@
       <c r="J45" t="s">
         <v>5</v>
       </c>
-      <c r="K45" t="str">
-        <f t="shared" si="0"/>
-        <v>uE92B-checkbox.svg</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>17</v>
       </c>
@@ -32986,12 +32810,8 @@
       <c r="J46" t="s">
         <v>169</v>
       </c>
-      <c r="K46" t="str">
-        <f t="shared" si="0"/>
-        <v>uE92C-chevron-down-light.svg</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>18</v>
       </c>
@@ -33013,12 +32833,8 @@
       <c r="J47" t="s">
         <v>170</v>
       </c>
-      <c r="K47" t="str">
-        <f t="shared" si="0"/>
-        <v>uE92D-chevron-down.svg</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>19</v>
       </c>
@@ -33040,12 +32856,8 @@
       <c r="J48" t="s">
         <v>171</v>
       </c>
-      <c r="K48" t="str">
-        <f t="shared" si="0"/>
-        <v>uE92E-chevron-left-light.svg</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>20</v>
       </c>
@@ -33067,12 +32879,8 @@
       <c r="J49" t="s">
         <v>172</v>
       </c>
-      <c r="K49" t="str">
-        <f t="shared" si="0"/>
-        <v>uE92F-chevron-left.svg</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>21</v>
       </c>
@@ -33094,12 +32902,8 @@
       <c r="J50" t="s">
         <v>173</v>
       </c>
-      <c r="K50" t="str">
-        <f t="shared" si="0"/>
-        <v>uE930-chevron-right-light.svg</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>22</v>
       </c>
@@ -33121,12 +32925,8 @@
       <c r="J51" t="s">
         <v>174</v>
       </c>
-      <c r="K51" t="str">
-        <f t="shared" si="0"/>
-        <v>uE931-chevron-right.svg</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>23</v>
       </c>
@@ -33148,12 +32948,8 @@
       <c r="J52" t="s">
         <v>175</v>
       </c>
-      <c r="K52" t="str">
-        <f t="shared" si="0"/>
-        <v>uE932-chevron-up-light.svg</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>24</v>
       </c>
@@ -33175,12 +32971,8 @@
       <c r="J53" t="s">
         <v>176</v>
       </c>
-      <c r="K53" t="str">
-        <f t="shared" si="0"/>
-        <v>uE933-chevron-up.svg</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>25</v>
       </c>
@@ -33202,12 +32994,8 @@
       <c r="J54" t="s">
         <v>177</v>
       </c>
-      <c r="K54" t="str">
-        <f t="shared" si="0"/>
-        <v>uE934-clone-to-desktop.svg</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>26</v>
       </c>
@@ -33229,12 +33017,8 @@
       <c r="J55" t="s">
         <v>178</v>
       </c>
-      <c r="K55" t="str">
-        <f t="shared" si="0"/>
-        <v>uE935-clone.svg</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>173</v>
       </c>
@@ -33256,12 +33040,8 @@
       <c r="J56" t="s">
         <v>23</v>
       </c>
-      <c r="K56" t="str">
-        <f t="shared" si="0"/>
-        <v>uE936-cloud-fill.svg</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>27</v>
       </c>
@@ -33283,12 +33063,8 @@
       <c r="J57" t="s">
         <v>106</v>
       </c>
-      <c r="K57" t="str">
-        <f t="shared" si="0"/>
-        <v>uE937-cloud.svg</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>29</v>
       </c>
@@ -33310,12 +33086,8 @@
       <c r="J58" t="s">
         <v>108</v>
       </c>
-      <c r="K58" t="str">
-        <f t="shared" si="0"/>
-        <v>uE938-comment-add.svg</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>30</v>
       </c>
@@ -33337,12 +33109,8 @@
       <c r="J59" t="s">
         <v>109</v>
       </c>
-      <c r="K59" t="str">
-        <f t="shared" si="0"/>
-        <v>uE939-comment-discussion.svg</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>31</v>
       </c>
@@ -33364,12 +33132,8 @@
       <c r="J60" t="s">
         <v>110</v>
       </c>
-      <c r="K60" t="str">
-        <f t="shared" si="0"/>
-        <v>uE93A-comment-lines.svg</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>32</v>
       </c>
@@ -33391,12 +33155,8 @@
       <c r="J61" t="s">
         <v>111</v>
       </c>
-      <c r="K61" t="str">
-        <f t="shared" si="0"/>
-        <v>uE93B-comment-next.svg</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>33</v>
       </c>
@@ -33418,12 +33178,8 @@
       <c r="J62" t="s">
         <v>179</v>
       </c>
-      <c r="K62" t="str">
-        <f t="shared" si="0"/>
-        <v>uE93C-comment-outline.svg</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>34</v>
       </c>
@@ -33445,12 +33201,8 @@
       <c r="J63" t="s">
         <v>180</v>
       </c>
-      <c r="K63" t="str">
-        <f t="shared" si="0"/>
-        <v>uE93D-comment-previous.svg</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>35</v>
       </c>
@@ -33472,12 +33224,8 @@
       <c r="J64" t="s">
         <v>181</v>
       </c>
-      <c r="K64" t="str">
-        <f t="shared" si="0"/>
-        <v>uE93E-comment-urgent.svg</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>28</v>
       </c>
@@ -33499,12 +33247,8 @@
       <c r="J65" t="s">
         <v>107</v>
       </c>
-      <c r="K65" t="str">
-        <f t="shared" si="0"/>
-        <v>uE93F-comment.svg</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>174</v>
       </c>
@@ -33526,12 +33270,8 @@
       <c r="J66" t="s">
         <v>24</v>
       </c>
-      <c r="K66" t="str">
-        <f t="shared" si="0"/>
-        <v>uE940-connect-to-feed.svg</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>175</v>
       </c>
@@ -33553,12 +33293,8 @@
       <c r="J67" t="s">
         <v>25</v>
       </c>
-      <c r="K67" t="str">
-        <f t="shared" ref="K67:K130" si="1">CONCATENATE(E67,"-",I67)</f>
-        <v>uE941-copy-to-clipboard.svg</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>176</v>
       </c>
@@ -33580,12 +33316,8 @@
       <c r="J68" t="s">
         <v>26</v>
       </c>
-      <c r="K68" t="str">
-        <f t="shared" si="1"/>
-        <v>uE942-dashboard-fill.svg</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>36</v>
       </c>
@@ -33607,12 +33339,8 @@
       <c r="J69" t="s">
         <v>182</v>
       </c>
-      <c r="K69" t="str">
-        <f t="shared" si="1"/>
-        <v>uE943-dashboard.svg</v>
-      </c>
-    </row>
-    <row r="70" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>37</v>
       </c>
@@ -33634,12 +33362,8 @@
       <c r="J70" t="s">
         <v>183</v>
       </c>
-      <c r="K70" t="str">
-        <f t="shared" si="1"/>
-        <v>uE944-database.svg</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="71" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>190</v>
       </c>
@@ -33661,12 +33385,8 @@
       <c r="J71" t="s">
         <v>40</v>
       </c>
-      <c r="K71" t="str">
-        <f t="shared" si="1"/>
-        <v>uE945-details-pane.svg</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="72" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>38</v>
       </c>
@@ -33688,12 +33408,8 @@
       <c r="J72" t="s">
         <v>184</v>
       </c>
-      <c r="K72" t="str">
-        <f t="shared" si="1"/>
-        <v>uE946-diff-image-overlay.svg</v>
-      </c>
-    </row>
-    <row r="73" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="73" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>39</v>
       </c>
@@ -33715,12 +33431,8 @@
       <c r="J73" t="s">
         <v>185</v>
       </c>
-      <c r="K73" t="str">
-        <f t="shared" si="1"/>
-        <v>uE947-diff-image-pixel.svg</v>
-      </c>
-    </row>
-    <row r="74" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="74" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>40</v>
       </c>
@@ -33742,12 +33454,8 @@
       <c r="J74" t="s">
         <v>186</v>
       </c>
-      <c r="K74" t="str">
-        <f t="shared" si="1"/>
-        <v>uE948-diff-image.svg</v>
-      </c>
-    </row>
-    <row r="75" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="75" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>41</v>
       </c>
@@ -33769,12 +33477,8 @@
       <c r="J75" t="s">
         <v>187</v>
       </c>
-      <c r="K75" t="str">
-        <f t="shared" si="1"/>
-        <v>uE949-diff-inline.svg</v>
-      </c>
-    </row>
-    <row r="76" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="76" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>42</v>
       </c>
@@ -33796,12 +33500,8 @@
       <c r="J76" t="s">
         <v>188</v>
       </c>
-      <c r="K76" t="str">
-        <f t="shared" si="1"/>
-        <v>uE94A-diff-side-by-side.svg</v>
-      </c>
-    </row>
-    <row r="77" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="77" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>43</v>
       </c>
@@ -33823,12 +33523,8 @@
       <c r="J77" t="s">
         <v>112</v>
       </c>
-      <c r="K77" t="str">
-        <f t="shared" si="1"/>
-        <v>uE94B-dot.svg</v>
-      </c>
-    </row>
-    <row r="78" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="78" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>45</v>
       </c>
@@ -33850,12 +33546,8 @@
       <c r="J78" t="s">
         <v>114</v>
       </c>
-      <c r="K78" t="str">
-        <f t="shared" si="1"/>
-        <v>uE94C-edit-copy.svg</v>
-      </c>
-    </row>
-    <row r="79" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="79" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>46</v>
       </c>
@@ -33877,12 +33569,8 @@
       <c r="J79" t="s">
         <v>115</v>
       </c>
-      <c r="K79" t="str">
-        <f t="shared" si="1"/>
-        <v>uE94D-edit-cut.svg</v>
-      </c>
-    </row>
-    <row r="80" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="80" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>253</v>
       </c>
@@ -33904,12 +33592,8 @@
       <c r="J80" t="s">
         <v>254</v>
       </c>
-      <c r="K80" t="str">
-        <f t="shared" si="1"/>
-        <v>uE94E-edit-delete.svg</v>
-      </c>
-    </row>
-    <row r="81" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="81" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>261</v>
       </c>
@@ -33931,12 +33615,8 @@
       <c r="J81" t="s">
         <v>0</v>
       </c>
-      <c r="K81" t="str">
-        <f t="shared" si="1"/>
-        <v>uE94F-edit-outline.svg</v>
-      </c>
-    </row>
-    <row r="82" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="82" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>48</v>
       </c>
@@ -33958,12 +33638,8 @@
       <c r="J82" t="s">
         <v>117</v>
       </c>
-      <c r="K82" t="str">
-        <f t="shared" si="1"/>
-        <v>uE950-edit-paste.svg</v>
-      </c>
-    </row>
-    <row r="83" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="83" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>49</v>
       </c>
@@ -33985,12 +33661,8 @@
       <c r="J83" t="s">
         <v>189</v>
       </c>
-      <c r="K83" t="str">
-        <f t="shared" si="1"/>
-        <v>uE951-edit-redo.svg</v>
-      </c>
-    </row>
-    <row r="84" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="84" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>50</v>
       </c>
@@ -34012,12 +33684,8 @@
       <c r="J84" t="s">
         <v>190</v>
       </c>
-      <c r="K84" t="str">
-        <f t="shared" si="1"/>
-        <v>uE952-edit-remove.svg</v>
-      </c>
-    </row>
-    <row r="85" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="85" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>51</v>
       </c>
@@ -34039,12 +33707,8 @@
       <c r="J85" t="s">
         <v>191</v>
       </c>
-      <c r="K85" t="str">
-        <f t="shared" si="1"/>
-        <v>uE953-edit-rename.svg</v>
-      </c>
-    </row>
-    <row r="86" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="86" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>52</v>
       </c>
@@ -34066,12 +33730,8 @@
       <c r="J86" t="s">
         <v>192</v>
       </c>
-      <c r="K86" t="str">
-        <f t="shared" si="1"/>
-        <v>uE954-edit-undo.svg</v>
-      </c>
-    </row>
-    <row r="87" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="87" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>44</v>
       </c>
@@ -34093,12 +33753,8 @@
       <c r="J87" t="s">
         <v>113</v>
       </c>
-      <c r="K87" t="str">
-        <f t="shared" si="1"/>
-        <v>uE955-edit.svg</v>
-      </c>
-    </row>
-    <row r="88" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="88" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>53</v>
       </c>
@@ -34120,12 +33776,8 @@
       <c r="J88" t="s">
         <v>193</v>
       </c>
-      <c r="K88" t="str">
-        <f t="shared" si="1"/>
-        <v>uE956-editor-list-bullet.svg</v>
-      </c>
-    </row>
-    <row r="89" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="89" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>55</v>
       </c>
@@ -34147,12 +33799,8 @@
       <c r="J89" t="s">
         <v>3</v>
       </c>
-      <c r="K89" t="str">
-        <f t="shared" si="1"/>
-        <v>uE957-ellipsis.svg</v>
-      </c>
-    </row>
-    <row r="90" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="90" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>54</v>
       </c>
@@ -34174,12 +33822,8 @@
       <c r="J90" t="s">
         <v>2</v>
       </c>
-      <c r="K90" t="str">
-        <f t="shared" si="1"/>
-        <v>uE958-ellipsis-vertical.svg</v>
-      </c>
-    </row>
-    <row r="91" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="91" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>56</v>
       </c>
@@ -34201,12 +33845,8 @@
       <c r="J91" t="s">
         <v>194</v>
       </c>
-      <c r="K91" t="str">
-        <f t="shared" si="1"/>
-        <v>uE959-favorite-outline.svg</v>
-      </c>
-    </row>
-    <row r="92" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="92" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>57</v>
       </c>
@@ -34228,12 +33868,8 @@
       <c r="J92" t="s">
         <v>195</v>
       </c>
-      <c r="K92" t="str">
-        <f t="shared" si="1"/>
-        <v>uE95A-favorite.svg</v>
-      </c>
-    </row>
-    <row r="93" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="93" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>182</v>
       </c>
@@ -34255,12 +33891,8 @@
       <c r="J93" t="s">
         <v>32</v>
       </c>
-      <c r="K93" t="str">
-        <f t="shared" si="1"/>
-        <v>uE95B-feed.svg</v>
-      </c>
-    </row>
-    <row r="94" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="94" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>58</v>
       </c>
@@ -34282,12 +33914,8 @@
       <c r="J94" t="s">
         <v>196</v>
       </c>
-      <c r="K94" t="str">
-        <f t="shared" si="1"/>
-        <v>uE95C-feedback-negative.svg</v>
-      </c>
-    </row>
-    <row r="95" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="95" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>59</v>
       </c>
@@ -34309,12 +33937,8 @@
       <c r="J95" t="s">
         <v>118</v>
       </c>
-      <c r="K95" t="str">
-        <f t="shared" si="1"/>
-        <v>uE95D-feedback-positive.svg</v>
-      </c>
-    </row>
-    <row r="96" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="96" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>61</v>
       </c>
@@ -34336,12 +33960,8 @@
       <c r="J96" t="s">
         <v>120</v>
       </c>
-      <c r="K96" t="str">
-        <f t="shared" si="1"/>
-        <v>uE95E-file-code.svg</v>
-      </c>
-    </row>
-    <row r="97" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="97" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>62</v>
       </c>
@@ -34363,12 +33983,8 @@
       <c r="J97" t="s">
         <v>121</v>
       </c>
-      <c r="K97" t="str">
-        <f t="shared" si="1"/>
-        <v>uE95F-file-comment.svg</v>
-      </c>
-    </row>
-    <row r="98" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="98" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>63</v>
       </c>
@@ -34390,12 +34006,8 @@
       <c r="J98" t="s">
         <v>122</v>
       </c>
-      <c r="K98" t="str">
-        <f t="shared" si="1"/>
-        <v>uE960-file-content.svg</v>
-      </c>
-    </row>
-    <row r="99" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="99" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>64</v>
       </c>
@@ -34417,12 +34029,8 @@
       <c r="J99" t="s">
         <v>123</v>
       </c>
-      <c r="K99" t="str">
-        <f t="shared" si="1"/>
-        <v>uE961-file-image.svg</v>
-      </c>
-    </row>
-    <row r="100" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="100" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>65</v>
       </c>
@@ -34444,12 +34052,8 @@
       <c r="J100" t="s">
         <v>197</v>
       </c>
-      <c r="K100" t="str">
-        <f t="shared" si="1"/>
-        <v>uE962-file-preview.svg</v>
-      </c>
-    </row>
-    <row r="101" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="101" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>66</v>
       </c>
@@ -34471,12 +34075,8 @@
       <c r="J101" t="s">
         <v>198</v>
       </c>
-      <c r="K101" t="str">
-        <f t="shared" si="1"/>
-        <v>uE963-file-symlink.svg</v>
-      </c>
-    </row>
-    <row r="102" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="102" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>60</v>
       </c>
@@ -34498,12 +34098,8 @@
       <c r="J102" t="s">
         <v>119</v>
       </c>
-      <c r="K102" t="str">
-        <f t="shared" si="1"/>
-        <v>uE964-file.svg</v>
-      </c>
-    </row>
-    <row r="103" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="103" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>67</v>
       </c>
@@ -34525,12 +34121,8 @@
       <c r="J103" t="s">
         <v>199</v>
       </c>
-      <c r="K103" t="str">
-        <f t="shared" si="1"/>
-        <v>uE965-fold-less.svg</v>
-      </c>
-    </row>
-    <row r="104" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="104" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>68</v>
       </c>
@@ -34552,12 +34144,8 @@
       <c r="J104" t="s">
         <v>200</v>
       </c>
-      <c r="K104" t="str">
-        <f t="shared" si="1"/>
-        <v>uE966-fold-more.svg</v>
-      </c>
-    </row>
-    <row r="105" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="105" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>69</v>
       </c>
@@ -34579,12 +34167,8 @@
       <c r="J105" t="s">
         <v>201</v>
       </c>
-      <c r="K105" t="str">
-        <f t="shared" si="1"/>
-        <v>uE967-folder.svg</v>
-      </c>
-    </row>
-    <row r="106" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="106" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>222</v>
       </c>
@@ -34606,12 +34190,8 @@
       <c r="J106" t="s">
         <v>72</v>
       </c>
-      <c r="K106" t="str">
-        <f t="shared" si="1"/>
-        <v>uE968-format-bold.svg</v>
-      </c>
-    </row>
-    <row r="107" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="107" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>236</v>
       </c>
@@ -34633,12 +34213,8 @@
       <c r="J107" t="s">
         <v>86</v>
       </c>
-      <c r="K107" t="str">
-        <f t="shared" si="1"/>
-        <v>uE969-format-clear.svg</v>
-      </c>
-    </row>
-    <row r="108" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="108" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>242</v>
       </c>
@@ -34660,12 +34236,8 @@
       <c r="J108" t="s">
         <v>92</v>
       </c>
-      <c r="K108" t="str">
-        <f t="shared" si="1"/>
-        <v>uE96A-format-font-color.svg</v>
-      </c>
-    </row>
-    <row r="109" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="109" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>243</v>
       </c>
@@ -34687,12 +34259,8 @@
       <c r="J109" t="s">
         <v>93</v>
       </c>
-      <c r="K109" t="str">
-        <f t="shared" si="1"/>
-        <v>uE96B-format-font-size.svg</v>
-      </c>
-    </row>
-    <row r="110" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="110" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>244</v>
       </c>
@@ -34714,12 +34282,8 @@
       <c r="J110" t="s">
         <v>94</v>
       </c>
-      <c r="K110" t="str">
-        <f t="shared" si="1"/>
-        <v>uE96C-format-indent-decrease.svg</v>
-      </c>
-    </row>
-    <row r="111" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="111" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>245</v>
       </c>
@@ -34741,12 +34305,8 @@
       <c r="J111" t="s">
         <v>95</v>
       </c>
-      <c r="K111" t="str">
-        <f t="shared" si="1"/>
-        <v>uE96D-format-indent-increase.svg</v>
-      </c>
-    </row>
-    <row r="112" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="112" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>246</v>
       </c>
@@ -34768,12 +34328,8 @@
       <c r="J112" t="s">
         <v>96</v>
       </c>
-      <c r="K112" t="str">
-        <f t="shared" si="1"/>
-        <v>uE96E-format-italic.svg</v>
-      </c>
-    </row>
-    <row r="113" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="113" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>247</v>
       </c>
@@ -34795,12 +34351,8 @@
       <c r="J113" t="s">
         <v>97</v>
       </c>
-      <c r="K113" t="str">
-        <f t="shared" si="1"/>
-        <v>uE96F-format-list-ordered.svg</v>
-      </c>
-    </row>
-    <row r="114" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="114" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>248</v>
       </c>
@@ -34822,12 +34374,8 @@
       <c r="J114" t="s">
         <v>98</v>
       </c>
-      <c r="K114" t="str">
-        <f t="shared" si="1"/>
-        <v>uE970-format-list-unordered.svg</v>
-      </c>
-    </row>
-    <row r="115" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="115" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>249</v>
       </c>
@@ -34849,12 +34397,8 @@
       <c r="J115" t="s">
         <v>99</v>
       </c>
-      <c r="K115" t="str">
-        <f t="shared" si="1"/>
-        <v>uE971-format-underline.svg</v>
-      </c>
-    </row>
-    <row r="116" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="116" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>70</v>
       </c>
@@ -34876,12 +34420,8 @@
       <c r="J116" t="s">
         <v>202</v>
       </c>
-      <c r="K116" t="str">
-        <f t="shared" si="1"/>
-        <v>uE972-git.svg</v>
-      </c>
-    </row>
-    <row r="117" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="117" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>187</v>
       </c>
@@ -34903,12 +34443,8 @@
       <c r="J117" t="s">
         <v>37</v>
       </c>
-      <c r="K117" t="str">
-        <f t="shared" si="1"/>
-        <v>uE973-heart-fill.svg</v>
-      </c>
-    </row>
-    <row r="118" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="118" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>188</v>
       </c>
@@ -34930,12 +34466,8 @@
       <c r="J118" t="s">
         <v>38</v>
       </c>
-      <c r="K118" t="str">
-        <f t="shared" si="1"/>
-        <v>uE974-heart.svg</v>
-      </c>
-    </row>
-    <row r="119" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="119" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>189</v>
       </c>
@@ -34957,12 +34489,8 @@
       <c r="J119" t="s">
         <v>39</v>
       </c>
-      <c r="K119" t="str">
-        <f t="shared" si="1"/>
-        <v>uE975-heartbeat-fill.svg</v>
-      </c>
-    </row>
-    <row r="120" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="120" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>71</v>
       </c>
@@ -34984,12 +34512,8 @@
       <c r="J120" t="s">
         <v>203</v>
       </c>
-      <c r="K120" t="str">
-        <f t="shared" si="1"/>
-        <v>uE976-heartbeat.svg</v>
-      </c>
-    </row>
-    <row r="121" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="121" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>191</v>
       </c>
@@ -35011,12 +34535,8 @@
       <c r="J121" t="s">
         <v>41</v>
       </c>
-      <c r="K121" t="str">
-        <f t="shared" si="1"/>
-        <v>uE977-image.svg</v>
-      </c>
-    </row>
-    <row r="122" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="122" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>72</v>
       </c>
@@ -35038,12 +34558,8 @@
       <c r="J122" t="s">
         <v>204</v>
       </c>
-      <c r="K122" t="str">
-        <f t="shared" si="1"/>
-        <v>uE978-install.svg</v>
-      </c>
-    </row>
-    <row r="123" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="123" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>73</v>
       </c>
@@ -35065,12 +34581,8 @@
       <c r="J123" t="s">
         <v>205</v>
       </c>
-      <c r="K123" t="str">
-        <f t="shared" si="1"/>
-        <v>uE979-link.svg</v>
-      </c>
-    </row>
-    <row r="124" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="124" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>74</v>
       </c>
@@ -35092,12 +34604,8 @@
       <c r="J124" t="s">
         <v>206</v>
       </c>
-      <c r="K124" t="str">
-        <f t="shared" si="1"/>
-        <v>uE97A-logo-visual-studio.svg</v>
-      </c>
-    </row>
-    <row r="125" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="125" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>192</v>
       </c>
@@ -35119,12 +34627,8 @@
       <c r="J125" t="s">
         <v>42</v>
       </c>
-      <c r="K125" t="str">
-        <f t="shared" si="1"/>
-        <v>uE97B-mail-message-fill.svg</v>
-      </c>
-    </row>
-    <row r="126" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="126" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>75</v>
       </c>
@@ -35146,12 +34650,8 @@
       <c r="J126" t="s">
         <v>124</v>
       </c>
-      <c r="K126" t="str">
-        <f t="shared" si="1"/>
-        <v>uE97C-mail-message.svg</v>
-      </c>
-    </row>
-    <row r="127" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="127" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>250</v>
       </c>
@@ -35173,12 +34673,8 @@
       <c r="J127" t="s">
         <v>8</v>
       </c>
-      <c r="K127" t="str">
-        <f t="shared" si="1"/>
-        <v>uE97D-math-minus-box-light.svg</v>
-      </c>
-    </row>
-    <row r="128" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="128" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>77</v>
       </c>
@@ -35200,12 +34696,8 @@
       <c r="J128" t="s">
         <v>126</v>
       </c>
-      <c r="K128" t="str">
-        <f t="shared" si="1"/>
-        <v>uE97E-math-minus-box.svg</v>
-      </c>
-    </row>
-    <row r="129" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="129" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>193</v>
       </c>
@@ -35227,12 +34719,8 @@
       <c r="J129" t="s">
         <v>43</v>
       </c>
-      <c r="K129" t="str">
-        <f t="shared" si="1"/>
-        <v>uE97F-math-minus-circle-outline.svg</v>
-      </c>
-    </row>
-    <row r="130" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="130" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>78</v>
       </c>
@@ -35254,12 +34742,8 @@
       <c r="J130" t="s">
         <v>127</v>
       </c>
-      <c r="K130" t="str">
-        <f t="shared" si="1"/>
-        <v>uE980-math-minus-circle.svg</v>
-      </c>
-    </row>
-    <row r="131" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="131" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>194</v>
       </c>
@@ -35281,12 +34765,8 @@
       <c r="J131" t="s">
         <v>44</v>
       </c>
-      <c r="K131" t="str">
-        <f t="shared" ref="K131:K194" si="2">CONCATENATE(E131,"-",I131)</f>
-        <v>uE981-math-minus-light.svg</v>
-      </c>
-    </row>
-    <row r="132" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="132" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>76</v>
       </c>
@@ -35308,12 +34788,8 @@
       <c r="J132" t="s">
         <v>125</v>
       </c>
-      <c r="K132" t="str">
-        <f t="shared" si="2"/>
-        <v>uE982-math-minus.svg</v>
-      </c>
-    </row>
-    <row r="133" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="133" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>251</v>
       </c>
@@ -35335,12 +34811,8 @@
       <c r="J133" t="s">
         <v>7</v>
       </c>
-      <c r="K133" t="str">
-        <f t="shared" si="2"/>
-        <v>uE983-math-multiply-box-light.svg</v>
-      </c>
-    </row>
-    <row r="134" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="134" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>195</v>
       </c>
@@ -35362,12 +34834,8 @@
       <c r="J134" t="s">
         <v>45</v>
       </c>
-      <c r="K134" t="str">
-        <f t="shared" si="2"/>
-        <v>uE984-math-multiply-box-outline.svg</v>
-      </c>
-    </row>
-    <row r="135" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="135" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>196</v>
       </c>
@@ -35389,12 +34857,8 @@
       <c r="J135" t="s">
         <v>46</v>
       </c>
-      <c r="K135" t="str">
-        <f t="shared" si="2"/>
-        <v>uE985-math-multiply-box.svg</v>
-      </c>
-    </row>
-    <row r="136" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="136" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>197</v>
       </c>
@@ -35416,12 +34880,8 @@
       <c r="J136" t="s">
         <v>47</v>
       </c>
-      <c r="K136" t="str">
-        <f t="shared" si="2"/>
-        <v>uE986-math-multiply-light.svg</v>
-      </c>
-    </row>
-    <row r="137" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="137" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>79</v>
       </c>
@@ -35443,12 +34903,8 @@
       <c r="J137" t="s">
         <v>128</v>
       </c>
-      <c r="K137" t="str">
-        <f t="shared" si="2"/>
-        <v>uE987-math-multiply.svg</v>
-      </c>
-    </row>
-    <row r="138" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="138" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>252</v>
       </c>
@@ -35470,12 +34926,8 @@
       <c r="J138" t="s">
         <v>6</v>
       </c>
-      <c r="K138" t="str">
-        <f t="shared" si="2"/>
-        <v>uE988-math-plus-box-light.svg</v>
-      </c>
-    </row>
-    <row r="139" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="139" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>80</v>
       </c>
@@ -35497,12 +34949,8 @@
       <c r="J139" t="s">
         <v>207</v>
       </c>
-      <c r="K139" t="str">
-        <f t="shared" si="2"/>
-        <v>uE989-math-plus-box.svg</v>
-      </c>
-    </row>
-    <row r="140" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="140" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>198</v>
       </c>
@@ -35524,12 +34972,8 @@
       <c r="J140" t="s">
         <v>48</v>
       </c>
-      <c r="K140" t="str">
-        <f t="shared" si="2"/>
-        <v>uE98A-math-plus-circle-outline.svg</v>
-      </c>
-    </row>
-    <row r="141" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="141" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>81</v>
       </c>
@@ -35551,12 +34995,8 @@
       <c r="J141" t="s">
         <v>208</v>
       </c>
-      <c r="K141" t="str">
-        <f t="shared" si="2"/>
-        <v>uE98B-math-plus-circle.svg</v>
-      </c>
-    </row>
-    <row r="142" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="142" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>82</v>
       </c>
@@ -35578,12 +35018,8 @@
       <c r="J142" t="s">
         <v>209</v>
       </c>
-      <c r="K142" t="str">
-        <f t="shared" si="2"/>
-        <v>uE98C-math-plus-heavy.svg</v>
-      </c>
-    </row>
-    <row r="143" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="143" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>199</v>
       </c>
@@ -35605,12 +35041,8 @@
       <c r="J143" t="s">
         <v>49</v>
       </c>
-      <c r="K143" t="str">
-        <f t="shared" si="2"/>
-        <v>uE98D-math-plus-light.svg</v>
-      </c>
-    </row>
-    <row r="144" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="144" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>83</v>
       </c>
@@ -35632,12 +35064,8 @@
       <c r="J144" t="s">
         <v>210</v>
       </c>
-      <c r="K144" t="str">
-        <f t="shared" si="2"/>
-        <v>uE98E-math-plus.svg</v>
-      </c>
-    </row>
-    <row r="145" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="145" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>200</v>
       </c>
@@ -35659,12 +35087,8 @@
       <c r="J145" t="s">
         <v>50</v>
       </c>
-      <c r="K145" t="str">
-        <f t="shared" si="2"/>
-        <v>uE98F-media-play-fill.svg</v>
-      </c>
-    </row>
-    <row r="146" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="146" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>84</v>
       </c>
@@ -35686,12 +35110,8 @@
       <c r="J146" t="s">
         <v>211</v>
       </c>
-      <c r="K146" t="str">
-        <f t="shared" si="2"/>
-        <v>uE990-media-play.svg</v>
-      </c>
-    </row>
-    <row r="147" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="147" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>85</v>
       </c>
@@ -35713,12 +35133,8 @@
       <c r="J147" t="s">
         <v>212</v>
       </c>
-      <c r="K147" t="str">
-        <f t="shared" si="2"/>
-        <v>uE991-menu.svg</v>
-      </c>
-    </row>
-    <row r="148" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="148" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>86</v>
       </c>
@@ -35740,12 +35156,8 @@
       <c r="J148" t="s">
         <v>213</v>
       </c>
-      <c r="K148" t="str">
-        <f t="shared" si="2"/>
-        <v>uE992-navigate-back-circle.svg</v>
-      </c>
-    </row>
-    <row r="149" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="149" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>87</v>
       </c>
@@ -35767,12 +35179,8 @@
       <c r="J149" t="s">
         <v>214</v>
       </c>
-      <c r="K149" t="str">
-        <f t="shared" si="2"/>
-        <v>uE993-navigate-back-disc.svg</v>
-      </c>
-    </row>
-    <row r="150" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="150" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>88</v>
       </c>
@@ -35794,12 +35202,8 @@
       <c r="J150" t="s">
         <v>215</v>
       </c>
-      <c r="K150" t="str">
-        <f t="shared" si="2"/>
-        <v>uE994-navigate-close.svg</v>
-      </c>
-    </row>
-    <row r="151" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="151" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>89</v>
       </c>
@@ -35821,12 +35225,8 @@
       <c r="J151" t="s">
         <v>216</v>
       </c>
-      <c r="K151" t="str">
-        <f t="shared" si="2"/>
-        <v>uE995-navigate-external.svg</v>
-      </c>
-    </row>
-    <row r="152" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="152" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>90</v>
       </c>
@@ -35848,12 +35248,8 @@
       <c r="J152" t="s">
         <v>129</v>
       </c>
-      <c r="K152" t="str">
-        <f t="shared" si="2"/>
-        <v>uE996-navigate-forward-circle.svg</v>
-      </c>
-    </row>
-    <row r="153" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="153" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>91</v>
       </c>
@@ -35875,12 +35271,8 @@
       <c r="J153" t="s">
         <v>130</v>
       </c>
-      <c r="K153" t="str">
-        <f t="shared" si="2"/>
-        <v>uE997-navigate-forward-disc.svg</v>
-      </c>
-    </row>
-    <row r="154" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="154" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>92</v>
       </c>
@@ -35902,12 +35294,8 @@
       <c r="J154" t="s">
         <v>131</v>
       </c>
-      <c r="K154" t="str">
-        <f t="shared" si="2"/>
-        <v>uE998-navigate-history.svg</v>
-      </c>
-    </row>
-    <row r="155" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="155" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>93</v>
       </c>
@@ -35929,12 +35317,8 @@
       <c r="J155" t="s">
         <v>132</v>
       </c>
-      <c r="K155" t="str">
-        <f t="shared" si="2"/>
-        <v>uE999-navigate-refresh.svg</v>
-      </c>
-    </row>
-    <row r="156" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="156" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>94</v>
       </c>
@@ -35956,12 +35340,8 @@
       <c r="J156" t="s">
         <v>133</v>
       </c>
-      <c r="K156" t="str">
-        <f t="shared" si="2"/>
-        <v>uE99A-navigate-reload.svg</v>
-      </c>
-    </row>
-    <row r="157" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="157" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>201</v>
       </c>
@@ -35983,12 +35363,8 @@
       <c r="J157" t="s">
         <v>51</v>
       </c>
-      <c r="K157" t="str">
-        <f t="shared" si="2"/>
-        <v>uE99B-network-tower.svg</v>
-      </c>
-    </row>
-    <row r="158" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="158" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>202</v>
       </c>
@@ -36010,12 +35386,8 @@
       <c r="J158" t="s">
         <v>52</v>
       </c>
-      <c r="K158" t="str">
-        <f t="shared" si="2"/>
-        <v>uE99C-package-fill.svg</v>
-      </c>
-    </row>
-    <row r="159" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="159" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>95</v>
       </c>
@@ -36037,12 +35409,8 @@
       <c r="J159" t="s">
         <v>134</v>
       </c>
-      <c r="K159" t="str">
-        <f t="shared" si="2"/>
-        <v>uE99D-package.svg</v>
-      </c>
-    </row>
-    <row r="160" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="160" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>203</v>
       </c>
@@ -36064,12 +35432,8 @@
       <c r="J160" t="s">
         <v>53</v>
       </c>
-      <c r="K160" t="str">
-        <f t="shared" si="2"/>
-        <v>uE99E-pin-fill.svg</v>
-      </c>
-    </row>
-    <row r="161" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="161" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>204</v>
       </c>
@@ -36091,12 +35455,8 @@
       <c r="J161" t="s">
         <v>54</v>
       </c>
-      <c r="K161" t="str">
-        <f t="shared" si="2"/>
-        <v>uE99F-pin-pinned-fill.svg</v>
-      </c>
-    </row>
-    <row r="162" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="162" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>205</v>
       </c>
@@ -36118,12 +35478,8 @@
       <c r="J162" t="s">
         <v>55</v>
       </c>
-      <c r="K162" t="str">
-        <f t="shared" si="2"/>
-        <v>uE9A0-pin-pinned.svg</v>
-      </c>
-    </row>
-    <row r="163" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="163" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>206</v>
       </c>
@@ -36145,12 +35501,8 @@
       <c r="J163" t="s">
         <v>56</v>
       </c>
-      <c r="K163" t="str">
-        <f t="shared" si="2"/>
-        <v>uE9A1-pin-unpin-fill.svg</v>
-      </c>
-    </row>
-    <row r="164" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="164" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>207</v>
       </c>
@@ -36172,12 +35524,8 @@
       <c r="J164" t="s">
         <v>57</v>
       </c>
-      <c r="K164" t="str">
-        <f t="shared" si="2"/>
-        <v>uE9A2-pin-unpin.svg</v>
-      </c>
-    </row>
-    <row r="165" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="165" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>96</v>
       </c>
@@ -36199,12 +35547,8 @@
       <c r="J165" t="s">
         <v>217</v>
       </c>
-      <c r="K165" t="str">
-        <f t="shared" si="2"/>
-        <v>uE9A3-pin.svg</v>
-      </c>
-    </row>
-    <row r="166" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="166" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>260</v>
       </c>
@@ -36226,12 +35570,8 @@
       <c r="J166" t="s">
         <v>261</v>
       </c>
-      <c r="K166" t="str">
-        <f t="shared" si="2"/>
-        <v>uE9A4-plug-outline.svg</v>
-      </c>
-    </row>
-    <row r="167" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="167" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>208</v>
       </c>
@@ -36253,12 +35593,8 @@
       <c r="J167" t="s">
         <v>58</v>
       </c>
-      <c r="K167" t="str">
-        <f t="shared" si="2"/>
-        <v>uE9A5-plug.svg</v>
-      </c>
-    </row>
-    <row r="168" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="168" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>230</v>
       </c>
@@ -36280,12 +35616,8 @@
       <c r="J168" t="s">
         <v>80</v>
       </c>
-      <c r="K168" t="str">
-        <f t="shared" si="2"/>
-        <v>uE9A6-policy.svg</v>
-      </c>
-    </row>
-    <row r="169" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="169" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>209</v>
       </c>
@@ -36307,12 +35639,8 @@
       <c r="J169" t="s">
         <v>59</v>
       </c>
-      <c r="K169" t="str">
-        <f t="shared" si="2"/>
-        <v>uE9A7-radio-button-empty.svg</v>
-      </c>
-    </row>
-    <row r="170" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="170" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>210</v>
       </c>
@@ -36334,12 +35662,8 @@
       <c r="J170" t="s">
         <v>60</v>
       </c>
-      <c r="K170" t="str">
-        <f t="shared" si="2"/>
-        <v>uE9A8-radio-button.svg</v>
-      </c>
-    </row>
-    <row r="171" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="171" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>218</v>
       </c>
@@ -36361,12 +35685,8 @@
       <c r="J171" t="s">
         <v>68</v>
       </c>
-      <c r="K171" t="str">
-        <f t="shared" si="2"/>
-        <v>uE9A9-recycle-bin-restore.svg</v>
-      </c>
-    </row>
-    <row r="172" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="172" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>211</v>
       </c>
@@ -36388,12 +35708,8 @@
       <c r="J172" t="s">
         <v>61</v>
       </c>
-      <c r="K172" t="str">
-        <f t="shared" si="2"/>
-        <v>uE9AA-recycle-bin.svg</v>
-      </c>
-    </row>
-    <row r="173" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="173" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>233</v>
       </c>
@@ -36415,12 +35731,8 @@
       <c r="J173" t="s">
         <v>83</v>
       </c>
-      <c r="K173" t="str">
-        <f t="shared" si="2"/>
-        <v>uE9AB-recycle.svg</v>
-      </c>
-    </row>
-    <row r="174" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="174" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>99</v>
       </c>
@@ -36442,12 +35754,8 @@
       <c r="J174" t="s">
         <v>220</v>
       </c>
-      <c r="K174" t="str">
-        <f t="shared" si="2"/>
-        <v>uE9AC-repo-fill.svg</v>
-      </c>
-    </row>
-    <row r="175" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="175" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>97</v>
       </c>
@@ -36469,12 +35777,8 @@
       <c r="J175" t="s">
         <v>218</v>
       </c>
-      <c r="K175" t="str">
-        <f t="shared" si="2"/>
-        <v>uE9AD-repo-git.svg</v>
-      </c>
-    </row>
-    <row r="176" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="176" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>100</v>
       </c>
@@ -36496,12 +35800,8 @@
       <c r="J176" t="s">
         <v>221</v>
       </c>
-      <c r="K176" t="str">
-        <f t="shared" si="2"/>
-        <v>uE9AE-repo-submodule.svg</v>
-      </c>
-    </row>
-    <row r="177" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="177" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>98</v>
       </c>
@@ -36523,12 +35823,8 @@
       <c r="J177" t="s">
         <v>219</v>
       </c>
-      <c r="K177" t="str">
-        <f t="shared" si="2"/>
-        <v>uE9AF-repo-tfvc.svg</v>
-      </c>
-    </row>
-    <row r="178" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="178" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>234</v>
       </c>
@@ -36550,12 +35846,8 @@
       <c r="J178" t="s">
         <v>84</v>
       </c>
-      <c r="K178" t="str">
-        <f t="shared" si="2"/>
-        <v>uE9B0-repo.svg</v>
-      </c>
-    </row>
-    <row r="179" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="179" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>101</v>
       </c>
@@ -36577,12 +35869,8 @@
       <c r="J179" t="s">
         <v>222</v>
       </c>
-      <c r="K179" t="str">
-        <f t="shared" si="2"/>
-        <v>uE9B1-save.svg</v>
-      </c>
-    </row>
-    <row r="180" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="180" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>220</v>
       </c>
@@ -36604,12 +35892,8 @@
       <c r="J180" t="s">
         <v>70</v>
       </c>
-      <c r="K180" t="str">
-        <f t="shared" si="2"/>
-        <v>uE9B2-search-filter-fill.svg</v>
-      </c>
-    </row>
-    <row r="181" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="181" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>102</v>
       </c>
@@ -36631,12 +35915,8 @@
       <c r="J181" t="s">
         <v>223</v>
       </c>
-      <c r="K181" t="str">
-        <f t="shared" si="2"/>
-        <v>uE9B3-search-filter.svg</v>
-      </c>
-    </row>
-    <row r="182" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="182" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>103</v>
       </c>
@@ -36658,12 +35938,8 @@
       <c r="J182" t="s">
         <v>224</v>
       </c>
-      <c r="K182" t="str">
-        <f t="shared" si="2"/>
-        <v>uE9B4-search.svg</v>
-      </c>
-    </row>
-    <row r="183" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="183" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>105</v>
       </c>
@@ -36685,12 +35961,8 @@
       <c r="J183" t="s">
         <v>135</v>
       </c>
-      <c r="K183" t="str">
-        <f t="shared" si="2"/>
-        <v>uE9B5-security-access.svg</v>
-      </c>
-    </row>
-    <row r="184" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="184" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>221</v>
       </c>
@@ -36712,12 +35984,8 @@
       <c r="J184" t="s">
         <v>71</v>
       </c>
-      <c r="K184" t="str">
-        <f t="shared" si="2"/>
-        <v>uE9B6-security-lock-fill.svg</v>
-      </c>
-    </row>
-    <row r="185" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="185" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>106</v>
       </c>
@@ -36739,12 +36007,8 @@
       <c r="J185" t="s">
         <v>136</v>
       </c>
-      <c r="K185" t="str">
-        <f t="shared" si="2"/>
-        <v>uE9B7-security-lock.svg</v>
-      </c>
-    </row>
-    <row r="186" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="186" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>223</v>
       </c>
@@ -36766,12 +36030,8 @@
       <c r="J186" t="s">
         <v>73</v>
       </c>
-      <c r="K186" t="str">
-        <f t="shared" si="2"/>
-        <v>uE9B8-security-unlock-fill.svg</v>
-      </c>
-    </row>
-    <row r="187" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="187" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>107</v>
       </c>
@@ -36793,12 +36053,8 @@
       <c r="J187" t="s">
         <v>137</v>
       </c>
-      <c r="K187" t="str">
-        <f t="shared" si="2"/>
-        <v>uE9B9-security-unlock.svg</v>
-      </c>
-    </row>
-    <row r="188" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="188" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>104</v>
       </c>
@@ -36820,12 +36076,8 @@
       <c r="J188" t="s">
         <v>225</v>
       </c>
-      <c r="K188" t="str">
-        <f t="shared" si="2"/>
-        <v>uE9BA-security.svg</v>
-      </c>
-    </row>
-    <row r="189" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="189" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>108</v>
       </c>
@@ -36847,12 +36099,8 @@
       <c r="J189" t="s">
         <v>138</v>
       </c>
-      <c r="K189" t="str">
-        <f t="shared" si="2"/>
-        <v>uE9BB-separator.svg</v>
-      </c>
-    </row>
-    <row r="190" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="190" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>109</v>
       </c>
@@ -36874,12 +36122,8 @@
       <c r="J190" t="s">
         <v>139</v>
       </c>
-      <c r="K190" t="str">
-        <f t="shared" si="2"/>
-        <v>uE9BC-settings-gear.svg</v>
-      </c>
-    </row>
-    <row r="191" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="191" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>110</v>
       </c>
@@ -36901,12 +36145,8 @@
       <c r="J191" t="s">
         <v>140</v>
       </c>
-      <c r="K191" t="str">
-        <f t="shared" si="2"/>
-        <v>uE9BD-settings-wrench.svg</v>
-      </c>
-    </row>
-    <row r="192" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="192" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>111</v>
       </c>
@@ -36928,12 +36168,8 @@
       <c r="J192" t="s">
         <v>226</v>
       </c>
-      <c r="K192" t="str">
-        <f t="shared" si="2"/>
-        <v>uE9BE-share.svg</v>
-      </c>
-    </row>
-    <row r="193" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="193" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>240</v>
       </c>
@@ -36955,12 +36191,8 @@
       <c r="J193" t="s">
         <v>90</v>
       </c>
-      <c r="K193" t="str">
-        <f t="shared" si="2"/>
-        <v>uE9BF-shop-server.svg</v>
-      </c>
-    </row>
-    <row r="194" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="194" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>112</v>
       </c>
@@ -36982,12 +36214,8 @@
       <c r="J194" t="s">
         <v>227</v>
       </c>
-      <c r="K194" t="str">
-        <f t="shared" si="2"/>
-        <v>uE9C0-shop.svg</v>
-      </c>
-    </row>
-    <row r="195" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="195" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>113</v>
       </c>
@@ -37009,12 +36237,8 @@
       <c r="J195" t="s">
         <v>228</v>
       </c>
-      <c r="K195" t="str">
-        <f t="shared" ref="K195:K258" si="3">CONCATENATE(E195,"-",I195)</f>
-        <v>uE9C1-sort-ascending.svg</v>
-      </c>
-    </row>
-    <row r="196" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="196" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>114</v>
       </c>
@@ -37036,12 +36260,8 @@
       <c r="J196" t="s">
         <v>229</v>
       </c>
-      <c r="K196" t="str">
-        <f t="shared" si="3"/>
-        <v>uE9C2-sort-descending.svg</v>
-      </c>
-    </row>
-    <row r="197" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="197" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>227</v>
       </c>
@@ -37063,12 +36283,8 @@
       <c r="J197" t="s">
         <v>77</v>
       </c>
-      <c r="K197" t="str">
-        <f t="shared" si="3"/>
-        <v>uE9C3-sort.svg</v>
-      </c>
-    </row>
-    <row r="198" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="198" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>115</v>
       </c>
@@ -37090,12 +36306,8 @@
       <c r="J198" t="s">
         <v>230</v>
       </c>
-      <c r="K198" t="str">
-        <f t="shared" si="3"/>
-        <v>uE9C4-square.svg</v>
-      </c>
-    </row>
-    <row r="199" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="199" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>228</v>
       </c>
@@ -37117,12 +36329,8 @@
       <c r="J199" t="s">
         <v>78</v>
       </c>
-      <c r="K199" t="str">
-        <f t="shared" si="3"/>
-        <v>uE9C5-star-half.svg</v>
-      </c>
-    </row>
-    <row r="200" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="200" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>262</v>
       </c>
@@ -37144,12 +36352,8 @@
       <c r="J200" t="s">
         <v>1</v>
       </c>
-      <c r="K200" t="str">
-        <f t="shared" si="3"/>
-        <v>uE9C6-status-error-outline.svg</v>
-      </c>
-    </row>
-    <row r="201" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="201" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>116</v>
       </c>
@@ -37171,12 +36375,8 @@
       <c r="J201" t="s">
         <v>231</v>
       </c>
-      <c r="K201" t="str">
-        <f t="shared" si="3"/>
-        <v>uE9C7-status-error.svg</v>
-      </c>
-    </row>
-    <row r="202" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="202" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>158</v>
       </c>
@@ -37198,12 +36398,8 @@
       <c r="J202" t="s">
         <v>10</v>
       </c>
-      <c r="K202" t="str">
-        <f t="shared" si="3"/>
-        <v>uE9C8-status-failure-outline.svg</v>
-      </c>
-    </row>
-    <row r="203" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="203" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>117</v>
       </c>
@@ -37225,12 +36421,8 @@
       <c r="J203" t="s">
         <v>232</v>
       </c>
-      <c r="K203" t="str">
-        <f t="shared" si="3"/>
-        <v>uE9C9-status-failure.svg</v>
-      </c>
-    </row>
-    <row r="204" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="204" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>231</v>
       </c>
@@ -37252,12 +36444,8 @@
       <c r="J204" t="s">
         <v>81</v>
       </c>
-      <c r="K204" t="str">
-        <f t="shared" si="3"/>
-        <v>uE9CA-status-help-outline.svg</v>
-      </c>
-    </row>
-    <row r="205" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="205" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A205">
         <v>118</v>
       </c>
@@ -37279,12 +36467,8 @@
       <c r="J205" t="s">
         <v>233</v>
       </c>
-      <c r="K205" t="str">
-        <f t="shared" si="3"/>
-        <v>uE9CB-status-help.svg</v>
-      </c>
-    </row>
-    <row r="206" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="206" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A206">
         <v>119</v>
       </c>
@@ -37306,12 +36490,8 @@
       <c r="J206" t="s">
         <v>141</v>
       </c>
-      <c r="K206" t="str">
-        <f t="shared" si="3"/>
-        <v>uE9CC-status-info-outline.svg</v>
-      </c>
-    </row>
-    <row r="207" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="207" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A207">
         <v>120</v>
       </c>
@@ -37333,12 +36513,8 @@
       <c r="J207" t="s">
         <v>142</v>
       </c>
-      <c r="K207" t="str">
-        <f t="shared" si="3"/>
-        <v>uE9CD-status-info.svg</v>
-      </c>
-    </row>
-    <row r="208" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="208" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A208">
         <v>232</v>
       </c>
@@ -37360,12 +36536,8 @@
       <c r="J208" t="s">
         <v>82</v>
       </c>
-      <c r="K208" t="str">
-        <f t="shared" si="3"/>
-        <v>uE9CE-status-no-fill.svg</v>
-      </c>
-    </row>
-    <row r="209" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="209" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>177</v>
       </c>
@@ -37387,12 +36559,8 @@
       <c r="J209" t="s">
         <v>27</v>
       </c>
-      <c r="K209" t="str">
-        <f t="shared" si="3"/>
-        <v>uE9CF-status-no.svg</v>
-      </c>
-    </row>
-    <row r="210" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="210" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A210">
         <v>180</v>
       </c>
@@ -37414,12 +36582,8 @@
       <c r="J210" t="s">
         <v>30</v>
       </c>
-      <c r="K210" t="str">
-        <f t="shared" si="3"/>
-        <v>uE9D0-status-pause-outline.svg</v>
-      </c>
-    </row>
-    <row r="211" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="211" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>179</v>
       </c>
@@ -37441,12 +36605,8 @@
       <c r="J211" t="s">
         <v>29</v>
       </c>
-      <c r="K211" t="str">
-        <f t="shared" si="3"/>
-        <v>uE9D1-status-pause.svg</v>
-      </c>
-    </row>
-    <row r="212" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="212" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A212">
         <v>259</v>
       </c>
@@ -37468,12 +36628,8 @@
       <c r="J212" t="s">
         <v>260</v>
       </c>
-      <c r="K212" t="str">
-        <f t="shared" si="3"/>
-        <v>uE9D2-status-run-outline.svg</v>
-      </c>
-    </row>
-    <row r="213" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="213" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A213">
         <v>258</v>
       </c>
@@ -37495,12 +36651,8 @@
       <c r="J213" t="s">
         <v>259</v>
       </c>
-      <c r="K213" t="str">
-        <f t="shared" si="3"/>
-        <v>uE9D3-status-run.svg</v>
-      </c>
-    </row>
-    <row r="214" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="214" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A214">
         <v>184</v>
       </c>
@@ -37522,12 +36674,8 @@
       <c r="J214" t="s">
         <v>34</v>
       </c>
-      <c r="K214" t="str">
-        <f t="shared" si="3"/>
-        <v>uE9D4-status-stop-outline.svg</v>
-      </c>
-    </row>
-    <row r="215" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="215" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A215">
         <v>181</v>
       </c>
@@ -37549,12 +36697,8 @@
       <c r="J215" t="s">
         <v>31</v>
       </c>
-      <c r="K215" t="str">
-        <f t="shared" si="3"/>
-        <v>uE9D5-status-stop.svg</v>
-      </c>
-    </row>
-    <row r="216" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="216" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A216">
         <v>239</v>
       </c>
@@ -37576,12 +36720,8 @@
       <c r="J216" t="s">
         <v>89</v>
       </c>
-      <c r="K216" t="str">
-        <f t="shared" si="3"/>
-        <v>uE9D6-status-success-box.svg</v>
-      </c>
-    </row>
-    <row r="217" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="217" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A217">
         <v>159</v>
       </c>
@@ -37603,12 +36743,8 @@
       <c r="J217" t="s">
         <v>11</v>
       </c>
-      <c r="K217" t="str">
-        <f t="shared" si="3"/>
-        <v>uE9D7-status-success-outline.svg</v>
-      </c>
-    </row>
-    <row r="218" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="218" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A218">
         <v>121</v>
       </c>
@@ -37630,12 +36766,8 @@
       <c r="J218" t="s">
         <v>143</v>
       </c>
-      <c r="K218" t="str">
-        <f t="shared" si="3"/>
-        <v>uE9D8-status-success.svg</v>
-      </c>
-    </row>
-    <row r="219" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="219" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A219">
         <v>186</v>
       </c>
@@ -37657,12 +36789,8 @@
       <c r="J219" t="s">
         <v>36</v>
       </c>
-      <c r="K219" t="str">
-        <f t="shared" si="3"/>
-        <v>uE9D9-status-waiting-fill.svg</v>
-      </c>
-    </row>
-    <row r="220" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="220" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A220">
         <v>122</v>
       </c>
@@ -37684,12 +36812,8 @@
       <c r="J220" t="s">
         <v>144</v>
       </c>
-      <c r="K220" t="str">
-        <f t="shared" si="3"/>
-        <v>uE9DA-status-waiting.svg</v>
-      </c>
-    </row>
-    <row r="221" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="221" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A221">
         <v>178</v>
       </c>
@@ -37711,12 +36835,8 @@
       <c r="J221" t="s">
         <v>28</v>
       </c>
-      <c r="K221" t="str">
-        <f t="shared" si="3"/>
-        <v>uE9DB-status-warning-outline.svg</v>
-      </c>
-    </row>
-    <row r="222" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="222" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A222">
         <v>123</v>
       </c>
@@ -37738,12 +36858,8 @@
       <c r="J222" t="s">
         <v>145</v>
       </c>
-      <c r="K222" t="str">
-        <f t="shared" si="3"/>
-        <v>uE9DC-status-warning.svg</v>
-      </c>
-    </row>
-    <row r="223" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="223" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A223">
         <v>214</v>
       </c>
@@ -37765,12 +36881,8 @@
       <c r="J223" t="s">
         <v>64</v>
       </c>
-      <c r="K223" t="str">
-        <f t="shared" si="3"/>
-        <v>uE9DD-storyboard.svg</v>
-      </c>
-    </row>
-    <row r="224" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="224" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A224">
         <v>124</v>
       </c>
@@ -37792,12 +36904,8 @@
       <c r="J224" t="s">
         <v>146</v>
       </c>
-      <c r="K224" t="str">
-        <f t="shared" si="3"/>
-        <v>uE9DE-switch.svg</v>
-      </c>
-    </row>
-    <row r="225" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="225" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A225">
         <v>237</v>
       </c>
@@ -37819,12 +36927,8 @@
       <c r="J225" t="s">
         <v>87</v>
       </c>
-      <c r="K225" t="str">
-        <f t="shared" si="3"/>
-        <v>uE9DF-synchronize.svg</v>
-      </c>
-    </row>
-    <row r="226" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="226" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A226">
         <v>238</v>
       </c>
@@ -37846,12 +36950,8 @@
       <c r="J226" t="s">
         <v>88</v>
       </c>
-      <c r="K226" t="str">
-        <f t="shared" si="3"/>
-        <v>uE9E0-tag-fill.svg</v>
-      </c>
-    </row>
-    <row r="227" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="227" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A227">
         <v>125</v>
       </c>
@@ -37873,12 +36973,8 @@
       <c r="J227" t="s">
         <v>234</v>
       </c>
-      <c r="K227" t="str">
-        <f t="shared" si="3"/>
-        <v>uE9E1-tag.svg</v>
-      </c>
-    </row>
-    <row r="228" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="228" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A228">
         <v>126</v>
       </c>
@@ -37900,12 +36996,8 @@
       <c r="J228" t="s">
         <v>235</v>
       </c>
-      <c r="K228" t="str">
-        <f t="shared" si="3"/>
-        <v>uE9E2-tfvc-branch-locked.svg</v>
-      </c>
-    </row>
-    <row r="229" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="229" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A229">
         <v>127</v>
       </c>
@@ -37927,12 +37019,8 @@
       <c r="J229" t="s">
         <v>236</v>
       </c>
-      <c r="K229" t="str">
-        <f t="shared" si="3"/>
-        <v>uE9E3-tfvc-branch.svg</v>
-      </c>
-    </row>
-    <row r="230" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="230" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A230">
         <v>128</v>
       </c>
@@ -37954,12 +37042,8 @@
       <c r="J230" t="s">
         <v>237</v>
       </c>
-      <c r="K230" t="str">
-        <f t="shared" si="3"/>
-        <v>uE9E4-tfvc-change-list.svg</v>
-      </c>
-    </row>
-    <row r="231" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="231" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A231">
         <v>129</v>
       </c>
@@ -37981,12 +37065,8 @@
       <c r="J231" t="s">
         <v>238</v>
       </c>
-      <c r="K231" t="str">
-        <f t="shared" si="3"/>
-        <v>uE9E5-tfvc-commit.svg</v>
-      </c>
-    </row>
-    <row r="232" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="232" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A232">
         <v>130</v>
       </c>
@@ -38008,12 +37088,8 @@
       <c r="J232" t="s">
         <v>239</v>
       </c>
-      <c r="K232" t="str">
-        <f t="shared" si="3"/>
-        <v>uE9E6-tfvc-compare.svg</v>
-      </c>
-    </row>
-    <row r="233" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="233" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A233">
         <v>241</v>
       </c>
@@ -38035,12 +37111,8 @@
       <c r="J233" t="s">
         <v>91</v>
       </c>
-      <c r="K233" t="str">
-        <f t="shared" si="3"/>
-        <v>uE9E7-tfvc-folder.svg</v>
-      </c>
-    </row>
-    <row r="234" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="234" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A234">
         <v>131</v>
       </c>
@@ -38062,12 +37134,8 @@
       <c r="J234" t="s">
         <v>240</v>
       </c>
-      <c r="K234" t="str">
-        <f t="shared" si="3"/>
-        <v>uE9E8-tfvc-merge.svg</v>
-      </c>
-    </row>
-    <row r="235" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="235" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A235">
         <v>132</v>
       </c>
@@ -38089,12 +37157,8 @@
       <c r="J235" t="s">
         <v>241</v>
       </c>
-      <c r="K235" t="str">
-        <f t="shared" si="3"/>
-        <v>uE9E9-tfvc-pull-request.svg</v>
-      </c>
-    </row>
-    <row r="236" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="236" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A236">
         <v>133</v>
       </c>
@@ -38116,12 +37180,8 @@
       <c r="J236" t="s">
         <v>242</v>
       </c>
-      <c r="K236" t="str">
-        <f t="shared" si="3"/>
-        <v>uE9EA-tfvc-raw-source.svg</v>
-      </c>
-    </row>
-    <row r="237" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="237" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A237">
         <v>134</v>
       </c>
@@ -38143,12 +37203,8 @@
       <c r="J237" t="s">
         <v>243</v>
       </c>
-      <c r="K237" t="str">
-        <f t="shared" si="3"/>
-        <v>uE9EB-tfvc-repo.svg</v>
-      </c>
-    </row>
-    <row r="238" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="238" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A238">
         <v>135</v>
       </c>
@@ -38170,12 +37226,8 @@
       <c r="J238" t="s">
         <v>147</v>
       </c>
-      <c r="K238" t="str">
-        <f t="shared" si="3"/>
-        <v>uE9EC-tfvc-shelveset.svg</v>
-      </c>
-    </row>
-    <row r="239" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="239" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A239">
         <v>136</v>
       </c>
@@ -38197,12 +37249,8 @@
       <c r="J239" t="s">
         <v>148</v>
       </c>
-      <c r="K239" t="str">
-        <f t="shared" si="3"/>
-        <v>uE9ED-toggle-collapse-all.svg</v>
-      </c>
-    </row>
-    <row r="240" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="240" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A240">
         <v>137</v>
       </c>
@@ -38224,12 +37272,8 @@
       <c r="J240" t="s">
         <v>149</v>
       </c>
-      <c r="K240" t="str">
-        <f t="shared" si="3"/>
-        <v>uE9EE-toggle-collapse.svg</v>
-      </c>
-    </row>
-    <row r="241" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="241" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A241">
         <v>138</v>
       </c>
@@ -38251,12 +37295,8 @@
       <c r="J241" t="s">
         <v>150</v>
       </c>
-      <c r="K241" t="str">
-        <f t="shared" si="3"/>
-        <v>uE9EF-toggle-expand-all.svg</v>
-      </c>
-    </row>
-    <row r="242" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="242" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A242">
         <v>139</v>
       </c>
@@ -38278,12 +37318,8 @@
       <c r="J242" t="s">
         <v>151</v>
       </c>
-      <c r="K242" t="str">
-        <f t="shared" si="3"/>
-        <v>uE9F0-toggle-expand.svg</v>
-      </c>
-    </row>
-    <row r="243" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="243" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A243">
         <v>140</v>
       </c>
@@ -38305,12 +37341,8 @@
       <c r="J243" t="s">
         <v>152</v>
       </c>
-      <c r="K243" t="str">
-        <f t="shared" si="3"/>
-        <v>uE9F1-toggle-tree-collapsed.svg</v>
-      </c>
-    </row>
-    <row r="244" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="244" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A244">
         <v>141</v>
       </c>
@@ -38332,12 +37364,8 @@
       <c r="J244" t="s">
         <v>244</v>
       </c>
-      <c r="K244" t="str">
-        <f t="shared" si="3"/>
-        <v>uE9F2-toggle-tree-expanded.svg</v>
-      </c>
-    </row>
-    <row r="245" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="245" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A245">
         <v>142</v>
       </c>
@@ -38359,12 +37387,8 @@
       <c r="J245" t="s">
         <v>245</v>
       </c>
-      <c r="K245" t="str">
-        <f t="shared" si="3"/>
-        <v>uE9F3-transfer-download.svg</v>
-      </c>
-    </row>
-    <row r="246" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="246" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A246">
         <v>143</v>
       </c>
@@ -38386,12 +37410,8 @@
       <c r="J246" t="s">
         <v>246</v>
       </c>
-      <c r="K246" t="str">
-        <f t="shared" si="3"/>
-        <v>uE9F4-transfer-upload.svg</v>
-      </c>
-    </row>
-    <row r="247" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="247" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A247">
         <v>47</v>
       </c>
@@ -38413,12 +37433,8 @@
       <c r="J247" t="s">
         <v>116</v>
       </c>
-      <c r="K247" t="str">
-        <f t="shared" si="3"/>
-        <v>uE9F5-trash.svg</v>
-      </c>
-    </row>
-    <row r="248" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="248" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A248">
         <v>144</v>
       </c>
@@ -38440,12 +37456,8 @@
       <c r="J248" t="s">
         <v>247</v>
       </c>
-      <c r="K248" t="str">
-        <f t="shared" si="3"/>
-        <v>uE9F6-triangle-down.svg</v>
-      </c>
-    </row>
-    <row r="249" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="249" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A249">
         <v>145</v>
       </c>
@@ -38467,12 +37479,8 @@
       <c r="J249" t="s">
         <v>248</v>
       </c>
-      <c r="K249" t="str">
-        <f t="shared" si="3"/>
-        <v>uE9F7-triangle-left.svg</v>
-      </c>
-    </row>
-    <row r="250" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="250" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A250">
         <v>146</v>
       </c>
@@ -38494,12 +37502,8 @@
       <c r="J250" t="s">
         <v>249</v>
       </c>
-      <c r="K250" t="str">
-        <f t="shared" si="3"/>
-        <v>uE9F8-triangle-right.svg</v>
-      </c>
-    </row>
-    <row r="251" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="251" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A251">
         <v>147</v>
       </c>
@@ -38521,12 +37525,8 @@
       <c r="J251" t="s">
         <v>250</v>
       </c>
-      <c r="K251" t="str">
-        <f t="shared" si="3"/>
-        <v>uE9F9-triangle-up.svg</v>
-      </c>
-    </row>
-    <row r="252" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="252" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A252">
         <v>148</v>
       </c>
@@ -38548,12 +37548,8 @@
       <c r="J252" t="s">
         <v>251</v>
       </c>
-      <c r="K252" t="str">
-        <f t="shared" si="3"/>
-        <v>uE9FA-user.svg</v>
-      </c>
-    </row>
-    <row r="253" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="253" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A253">
         <v>149</v>
       </c>
@@ -38575,12 +37571,8 @@
       <c r="J253" t="s">
         <v>252</v>
       </c>
-      <c r="K253" t="str">
-        <f t="shared" si="3"/>
-        <v>uE9FB-users.svg</v>
-      </c>
-    </row>
-    <row r="254" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="254" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A254">
         <v>151</v>
       </c>
@@ -38602,12 +37594,8 @@
       <c r="J254" t="s">
         <v>153</v>
       </c>
-      <c r="K254" t="str">
-        <f t="shared" si="3"/>
-        <v>uE9FC-view-full-screen-exit.svg</v>
-      </c>
-    </row>
-    <row r="255" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="255" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A255">
         <v>150</v>
       </c>
@@ -38629,12 +37617,8 @@
       <c r="J255" t="s">
         <v>253</v>
       </c>
-      <c r="K255" t="str">
-        <f t="shared" si="3"/>
-        <v>uE9FD-view-full-screen.svg</v>
-      </c>
-    </row>
-    <row r="256" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="256" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A256">
         <v>212</v>
       </c>
@@ -38655,10 +37639,6 @@
       </c>
       <c r="J256" t="s">
         <v>62</v>
-      </c>
-      <c r="K256" t="str">
-        <f t="shared" si="3"/>
-        <v>uE9FE-view-grid.svg</v>
       </c>
     </row>
     <row r="257" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -38683,10 +37663,6 @@
       <c r="J257" t="s">
         <v>154</v>
       </c>
-      <c r="K257" t="str">
-        <f t="shared" si="3"/>
-        <v>uE9FF-view-list-group.svg</v>
-      </c>
     </row>
     <row r="258" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A258">
@@ -38710,10 +37686,6 @@
       <c r="J258" t="s">
         <v>155</v>
       </c>
-      <c r="K258" t="str">
-        <f t="shared" si="3"/>
-        <v>uEA00-view-list-tree.svg</v>
-      </c>
     </row>
     <row r="259" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A259">
@@ -38737,10 +37709,6 @@
       <c r="J259" t="s">
         <v>156</v>
       </c>
-      <c r="K259" t="str">
-        <f t="shared" ref="K259:K301" si="4">CONCATENATE(E259,"-",I259)</f>
-        <v>uEA01-view-list.svg</v>
-      </c>
     </row>
     <row r="260" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A260">
@@ -38764,10 +37732,6 @@
       <c r="J260" t="s">
         <v>157</v>
       </c>
-      <c r="K260" t="str">
-        <f t="shared" si="4"/>
-        <v>uEA02-watch-eye.svg</v>
-      </c>
     </row>
     <row r="261" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A261">
@@ -38791,10 +37755,6 @@
       <c r="J261" t="s">
         <v>9</v>
       </c>
-      <c r="K261" t="str">
-        <f t="shared" si="4"/>
-        <v>uEA03-work-item-bar.svg</v>
-      </c>
     </row>
     <row r="262" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A262">
@@ -38818,10 +37778,6 @@
       <c r="J262" t="s">
         <v>85</v>
       </c>
-      <c r="K262" t="str">
-        <f t="shared" si="4"/>
-        <v>uEA04-work-item-move.svg</v>
-      </c>
     </row>
     <row r="263" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A263">
@@ -38845,10 +37801,6 @@
       <c r="J263" t="s">
         <v>158</v>
       </c>
-      <c r="K263" t="str">
-        <f t="shared" si="4"/>
-        <v>uEA05-work-item.svg</v>
-      </c>
     </row>
     <row r="264" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C264" t="s">
@@ -38870,10 +37822,6 @@
       <c r="J264" t="s">
         <v>1092</v>
       </c>
-      <c r="K264" t="str">
-        <f t="shared" si="4"/>
-        <v>uEA27-watch-eye-fill.svg</v>
-      </c>
       <c r="L264" t="s">
         <v>1244</v>
       </c>
@@ -38883,7 +37831,7 @@
         <v>1126</v>
       </c>
       <c r="D265" s="4">
-        <f t="shared" ref="D265:D296" si="5">HEX2DEC(REPLACE(C265,1,2,""))</f>
+        <f t="shared" ref="D265:D296" si="0">HEX2DEC(REPLACE(C265,1,2,""))</f>
         <v>2659</v>
       </c>
       <c r="E265" s="1" t="s">
@@ -38897,10 +37845,6 @@
       </c>
       <c r="J265" t="s">
         <v>1093</v>
-      </c>
-      <c r="K265" t="str">
-        <f t="shared" si="4"/>
-        <v>uE911-blur.svg</v>
       </c>
       <c r="L265" t="s">
         <v>1244</v>
@@ -38911,7 +37855,7 @@
         <v>1127</v>
       </c>
       <c r="D266" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="0"/>
         <v>2660</v>
       </c>
       <c r="E266" s="1" t="s">
@@ -38925,10 +37869,6 @@
       </c>
       <c r="J266" t="s">
         <v>1094</v>
-      </c>
-      <c r="K266" t="str">
-        <f t="shared" si="4"/>
-        <v>uE924-camera.svg</v>
       </c>
       <c r="L266" t="s">
         <v>1244</v>
@@ -38939,7 +37879,7 @@
         <v>1128</v>
       </c>
       <c r="D267" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="0"/>
         <v>2661</v>
       </c>
       <c r="E267" s="1" t="s">
@@ -38953,10 +37893,6 @@
       </c>
       <c r="J267" t="s">
         <v>1095</v>
-      </c>
-      <c r="K267" t="str">
-        <f t="shared" si="4"/>
-        <v>uE9FF-test-user.svg</v>
       </c>
       <c r="L267" t="s">
         <v>1244</v>
@@ -38967,7 +37903,7 @@
         <v>1129</v>
       </c>
       <c r="D268" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="0"/>
         <v>2662</v>
       </c>
       <c r="E268" s="1" t="s">
@@ -38981,10 +37917,6 @@
       </c>
       <c r="J268" t="s">
         <v>1096</v>
-      </c>
-      <c r="K268" t="str">
-        <f t="shared" si="4"/>
-        <v>uEA1C-trigger.svg</v>
       </c>
       <c r="L268" t="s">
         <v>1244</v>
@@ -38995,7 +37927,7 @@
         <v>1130</v>
       </c>
       <c r="D269" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="0"/>
         <v>2663</v>
       </c>
       <c r="E269" s="1" t="s">
@@ -39009,10 +37941,6 @@
       </c>
       <c r="J269" t="s">
         <v>1097</v>
-      </c>
-      <c r="K269" t="str">
-        <f t="shared" si="4"/>
-        <v>uEA1A-trigger-auto.svg</v>
       </c>
       <c r="L269" t="s">
         <v>1244</v>
@@ -39023,7 +37951,7 @@
         <v>1131</v>
       </c>
       <c r="D270" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="0"/>
         <v>2664</v>
       </c>
       <c r="E270" s="1" t="s">
@@ -39037,10 +37965,6 @@
       </c>
       <c r="J270" t="s">
         <v>1098</v>
-      </c>
-      <c r="K270" t="str">
-        <f t="shared" si="4"/>
-        <v>uEA1B-trigger-user.svg</v>
       </c>
       <c r="L270" t="s">
         <v>1244</v>
@@ -39051,7 +37975,7 @@
         <v>1132</v>
       </c>
       <c r="D271" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="0"/>
         <v>2665</v>
       </c>
       <c r="E271" s="1" t="s">
@@ -39065,10 +37989,6 @@
       </c>
       <c r="J271" t="s">
         <v>1099</v>
-      </c>
-      <c r="K271" t="str">
-        <f t="shared" si="4"/>
-        <v>uEA1F-variable.svg</v>
       </c>
       <c r="L271" t="s">
         <v>1244</v>
@@ -39079,7 +37999,7 @@
         <v>1133</v>
       </c>
       <c r="D272" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="0"/>
         <v>2666</v>
       </c>
       <c r="E272" s="1" t="s">
@@ -39093,10 +38013,6 @@
       </c>
       <c r="J272" t="s">
         <v>1100</v>
-      </c>
-      <c r="K272" t="str">
-        <f t="shared" si="4"/>
-        <v>uE9FD-test-fill.svg</v>
       </c>
       <c r="L272" t="s">
         <v>1244</v>
@@ -39107,7 +38023,7 @@
         <v>1134</v>
       </c>
       <c r="D273" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="0"/>
         <v>2667</v>
       </c>
       <c r="E273" s="1" t="s">
@@ -39121,10 +38037,6 @@
       </c>
       <c r="J273" t="s">
         <v>1101</v>
-      </c>
-      <c r="K273" t="str">
-        <f t="shared" si="4"/>
-        <v>uE950-devices.svg</v>
       </c>
       <c r="L273" t="s">
         <v>1244</v>
@@ -39135,7 +38047,7 @@
         <v>1135</v>
       </c>
       <c r="D274" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="0"/>
         <v>2668</v>
       </c>
       <c r="E274" s="1" t="s">
@@ -39149,10 +38061,6 @@
       </c>
       <c r="J274" t="s">
         <v>1102</v>
-      </c>
-      <c r="K274" t="str">
-        <f t="shared" si="4"/>
-        <v>uE979-format-font.svg</v>
       </c>
       <c r="L274" t="s">
         <v>1244</v>
@@ -39163,7 +38071,7 @@
         <v>1136</v>
       </c>
       <c r="D275" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="0"/>
         <v>2669</v>
       </c>
       <c r="E275" s="1" t="s">
@@ -39177,10 +38085,6 @@
       </c>
       <c r="J275" t="s">
         <v>1103</v>
-      </c>
-      <c r="K275" t="str">
-        <f t="shared" si="4"/>
-        <v>uE9A2-merge-duplicate.svg</v>
       </c>
       <c r="L275" t="s">
         <v>1244</v>
@@ -39191,7 +38095,7 @@
         <v>1137</v>
       </c>
       <c r="D276" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="0"/>
         <v>2670</v>
       </c>
       <c r="E276" s="1" t="s">
@@ -39205,10 +38109,6 @@
       </c>
       <c r="J276" t="s">
         <v>1104</v>
-      </c>
-      <c r="K276" t="str">
-        <f t="shared" si="4"/>
-        <v>uE94E-deploy.svg</v>
       </c>
       <c r="L276" t="s">
         <v>1244</v>
@@ -39219,7 +38119,7 @@
         <v>1138</v>
       </c>
       <c r="D277" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="0"/>
         <v>2671</v>
       </c>
       <c r="E277" s="1" t="s">
@@ -39233,10 +38133,6 @@
       </c>
       <c r="J277" t="s">
         <v>1105</v>
-      </c>
-      <c r="K277" t="str">
-        <f t="shared" si="4"/>
-        <v>uE9BE-redeploy.svg</v>
       </c>
       <c r="L277" t="s">
         <v>1244</v>
@@ -39247,7 +38143,7 @@
         <v>1139</v>
       </c>
       <c r="D278" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="0"/>
         <v>2672</v>
       </c>
       <c r="E278" s="1" t="s">
@@ -39261,10 +38157,6 @@
       </c>
       <c r="J278" t="s">
         <v>1106</v>
-      </c>
-      <c r="K278" t="str">
-        <f t="shared" si="4"/>
-        <v>uE9F4-step.svg</v>
       </c>
       <c r="L278" t="s">
         <v>1244</v>
@@ -39275,7 +38167,7 @@
         <v>1140</v>
       </c>
       <c r="D279" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="0"/>
         <v>2673</v>
       </c>
       <c r="E279" s="1" t="s">
@@ -39289,10 +38181,6 @@
       </c>
       <c r="J279" t="s">
         <v>1107</v>
-      </c>
-      <c r="K279" t="str">
-        <f t="shared" si="4"/>
-        <v>uE9C4-robot.svg</v>
       </c>
       <c r="L279" t="s">
         <v>1244</v>
@@ -39303,7 +38191,7 @@
         <v>1141</v>
       </c>
       <c r="D280" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="0"/>
         <v>2674</v>
       </c>
       <c r="E280" s="1" t="s">
@@ -39317,10 +38205,6 @@
       </c>
       <c r="J280" t="s">
         <v>1108</v>
-      </c>
-      <c r="K280" t="str">
-        <f t="shared" si="4"/>
-        <v>uE989-log.svg</v>
       </c>
       <c r="L280" t="s">
         <v>1244</v>
@@ -39331,7 +38215,7 @@
         <v>1142</v>
       </c>
       <c r="D281" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="0"/>
         <v>2675</v>
       </c>
       <c r="E281" s="1" t="s">
@@ -39345,10 +38229,6 @@
       </c>
       <c r="J281" t="s">
         <v>1109</v>
-      </c>
-      <c r="K281" t="str">
-        <f t="shared" si="4"/>
-        <v>uE9D1-server.svg</v>
       </c>
       <c r="L281" t="s">
         <v>1244</v>
@@ -39359,7 +38239,7 @@
         <v>1143</v>
       </c>
       <c r="D282" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="0"/>
         <v>2676</v>
       </c>
       <c r="E282" s="1" t="s">
@@ -39373,10 +38253,6 @@
       </c>
       <c r="J282" t="s">
         <v>1110</v>
-      </c>
-      <c r="K282" t="str">
-        <f t="shared" si="4"/>
-        <v>uE964-environment.svg</v>
       </c>
       <c r="L282" t="s">
         <v>1244</v>
@@ -39387,7 +38263,7 @@
         <v>1144</v>
       </c>
       <c r="D283" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="0"/>
         <v>2677</v>
       </c>
       <c r="E283" s="1" t="s">
@@ -39401,10 +38277,6 @@
       </c>
       <c r="J283" t="s">
         <v>1111</v>
-      </c>
-      <c r="K283" t="str">
-        <f t="shared" si="4"/>
-        <v>uEA00-test.svg</v>
       </c>
       <c r="L283" t="s">
         <v>1244</v>
@@ -39415,7 +38287,7 @@
         <v>1145</v>
       </c>
       <c r="D284" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="0"/>
         <v>2678</v>
       </c>
       <c r="E284" s="1" t="s">
@@ -39429,10 +38301,6 @@
       </c>
       <c r="J284" t="s">
         <v>1112</v>
-      </c>
-      <c r="K284" t="str">
-        <f t="shared" si="4"/>
-        <v>uE9FB-test-auto.svg</v>
       </c>
       <c r="L284" t="s">
         <v>1244</v>
@@ -39443,7 +38311,7 @@
         <v>1146</v>
       </c>
       <c r="D285" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="0"/>
         <v>2679</v>
       </c>
       <c r="E285" s="1" t="s">
@@ -39457,10 +38325,6 @@
       </c>
       <c r="J285" t="s">
         <v>1113</v>
-      </c>
-      <c r="K285" t="str">
-        <f t="shared" si="4"/>
-        <v>uE9FA-test-auto-fill.svg</v>
       </c>
       <c r="L285" t="s">
         <v>1244</v>
@@ -39471,7 +38335,7 @@
         <v>1147</v>
       </c>
       <c r="D286" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="0"/>
         <v>2680</v>
       </c>
       <c r="E286" s="1" t="s">
@@ -39485,10 +38349,6 @@
       </c>
       <c r="J286" t="s">
         <v>1114</v>
-      </c>
-      <c r="K286" t="str">
-        <f t="shared" si="4"/>
-        <v>uE9FE-test-user-fill.svg</v>
       </c>
       <c r="L286" t="s">
         <v>1244</v>
@@ -39499,7 +38359,7 @@
         <v>1148</v>
       </c>
       <c r="D287" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="0"/>
         <v>2681</v>
       </c>
       <c r="E287" s="1" t="s">
@@ -39513,10 +38373,6 @@
       </c>
       <c r="J287" t="s">
         <v>1115</v>
-      </c>
-      <c r="K287" t="str">
-        <f t="shared" si="4"/>
-        <v>uE9FC-test-explore-fill.svg</v>
       </c>
       <c r="L287" t="s">
         <v>1244</v>
@@ -39527,7 +38383,7 @@
         <v>1149</v>
       </c>
       <c r="D288" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="0"/>
         <v>2682</v>
       </c>
       <c r="E288" s="1" t="s">
@@ -39541,10 +38397,6 @@
       </c>
       <c r="J288" t="s">
         <v>1116</v>
-      </c>
-      <c r="K288" t="str">
-        <f t="shared" si="4"/>
-        <v>uE917-brand-mtm.svg</v>
       </c>
       <c r="L288" t="s">
         <v>1244</v>
@@ -39555,7 +38407,7 @@
         <v>1150</v>
       </c>
       <c r="D289" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="0"/>
         <v>2683</v>
       </c>
       <c r="E289" s="1" t="s">
@@ -39569,10 +38421,6 @@
       </c>
       <c r="J289" t="s">
         <v>1117</v>
-      </c>
-      <c r="K289" t="str">
-        <f t="shared" si="4"/>
-        <v>uE9B8-print.svg</v>
       </c>
       <c r="L289" t="s">
         <v>1244</v>
@@ -39583,7 +38431,7 @@
         <v>1151</v>
       </c>
       <c r="D290" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="0"/>
         <v>2684</v>
       </c>
       <c r="E290" s="1" t="s">
@@ -39597,10 +38445,6 @@
       </c>
       <c r="J290" t="s">
         <v>1118</v>
-      </c>
-      <c r="K290" t="str">
-        <f t="shared" si="4"/>
-        <v>uE908-arrow-open.svg</v>
       </c>
       <c r="L290" t="s">
         <v>1244</v>
@@ -39611,7 +38455,7 @@
         <v>1152</v>
       </c>
       <c r="D291" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="0"/>
         <v>2685</v>
       </c>
       <c r="E291" s="1" t="s">
@@ -39625,10 +38469,6 @@
       </c>
       <c r="J291" t="s">
         <v>1119</v>
-      </c>
-      <c r="K291" t="str">
-        <f t="shared" si="4"/>
-        <v>uE9C5-save-all.svg</v>
       </c>
       <c r="L291" t="s">
         <v>1244</v>
@@ -39639,7 +38479,7 @@
         <v>1153</v>
       </c>
       <c r="D292" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="0"/>
         <v>2686</v>
       </c>
       <c r="E292" s="1" t="s">
@@ -39653,10 +38493,6 @@
       </c>
       <c r="J292" t="s">
         <v>1120</v>
-      </c>
-      <c r="K292" t="str">
-        <f t="shared" si="4"/>
-        <v>uE9F3-step-shared.svg</v>
       </c>
       <c r="L292" t="s">
         <v>1244</v>
@@ -39667,7 +38503,7 @@
         <v>1154</v>
       </c>
       <c r="D293" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="0"/>
         <v>2687</v>
       </c>
       <c r="E293" s="1" t="s">
@@ -39681,10 +38517,6 @@
       </c>
       <c r="J293" t="s">
         <v>1121</v>
-      </c>
-      <c r="K293" t="str">
-        <f t="shared" si="4"/>
-        <v>uE981-group-rows.svg</v>
       </c>
       <c r="L293" t="s">
         <v>1244</v>
@@ -39695,7 +38527,7 @@
         <v>1155</v>
       </c>
       <c r="D294" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="0"/>
         <v>2688</v>
       </c>
       <c r="E294" s="1" t="s">
@@ -39709,10 +38541,6 @@
       </c>
       <c r="J294" t="s">
         <v>1122</v>
-      </c>
-      <c r="K294" t="str">
-        <f t="shared" si="4"/>
-        <v>uE906-arrow-export.svg</v>
       </c>
       <c r="L294" t="s">
         <v>1244</v>
@@ -39723,7 +38551,7 @@
         <v>1156</v>
       </c>
       <c r="D295" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="0"/>
         <v>2689</v>
       </c>
       <c r="E295" s="1" t="s">
@@ -39737,10 +38565,6 @@
       </c>
       <c r="J295" t="s">
         <v>1123</v>
-      </c>
-      <c r="K295" t="str">
-        <f t="shared" si="4"/>
-        <v>uEA11-toggle-tree-expanded-outline.svg</v>
       </c>
       <c r="L295" t="s">
         <v>1244</v>
@@ -39751,7 +38575,7 @@
         <v>1157</v>
       </c>
       <c r="D296" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="0"/>
         <v>2690</v>
       </c>
       <c r="E296" s="1" t="s">
@@ -39765,10 +38589,6 @@
       </c>
       <c r="J296" t="s">
         <v>1124</v>
-      </c>
-      <c r="K296" t="str">
-        <f t="shared" si="4"/>
-        <v>uEA20-video.svg</v>
       </c>
       <c r="L296" t="s">
         <v>1244</v>
@@ -39793,10 +38613,6 @@
       <c r="J297" t="s">
         <v>1158</v>
       </c>
-      <c r="K297" t="str">
-        <f t="shared" si="4"/>
-        <v>uE96A-file-bug.svg</v>
-      </c>
       <c r="L297" t="s">
         <v>1243</v>
       </c>
@@ -39820,10 +38636,6 @@
       <c r="J298" t="s">
         <v>1159</v>
       </c>
-      <c r="K298" t="str">
-        <f t="shared" si="4"/>
-        <v>uE93A-chevron-up-all.svg</v>
-      </c>
       <c r="L298" t="s">
         <v>1243</v>
       </c>
@@ -39847,10 +38659,6 @@
       <c r="J299" t="s">
         <v>1160</v>
       </c>
-      <c r="K299" t="str">
-        <f t="shared" si="4"/>
-        <v>uE931-chevron-down-all.svg</v>
-      </c>
       <c r="L299" t="s">
         <v>1243</v>
       </c>
@@ -39874,10 +38682,6 @@
       <c r="J300" t="s">
         <v>1161</v>
       </c>
-      <c r="K300" t="str">
-        <f t="shared" si="4"/>
-        <v>uE934-chevron-left-all.svg</v>
-      </c>
       <c r="L300" t="s">
         <v>1243</v>
       </c>
@@ -39900,10 +38704,6 @@
       </c>
       <c r="J301" t="s">
         <v>1162</v>
-      </c>
-      <c r="K301" t="str">
-        <f t="shared" si="4"/>
-        <v>uE937-chevron-right-all.svg</v>
       </c>
       <c r="L301" t="s">
         <v>1243</v>

</xml_diff>

<commit_message>
added some icons for VSCOM
</commit_message>
<xml_diff>
--- a/assets/icons/bowtie.xlsx
+++ b/assets/icons/bowtie.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Bowtie v1.0" sheetId="1" r:id="rId1"/>
     <sheet name="Bowtie v1.0 reorg" sheetId="2" r:id="rId2"/>
+    <sheet name="rename utility" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2642" uniqueCount="1254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3619" uniqueCount="1558">
   <si>
     <t>uE709-edit-outline.svg</t>
   </si>
@@ -3782,6 +3783,918 @@
   </si>
   <si>
     <t>uEAA0-chevron-right-end.svg</t>
+  </si>
+  <si>
+    <t>build-queue-new.svg</t>
+  </si>
+  <si>
+    <t>uE9A0-media-play.svg</t>
+  </si>
+  <si>
+    <t>uE9A1-menu.svg</t>
+  </si>
+  <si>
+    <t>uE9A2-merge-duplicate.svg</t>
+  </si>
+  <si>
+    <t>uE9A3-navigate-back-circle.svg</t>
+  </si>
+  <si>
+    <t>uE9A4-navigate-back-disc.svg</t>
+  </si>
+  <si>
+    <t>uE9A5-navigate-close.svg</t>
+  </si>
+  <si>
+    <t>uE9A6-navigate-external.svg</t>
+  </si>
+  <si>
+    <t>uE9A7-navigate-forward-circle.svg</t>
+  </si>
+  <si>
+    <t>uE9A8-navigate-forward-disc.svg</t>
+  </si>
+  <si>
+    <t>uE9A9-navigate-history.svg</t>
+  </si>
+  <si>
+    <t>uE9AA-navigate-refresh.svg</t>
+  </si>
+  <si>
+    <t>uE9AB-navigate-reload.svg</t>
+  </si>
+  <si>
+    <t>uE9AC-network-tower.svg</t>
+  </si>
+  <si>
+    <t>uE9AD-package-fill.svg</t>
+  </si>
+  <si>
+    <t>uE9AE-package.svg</t>
+  </si>
+  <si>
+    <t>uE9AF-pin-fill.svg</t>
+  </si>
+  <si>
+    <t>uE9B0-pin-pinned-fill.svg</t>
+  </si>
+  <si>
+    <t>uE9B1-pin-pinned.svg</t>
+  </si>
+  <si>
+    <t>uE9B2-pin-unpin-fill.svg</t>
+  </si>
+  <si>
+    <t>uE9B3-pin-unpin.svg</t>
+  </si>
+  <si>
+    <t>uE9B4-pin.svg</t>
+  </si>
+  <si>
+    <t>uE9B5-plug-outline.svg</t>
+  </si>
+  <si>
+    <t>uE9B6-plug.svg</t>
+  </si>
+  <si>
+    <t>uE9B7-policy.svg</t>
+  </si>
+  <si>
+    <t>uE9B8-print.svg</t>
+  </si>
+  <si>
+    <t>uE9B9-radio-button-empty.svg</t>
+  </si>
+  <si>
+    <t>uE9BA-radio-button.svg</t>
+  </si>
+  <si>
+    <t>uE9BB-recycle-bin-restore.svg</t>
+  </si>
+  <si>
+    <t>uE9BC-recycle-bin.svg</t>
+  </si>
+  <si>
+    <t>uE9BD-recycle.svg</t>
+  </si>
+  <si>
+    <t>uE9BE-redeploy.svg</t>
+  </si>
+  <si>
+    <t>uE9BF-repo-fill.svg</t>
+  </si>
+  <si>
+    <t>uE9C0-repo-git.svg</t>
+  </si>
+  <si>
+    <t>uE9C1-repo-submodule.svg</t>
+  </si>
+  <si>
+    <t>uE9C2-repo-tfvc.svg</t>
+  </si>
+  <si>
+    <t>uE9C3-repo.svg</t>
+  </si>
+  <si>
+    <t>uE9C4-robot.svg</t>
+  </si>
+  <si>
+    <t>uE9C5-save-all.svg</t>
+  </si>
+  <si>
+    <t>uE9C6-save.svg</t>
+  </si>
+  <si>
+    <t>uE9C7-search-filter-fill.svg</t>
+  </si>
+  <si>
+    <t>uE9C8-search-filter.svg</t>
+  </si>
+  <si>
+    <t>uE9C9-search.svg</t>
+  </si>
+  <si>
+    <t>uE9CA-security-access.svg</t>
+  </si>
+  <si>
+    <t>uE9CB-security-lock-fill.svg</t>
+  </si>
+  <si>
+    <t>uE9CC-security-lock.svg</t>
+  </si>
+  <si>
+    <t>uE9CD-security-unlock-fill.svg</t>
+  </si>
+  <si>
+    <t>uE9CE-security-unlock.svg</t>
+  </si>
+  <si>
+    <t>uE9CF-security.svg</t>
+  </si>
+  <si>
+    <t>uE9D0-separator.svg</t>
+  </si>
+  <si>
+    <t>uE9D1-server.svg</t>
+  </si>
+  <si>
+    <t>uE9D2-settings-gear.svg</t>
+  </si>
+  <si>
+    <t>uE9D3-settings-wrench.svg</t>
+  </si>
+  <si>
+    <t>uE9D4-share.svg</t>
+  </si>
+  <si>
+    <t>uE9D5-shop-server.svg</t>
+  </si>
+  <si>
+    <t>uE9D6-shop.svg</t>
+  </si>
+  <si>
+    <t>uE9D7-sort-ascending.svg</t>
+  </si>
+  <si>
+    <t>uE9D8-sort-descending.svg</t>
+  </si>
+  <si>
+    <t>uE9D9-sort.svg</t>
+  </si>
+  <si>
+    <t>uE9DA-square.svg</t>
+  </si>
+  <si>
+    <t>uE9DB-star-half.svg</t>
+  </si>
+  <si>
+    <t>uE9DC-status-error-outline.svg</t>
+  </si>
+  <si>
+    <t>uE9DD-status-error.svg</t>
+  </si>
+  <si>
+    <t>uE9DE-status-failure-outline.svg</t>
+  </si>
+  <si>
+    <t>uE9DF-status-failure.svg</t>
+  </si>
+  <si>
+    <t>uE9E0-status-help-outline.svg</t>
+  </si>
+  <si>
+    <t>uE9E1-status-help.svg</t>
+  </si>
+  <si>
+    <t>uE9E2-status-info-outline.svg</t>
+  </si>
+  <si>
+    <t>uE9E3-status-info.svg</t>
+  </si>
+  <si>
+    <t>uE9E4-status-no-fill.svg</t>
+  </si>
+  <si>
+    <t>uE9E5-status-no.svg</t>
+  </si>
+  <si>
+    <t>uE9E6-status-pause-outline.svg</t>
+  </si>
+  <si>
+    <t>uE9E7-status-pause.svg</t>
+  </si>
+  <si>
+    <t>uE9E8-status-run-outline.svg</t>
+  </si>
+  <si>
+    <t>uE9E9-status-run.svg</t>
+  </si>
+  <si>
+    <t>uE9EA-status-stop-outline.svg</t>
+  </si>
+  <si>
+    <t>uE9EB-status-stop.svg</t>
+  </si>
+  <si>
+    <t>uE9EC-status-success-box.svg</t>
+  </si>
+  <si>
+    <t>uE9ED-status-success-outline.svg</t>
+  </si>
+  <si>
+    <t>uE9EE-status-success.svg</t>
+  </si>
+  <si>
+    <t>uE9EF-status-waiting-fill.svg</t>
+  </si>
+  <si>
+    <t>uE9F0-status-waiting.svg</t>
+  </si>
+  <si>
+    <t>uE9F1-status-warning-outline.svg</t>
+  </si>
+  <si>
+    <t>uE9F2-status-warning.svg</t>
+  </si>
+  <si>
+    <t>uE9F3-step-shared.svg</t>
+  </si>
+  <si>
+    <t>uE9F4-step.svg</t>
+  </si>
+  <si>
+    <t>uE9F5-storyboard.svg</t>
+  </si>
+  <si>
+    <t>uE9F6-switch.svg</t>
+  </si>
+  <si>
+    <t>uE9F7-synchronize.svg</t>
+  </si>
+  <si>
+    <t>uE9F8-tag-fill.svg</t>
+  </si>
+  <si>
+    <t>uE9F9-tag.svg</t>
+  </si>
+  <si>
+    <t>uE9FA-test-auto-fill.svg</t>
+  </si>
+  <si>
+    <t>uE9FB-test-auto.svg</t>
+  </si>
+  <si>
+    <t>uE9FC-test-explore-fill.svg</t>
+  </si>
+  <si>
+    <t>uE9FD-test-fill.svg</t>
+  </si>
+  <si>
+    <t>uE9FE-test-user-fill.svg</t>
+  </si>
+  <si>
+    <t>uE9FF-test-user.svg</t>
+  </si>
+  <si>
+    <t>uE90A-arrow-up-left.svg</t>
+  </si>
+  <si>
+    <t>uE90B-arrow-up-right.svg</t>
+  </si>
+  <si>
+    <t>uE90C-arrow-up.svg</t>
+  </si>
+  <si>
+    <t>uE90D-attach.svg</t>
+  </si>
+  <si>
+    <t>uE90E-auto-fill-template.svg</t>
+  </si>
+  <si>
+    <t>uE90F-azure-api-management.svg</t>
+  </si>
+  <si>
+    <t>uE91A-brand-tfvc.svg</t>
+  </si>
+  <si>
+    <t>uE91B-brand-twitter.svg</t>
+  </si>
+  <si>
+    <t>uE91C-brand-visualstudio.svg</t>
+  </si>
+  <si>
+    <t>uE91D-brand-windows.svg</t>
+  </si>
+  <si>
+    <t>uE91E-build-queue-new.svg</t>
+  </si>
+  <si>
+    <t>uE91F-build-queue.svg</t>
+  </si>
+  <si>
+    <t>uE92A-chart-stacked-area.svg</t>
+  </si>
+  <si>
+    <t>uE92B-chart-stacked-bar.svg</t>
+  </si>
+  <si>
+    <t>uE92C-chart-stacked-line.svg</t>
+  </si>
+  <si>
+    <t>uE92D-check-light.svg</t>
+  </si>
+  <si>
+    <t>uE92E-check.svg</t>
+  </si>
+  <si>
+    <t>uE92F-checkbox-empty.svg</t>
+  </si>
+  <si>
+    <t>uE93A-chevron-up-all.svg</t>
+  </si>
+  <si>
+    <t>uE93B-chevron-up-light.svg</t>
+  </si>
+  <si>
+    <t>uE93C-chevron-up.svg</t>
+  </si>
+  <si>
+    <t>uE93D-clone-to-desktop.svg</t>
+  </si>
+  <si>
+    <t>uE93E-clone.svg</t>
+  </si>
+  <si>
+    <t>uE93F-cloud-fill.svg</t>
+  </si>
+  <si>
+    <t>uE94A-copy-to-clipboard.svg</t>
+  </si>
+  <si>
+    <t>uE94B-dashboard-fill.svg</t>
+  </si>
+  <si>
+    <t>uE94C-dashboard.svg</t>
+  </si>
+  <si>
+    <t>uE94D-database.svg</t>
+  </si>
+  <si>
+    <t>uE94E-deploy.svg</t>
+  </si>
+  <si>
+    <t>uE94F-details-pane.svg</t>
+  </si>
+  <si>
+    <t>uE95A-edit-outline.svg</t>
+  </si>
+  <si>
+    <t>uE95B-edit-paste.svg</t>
+  </si>
+  <si>
+    <t>uE95C-edit-redo.svg</t>
+  </si>
+  <si>
+    <t>uE95D-edit-remove.svg</t>
+  </si>
+  <si>
+    <t>uE95E-edit-rename.svg</t>
+  </si>
+  <si>
+    <t>uE95F-edit-undo.svg</t>
+  </si>
+  <si>
+    <t>uE96A-file-bug.svg</t>
+  </si>
+  <si>
+    <t>uE96B-file-code.svg</t>
+  </si>
+  <si>
+    <t>uE96C-file-comment.svg</t>
+  </si>
+  <si>
+    <t>uE96D-file-content.svg</t>
+  </si>
+  <si>
+    <t>uE96E-file-image.svg</t>
+  </si>
+  <si>
+    <t>uE96F-file-preview.svg</t>
+  </si>
+  <si>
+    <t>uE97A-format-indent-decrease.svg</t>
+  </si>
+  <si>
+    <t>uE97B-format-indent-increase.svg</t>
+  </si>
+  <si>
+    <t>uE97C-format-italic.svg</t>
+  </si>
+  <si>
+    <t>uE97D-format-list-ordered.svg</t>
+  </si>
+  <si>
+    <t>uE97E-format-list-unordered.svg</t>
+  </si>
+  <si>
+    <t>uE97F-format-underline.svg</t>
+  </si>
+  <si>
+    <t>uE98A-logo-visual-studio.svg</t>
+  </si>
+  <si>
+    <t>uE98B-mail-message-fill.svg</t>
+  </si>
+  <si>
+    <t>uE98C-mail-message.svg</t>
+  </si>
+  <si>
+    <t>uE98D-math-minus-box-light.svg</t>
+  </si>
+  <si>
+    <t>uE98E-math-minus-box.svg</t>
+  </si>
+  <si>
+    <t>uE98F-math-minus-circle-outline.svg</t>
+  </si>
+  <si>
+    <t>uE99A-math-plus-circle-outline.svg</t>
+  </si>
+  <si>
+    <t>uE99B-math-plus-circle.svg</t>
+  </si>
+  <si>
+    <t>uE99C-math-plus-heavy.svg</t>
+  </si>
+  <si>
+    <t>uE99D-math-plus-light.svg</t>
+  </si>
+  <si>
+    <t>uE99E-math-plus.svg</t>
+  </si>
+  <si>
+    <t>uE99F-media-play-fill.svg</t>
+  </si>
+  <si>
+    <t>uE900-alert.svg</t>
+  </si>
+  <si>
+    <t>uE901-approve-disapprove.svg</t>
+  </si>
+  <si>
+    <t>uE902-approve.svg</t>
+  </si>
+  <si>
+    <t>uE903-arrow-down-left.svg</t>
+  </si>
+  <si>
+    <t>uE904-arrow-down-right.svg</t>
+  </si>
+  <si>
+    <t>uE905-arrow-down.svg</t>
+  </si>
+  <si>
+    <t>uE906-arrow-export.svg</t>
+  </si>
+  <si>
+    <t>uE907-arrow-left.svg</t>
+  </si>
+  <si>
+    <t>uE908-arrow-open.svg</t>
+  </si>
+  <si>
+    <t>uE909-arrow-right.svg</t>
+  </si>
+  <si>
+    <t>uE910-azure-service-endpoint.svg</t>
+  </si>
+  <si>
+    <t>uE911-blur.svg</t>
+  </si>
+  <si>
+    <t>uE912-brand-android.svg</t>
+  </si>
+  <si>
+    <t>uE913-brand-facebook.svg</t>
+  </si>
+  <si>
+    <t>uE914-brand-git.svg</t>
+  </si>
+  <si>
+    <t>uE915-brand-github.svg</t>
+  </si>
+  <si>
+    <t>uE916-brand-maven.svg</t>
+  </si>
+  <si>
+    <t>uE917-brand-mtm.svg</t>
+  </si>
+  <si>
+    <t>uE918-brand-npm.svg</t>
+  </si>
+  <si>
+    <t>uE919-brand-nuget.svg</t>
+  </si>
+  <si>
+    <t>uE920-build-reason-checkin-shelveset.svg</t>
+  </si>
+  <si>
+    <t>uE921-build.svg</t>
+  </si>
+  <si>
+    <t>uE922-calendar-month.svg</t>
+  </si>
+  <si>
+    <t>uE923-calendar.svg</t>
+  </si>
+  <si>
+    <t>uE924-camera.svg</t>
+  </si>
+  <si>
+    <t>uE925-chart-area.svg</t>
+  </si>
+  <si>
+    <t>uE926-chart-bar.svg</t>
+  </si>
+  <si>
+    <t>uE927-chart-column.svg</t>
+  </si>
+  <si>
+    <t>uE928-chart-pie.svg</t>
+  </si>
+  <si>
+    <t>uE929-chart-pivot.svg</t>
+  </si>
+  <si>
+    <t>uE930-checkbox.svg</t>
+  </si>
+  <si>
+    <t>uE931-chevron-down-all.svg</t>
+  </si>
+  <si>
+    <t>uE932-chevron-down-light.svg</t>
+  </si>
+  <si>
+    <t>uE933-chevron-down.svg</t>
+  </si>
+  <si>
+    <t>uE934-chevron-left-all.svg</t>
+  </si>
+  <si>
+    <t>uE935-chevron-left-light.svg</t>
+  </si>
+  <si>
+    <t>uE936-chevron-left.svg</t>
+  </si>
+  <si>
+    <t>uE937-chevron-right-all.svg</t>
+  </si>
+  <si>
+    <t>uE938-chevron-right-light.svg</t>
+  </si>
+  <si>
+    <t>uE939-chevron-right.svg</t>
+  </si>
+  <si>
+    <t>uE940-cloud.svg</t>
+  </si>
+  <si>
+    <t>uE941-comment-add.svg</t>
+  </si>
+  <si>
+    <t>uE942-comment-discussion.svg</t>
+  </si>
+  <si>
+    <t>uE943-comment-lines.svg</t>
+  </si>
+  <si>
+    <t>uE944-comment-next.svg</t>
+  </si>
+  <si>
+    <t>uE945-comment-outline.svg</t>
+  </si>
+  <si>
+    <t>uE946-comment-previous.svg</t>
+  </si>
+  <si>
+    <t>uE947-comment-urgent.svg</t>
+  </si>
+  <si>
+    <t>uE948-comment.svg</t>
+  </si>
+  <si>
+    <t>uE949-connect-to-feed.svg</t>
+  </si>
+  <si>
+    <t>uE950-devices.svg</t>
+  </si>
+  <si>
+    <t>uE951-diff-image-overlay.svg</t>
+  </si>
+  <si>
+    <t>uE952-diff-image-pixel.svg</t>
+  </si>
+  <si>
+    <t>uE953-diff-image.svg</t>
+  </si>
+  <si>
+    <t>uE954-diff-inline.svg</t>
+  </si>
+  <si>
+    <t>uE955-diff-side-by-side.svg</t>
+  </si>
+  <si>
+    <t>uE956-dot.svg</t>
+  </si>
+  <si>
+    <t>uE957-edit-copy.svg</t>
+  </si>
+  <si>
+    <t>uE958-edit-cut.svg</t>
+  </si>
+  <si>
+    <t>uE959-edit-delete.svg</t>
+  </si>
+  <si>
+    <t>uE960-edit.svg</t>
+  </si>
+  <si>
+    <t>uE961-editor-list-bullet.svg</t>
+  </si>
+  <si>
+    <t>uE962-ellipsis-vertical.svg</t>
+  </si>
+  <si>
+    <t>uE963-ellipsis.svg</t>
+  </si>
+  <si>
+    <t>uE964-environment.svg</t>
+  </si>
+  <si>
+    <t>uE965-favorite-outline.svg</t>
+  </si>
+  <si>
+    <t>uE966-favorite.svg</t>
+  </si>
+  <si>
+    <t>uE967-feed.svg</t>
+  </si>
+  <si>
+    <t>uE968-feedback-negative.svg</t>
+  </si>
+  <si>
+    <t>uE969-feedback-positive.svg</t>
+  </si>
+  <si>
+    <t>uE970-file-symlink.svg</t>
+  </si>
+  <si>
+    <t>uE971-file.svg</t>
+  </si>
+  <si>
+    <t>uE972-fold-less.svg</t>
+  </si>
+  <si>
+    <t>uE973-fold-more.svg</t>
+  </si>
+  <si>
+    <t>uE974-folder.svg</t>
+  </si>
+  <si>
+    <t>uE975-format-bold.svg</t>
+  </si>
+  <si>
+    <t>uE976-format-clear.svg</t>
+  </si>
+  <si>
+    <t>uE977-format-font-color.svg</t>
+  </si>
+  <si>
+    <t>uE978-format-font-size.svg</t>
+  </si>
+  <si>
+    <t>uE979-format-font.svg</t>
+  </si>
+  <si>
+    <t>uE980-git.svg</t>
+  </si>
+  <si>
+    <t>uE981-group-rows.svg</t>
+  </si>
+  <si>
+    <t>uE982-heart-fill.svg</t>
+  </si>
+  <si>
+    <t>uE983-heart.svg</t>
+  </si>
+  <si>
+    <t>uE984-heartbeat-fill.svg</t>
+  </si>
+  <si>
+    <t>uE985-heartbeat.svg</t>
+  </si>
+  <si>
+    <t>uE986-image.svg</t>
+  </si>
+  <si>
+    <t>uE987-install.svg</t>
+  </si>
+  <si>
+    <t>uE988-link.svg</t>
+  </si>
+  <si>
+    <t>uE989-log.svg</t>
+  </si>
+  <si>
+    <t>uE990-math-minus-circle.svg</t>
+  </si>
+  <si>
+    <t>uE991-math-minus-light.svg</t>
+  </si>
+  <si>
+    <t>uE992-math-minus.svg</t>
+  </si>
+  <si>
+    <t>uE993-math-multiply-box-light.svg</t>
+  </si>
+  <si>
+    <t>uE994-math-multiply-box-outline.svg</t>
+  </si>
+  <si>
+    <t>uE995-math-multiply-box.svg</t>
+  </si>
+  <si>
+    <t>uE996-math-multiply-light.svg</t>
+  </si>
+  <si>
+    <t>uE997-math-multiply.svg</t>
+  </si>
+  <si>
+    <t>uE998-math-plus-box-light.svg</t>
+  </si>
+  <si>
+    <t>uE999-math-plus-box.svg</t>
+  </si>
+  <si>
+    <t>uEA00-test.svg</t>
+  </si>
+  <si>
+    <t>uEA0A-tfvc-repo.svg</t>
+  </si>
+  <si>
+    <t>uEA0B-tfvc-shelveset.svg</t>
+  </si>
+  <si>
+    <t>uEA0C-toggle-collapse-all.svg</t>
+  </si>
+  <si>
+    <t>uEA0D-toggle-collapse.svg</t>
+  </si>
+  <si>
+    <t>uEA0E-toggle-expand-all.svg</t>
+  </si>
+  <si>
+    <t>uEA0F-toggle-expand.svg</t>
+  </si>
+  <si>
+    <t>uEA01-tfvc-branch-locked.svg</t>
+  </si>
+  <si>
+    <t>uEA1A-trigger-auto.svg</t>
+  </si>
+  <si>
+    <t>uEA1B-trigger-user.svg</t>
+  </si>
+  <si>
+    <t>uEA1C-trigger.svg</t>
+  </si>
+  <si>
+    <t>uEA1D-user.svg</t>
+  </si>
+  <si>
+    <t>uEA1E-users.svg</t>
+  </si>
+  <si>
+    <t>uEA1F-variable.svg</t>
+  </si>
+  <si>
+    <t>uEA02-tfvc-branch.svg</t>
+  </si>
+  <si>
+    <t>uEA2A-work-item-move.svg</t>
+  </si>
+  <si>
+    <t>uEA2B-work-item.svg</t>
+  </si>
+  <si>
+    <t>uEA03-tfvc-change-list.svg</t>
+  </si>
+  <si>
+    <t>uEA04-tfvc-commit.svg</t>
+  </si>
+  <si>
+    <t>uEA05-tfvc-compare.svg</t>
+  </si>
+  <si>
+    <t>uEA06-tfvc-folder.svg</t>
+  </si>
+  <si>
+    <t>uEA07-tfvc-merge.svg</t>
+  </si>
+  <si>
+    <t>uEA08-tfvc-pull-request.svg</t>
+  </si>
+  <si>
+    <t>uEA09-tfvc-raw-source.svg</t>
+  </si>
+  <si>
+    <t>uEA10-toggle-tree-collapsed.svg</t>
+  </si>
+  <si>
+    <t>uEA11-toggle-tree-expanded-outline.svg</t>
+  </si>
+  <si>
+    <t>uEA12-toggle-tree-expanded.svg</t>
+  </si>
+  <si>
+    <t>uEA13-transfer-download.svg</t>
+  </si>
+  <si>
+    <t>uEA14-transfer-upload.svg</t>
+  </si>
+  <si>
+    <t>uEA15-trash.svg</t>
+  </si>
+  <si>
+    <t>uEA16-triangle-down.svg</t>
+  </si>
+  <si>
+    <t>uEA17-triangle-left.svg</t>
+  </si>
+  <si>
+    <t>uEA18-triangle-right.svg</t>
+  </si>
+  <si>
+    <t>uEA19-triangle-up.svg</t>
+  </si>
+  <si>
+    <t>uEA20-video.svg</t>
+  </si>
+  <si>
+    <t>uEA21-view-full-screen-exit.svg</t>
+  </si>
+  <si>
+    <t>uEA22-view-full-screen.svg</t>
+  </si>
+  <si>
+    <t>uEA23-view-grid.svg</t>
+  </si>
+  <si>
+    <t>uEA24-view-list-group.svg</t>
+  </si>
+  <si>
+    <t>uEA25-view-list-tree.svg</t>
+  </si>
+  <si>
+    <t>uEA26-view-list.svg</t>
+  </si>
+  <si>
+    <t>uEA27-watch-eye-fill.svg</t>
+  </si>
+  <si>
+    <t>uEA28-watch-eye.svg</t>
+  </si>
+  <si>
+    <t>uEA29-work-item-bar.svg</t>
+  </si>
+  <si>
+    <t>filename plain</t>
+  </si>
+  <si>
+    <t>filename prefix</t>
+  </si>
+  <si>
+    <t>git mv</t>
   </si>
 </sst>
 </file>
@@ -31720,9 +32633,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L326"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A293" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I299" sqref="I299"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A299" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F302" sqref="F302"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -39040,4 +39953,3610 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C326"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A307" workbookViewId="0">
+      <selection activeCell="E325" sqref="E325"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" customWidth="1"/>
+    <col min="3" max="3" width="35.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>1555</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1556</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B2" t="s">
+        <v>531</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1411</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B3" t="s">
+        <v>532</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1413</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B4" t="s">
+        <v>533</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1412</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B5" t="s">
+        <v>534</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1416</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B6" t="s">
+        <v>787</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1414</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B7" t="s">
+        <v>785</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1415</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1089</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1417</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B9" t="s">
+        <v>535</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1418</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1085</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1419</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B11" t="s">
+        <v>536</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1420</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B12" t="s">
+        <v>537</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1353</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B13" t="s">
+        <v>786</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1351</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B14" t="s">
+        <v>784</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1352</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B15" t="s">
+        <v>538</v>
+      </c>
+      <c r="C15" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B16" t="s">
+        <v>743</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1355</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B17" t="s">
+        <v>539</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1356</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B18" t="s">
+        <v>540</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1421</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1060</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1422</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B20" t="s">
+        <v>690</v>
+      </c>
+      <c r="C20" t="s">
+        <v>1423</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B21" t="s">
+        <v>691</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1424</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B22" t="s">
+        <v>692</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1425</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B23" t="s">
+        <v>693</v>
+      </c>
+      <c r="C23" t="s">
+        <v>1426</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B24" t="s">
+        <v>715</v>
+      </c>
+      <c r="C24" t="s">
+        <v>1427</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1083</v>
+      </c>
+      <c r="C25" t="s">
+        <v>1428</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B26" t="s">
+        <v>713</v>
+      </c>
+      <c r="C26" t="s">
+        <v>1429</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B27" t="s">
+        <v>694</v>
+      </c>
+      <c r="C27" t="s">
+        <v>1430</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B28" t="s">
+        <v>695</v>
+      </c>
+      <c r="C28" t="s">
+        <v>1357</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B29" t="s">
+        <v>696</v>
+      </c>
+      <c r="C29" t="s">
+        <v>1358</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B30" t="s">
+        <v>697</v>
+      </c>
+      <c r="C30" t="s">
+        <v>1359</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B31" t="s">
+        <v>698</v>
+      </c>
+      <c r="C31" t="s">
+        <v>1360</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B32" t="s">
+        <v>541</v>
+      </c>
+      <c r="C32" t="s">
+        <v>1432</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B33" t="s">
+        <v>542</v>
+      </c>
+      <c r="C33" t="s">
+        <v>1362</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B34" t="s">
+        <v>1254</v>
+      </c>
+      <c r="C34" t="s">
+        <v>1361</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B35" t="s">
+        <v>544</v>
+      </c>
+      <c r="C35" t="s">
+        <v>1431</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B36" t="s">
+        <v>545</v>
+      </c>
+      <c r="C36" t="s">
+        <v>1434</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B37" t="s">
+        <v>699</v>
+      </c>
+      <c r="C37" t="s">
+        <v>1433</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B38" t="s">
+        <v>1061</v>
+      </c>
+      <c r="C38" t="s">
+        <v>1435</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B39" t="s">
+        <v>755</v>
+      </c>
+      <c r="C39" t="s">
+        <v>1436</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B40" t="s">
+        <v>746</v>
+      </c>
+      <c r="C40" t="s">
+        <v>1437</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B41" t="s">
+        <v>747</v>
+      </c>
+      <c r="C41" t="s">
+        <v>1438</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B42" t="s">
+        <v>745</v>
+      </c>
+      <c r="C42" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B43" t="s">
+        <v>754</v>
+      </c>
+      <c r="C43" t="s">
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B44" t="s">
+        <v>759</v>
+      </c>
+      <c r="C44" t="s">
+        <v>1363</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B45" t="s">
+        <v>749</v>
+      </c>
+      <c r="C45" t="s">
+        <v>1364</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B46" t="s">
+        <v>756</v>
+      </c>
+      <c r="C46" t="s">
+        <v>1365</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B47" t="s">
+        <v>546</v>
+      </c>
+      <c r="C47" t="s">
+        <v>1367</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B48" t="s">
+        <v>702</v>
+      </c>
+      <c r="C48" t="s">
+        <v>1441</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B49" t="s">
+        <v>701</v>
+      </c>
+      <c r="C49" t="s">
+        <v>1368</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B50" t="s">
+        <v>700</v>
+      </c>
+      <c r="C50" t="s">
+        <v>1366</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B51" t="s">
+        <v>548</v>
+      </c>
+      <c r="C51" t="s">
+        <v>1444</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B52" t="s">
+        <v>1170</v>
+      </c>
+      <c r="C52" t="s">
+        <v>1442</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B53" t="s">
+        <v>1247</v>
+      </c>
+      <c r="C53" t="s">
+        <v>1251</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B54" t="s">
+        <v>547</v>
+      </c>
+      <c r="C54" t="s">
+        <v>1443</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B55" t="s">
+        <v>550</v>
+      </c>
+      <c r="C55" t="s">
+        <v>1447</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B56" t="s">
+        <v>1171</v>
+      </c>
+      <c r="C56" t="s">
+        <v>1445</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B57" t="s">
+        <v>1248</v>
+      </c>
+      <c r="C57" t="s">
+        <v>1252</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B58" t="s">
+        <v>549</v>
+      </c>
+      <c r="C58" t="s">
+        <v>1446</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B59" t="s">
+        <v>552</v>
+      </c>
+      <c r="C59" t="s">
+        <v>1450</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B60" t="s">
+        <v>1172</v>
+      </c>
+      <c r="C60" t="s">
+        <v>1448</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B61" t="s">
+        <v>1249</v>
+      </c>
+      <c r="C61" t="s">
+        <v>1253</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B62" t="s">
+        <v>551</v>
+      </c>
+      <c r="C62" t="s">
+        <v>1449</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B63" t="s">
+        <v>554</v>
+      </c>
+      <c r="C63" t="s">
+        <v>1371</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B64" t="s">
+        <v>1169</v>
+      </c>
+      <c r="C64" t="s">
+        <v>1369</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B65" t="s">
+        <v>1246</v>
+      </c>
+      <c r="C65" t="s">
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B66" t="s">
+        <v>553</v>
+      </c>
+      <c r="C66" t="s">
+        <v>1370</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B67" t="s">
+        <v>556</v>
+      </c>
+      <c r="C67" t="s">
+        <v>1373</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B68" t="s">
+        <v>555</v>
+      </c>
+      <c r="C68" t="s">
+        <v>1372</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B69" t="s">
+        <v>557</v>
+      </c>
+      <c r="C69" t="s">
+        <v>1451</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B70" t="s">
+        <v>703</v>
+      </c>
+      <c r="C70" t="s">
+        <v>1374</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B71" t="s">
+        <v>558</v>
+      </c>
+      <c r="C71" t="s">
+        <v>1459</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B72" t="s">
+        <v>559</v>
+      </c>
+      <c r="C72" t="s">
+        <v>1452</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B73" t="s">
+        <v>560</v>
+      </c>
+      <c r="C73" t="s">
+        <v>1453</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B74" t="s">
+        <v>561</v>
+      </c>
+      <c r="C74" t="s">
+        <v>1454</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B75" t="s">
+        <v>562</v>
+      </c>
+      <c r="C75" t="s">
+        <v>1455</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B76" t="s">
+        <v>563</v>
+      </c>
+      <c r="C76" t="s">
+        <v>1456</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B77" t="s">
+        <v>564</v>
+      </c>
+      <c r="C77" t="s">
+        <v>1457</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B78" t="s">
+        <v>565</v>
+      </c>
+      <c r="C78" t="s">
+        <v>1458</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B79" t="s">
+        <v>704</v>
+      </c>
+      <c r="C79" t="s">
+        <v>1460</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B80" t="s">
+        <v>705</v>
+      </c>
+      <c r="C80" t="s">
+        <v>1375</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B81" t="s">
+        <v>566</v>
+      </c>
+      <c r="C81" t="s">
+        <v>1377</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B82" t="s">
+        <v>706</v>
+      </c>
+      <c r="C82" t="s">
+        <v>1376</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B83" t="s">
+        <v>567</v>
+      </c>
+      <c r="C83" t="s">
+        <v>1378</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B84" t="s">
+        <v>1071</v>
+      </c>
+      <c r="C84" t="s">
+        <v>1379</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B85" t="s">
+        <v>720</v>
+      </c>
+      <c r="C85" t="s">
+        <v>1380</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B86" t="s">
+        <v>1068</v>
+      </c>
+      <c r="C86" t="s">
+        <v>1461</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B87" t="s">
+        <v>570</v>
+      </c>
+      <c r="C87" t="s">
+        <v>1464</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B88" t="s">
+        <v>568</v>
+      </c>
+      <c r="C88" t="s">
+        <v>1462</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B89" t="s">
+        <v>569</v>
+      </c>
+      <c r="C89" t="s">
+        <v>1463</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B90" t="s">
+        <v>571</v>
+      </c>
+      <c r="C90" t="s">
+        <v>1465</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B91" t="s">
+        <v>572</v>
+      </c>
+      <c r="C91" t="s">
+        <v>1466</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B92" t="s">
+        <v>573</v>
+      </c>
+      <c r="C92" t="s">
+        <v>1467</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B93" t="s">
+        <v>574</v>
+      </c>
+      <c r="C93" t="s">
+        <v>1471</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B94" t="s">
+        <v>575</v>
+      </c>
+      <c r="C94" t="s">
+        <v>1468</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B95" t="s">
+        <v>576</v>
+      </c>
+      <c r="C95" t="s">
+        <v>1469</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B96" t="s">
+        <v>783</v>
+      </c>
+      <c r="C96" t="s">
+        <v>1470</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B97" t="s">
+        <v>583</v>
+      </c>
+      <c r="C97" t="s">
+        <v>1472</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B98" t="s">
+        <v>791</v>
+      </c>
+      <c r="C98" t="s">
+        <v>1381</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B99" t="s">
+        <v>578</v>
+      </c>
+      <c r="C99" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B100" t="s">
+        <v>579</v>
+      </c>
+      <c r="C100" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B101" t="s">
+        <v>580</v>
+      </c>
+      <c r="C101" t="s">
+        <v>1384</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B102" t="s">
+        <v>581</v>
+      </c>
+      <c r="C102" t="s">
+        <v>1385</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B103" t="s">
+        <v>582</v>
+      </c>
+      <c r="C103" t="s">
+        <v>1386</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B104" t="s">
+        <v>585</v>
+      </c>
+      <c r="C104" t="s">
+        <v>1474</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B105" t="s">
+        <v>584</v>
+      </c>
+      <c r="C105" t="s">
+        <v>1473</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B106" t="s">
+        <v>1077</v>
+      </c>
+      <c r="C106" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B107" t="s">
+        <v>1228</v>
+      </c>
+      <c r="C107" t="s">
+        <v>1207</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B108" t="s">
+        <v>1221</v>
+      </c>
+      <c r="C108" t="s">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B109" t="s">
+        <v>1227</v>
+      </c>
+      <c r="C109" t="s">
+        <v>1206</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B110" t="s">
+        <v>1220</v>
+      </c>
+      <c r="C110" t="s">
+        <v>1199</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B111" t="s">
+        <v>587</v>
+      </c>
+      <c r="C111" t="s">
+        <v>1477</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B112" t="s">
+        <v>586</v>
+      </c>
+      <c r="C112" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B113" t="s">
+        <v>712</v>
+      </c>
+      <c r="C113" t="s">
+        <v>1478</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B114" t="s">
+        <v>588</v>
+      </c>
+      <c r="C114" t="s">
+        <v>1479</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B115" t="s">
+        <v>589</v>
+      </c>
+      <c r="C115" t="s">
+        <v>1480</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B116" t="s">
+        <v>590</v>
+      </c>
+      <c r="C116" t="s">
+        <v>1482</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B117" t="s">
+        <v>1168</v>
+      </c>
+      <c r="C117" t="s">
+        <v>1387</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B118" t="s">
+        <v>591</v>
+      </c>
+      <c r="C118" t="s">
+        <v>1388</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B119" t="s">
+        <v>592</v>
+      </c>
+      <c r="C119" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B120" t="s">
+        <v>593</v>
+      </c>
+      <c r="C120" t="s">
+        <v>1390</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B121" t="s">
+        <v>594</v>
+      </c>
+      <c r="C121" t="s">
+        <v>1391</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B122" t="s">
+        <v>595</v>
+      </c>
+      <c r="C122" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B123" t="s">
+        <v>596</v>
+      </c>
+      <c r="C123" t="s">
+        <v>1481</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B124" t="s">
+        <v>599</v>
+      </c>
+      <c r="C124" t="s">
+        <v>1485</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B125" t="s">
+        <v>597</v>
+      </c>
+      <c r="C125" t="s">
+        <v>1483</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B126" t="s">
+        <v>598</v>
+      </c>
+      <c r="C126" t="s">
+        <v>1484</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B127" t="s">
+        <v>752</v>
+      </c>
+      <c r="C127" t="s">
+        <v>1486</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B128" t="s">
+        <v>766</v>
+      </c>
+      <c r="C128" t="s">
+        <v>1487</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B129" t="s">
+        <v>1069</v>
+      </c>
+      <c r="C129" t="s">
+        <v>1490</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B130" t="s">
+        <v>772</v>
+      </c>
+      <c r="C130" t="s">
+        <v>1488</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B131" t="s">
+        <v>773</v>
+      </c>
+      <c r="C131" t="s">
+        <v>1489</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B132" t="s">
+        <v>774</v>
+      </c>
+      <c r="C132" t="s">
+        <v>1393</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B133" t="s">
+        <v>775</v>
+      </c>
+      <c r="C133" t="s">
+        <v>1394</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B134" t="s">
+        <v>776</v>
+      </c>
+      <c r="C134" t="s">
+        <v>1395</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B135" t="s">
+        <v>777</v>
+      </c>
+      <c r="C135" t="s">
+        <v>1396</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B136" t="s">
+        <v>778</v>
+      </c>
+      <c r="C136" t="s">
+        <v>1397</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B137" t="s">
+        <v>779</v>
+      </c>
+      <c r="C137" t="s">
+        <v>1398</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B138" t="s">
+        <v>600</v>
+      </c>
+      <c r="C138" t="s">
+        <v>1491</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B139" t="s">
+        <v>1088</v>
+      </c>
+      <c r="C139" t="s">
+        <v>1492</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B140" t="s">
+        <v>718</v>
+      </c>
+      <c r="C140" t="s">
+        <v>1494</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B141" t="s">
+        <v>601</v>
+      </c>
+      <c r="C141" t="s">
+        <v>1496</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B142" t="s">
+        <v>719</v>
+      </c>
+      <c r="C142" t="s">
+        <v>1495</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B143" t="s">
+        <v>717</v>
+      </c>
+      <c r="C143" t="s">
+        <v>1493</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B144" t="s">
+        <v>721</v>
+      </c>
+      <c r="C144" t="s">
+        <v>1497</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B145" t="s">
+        <v>602</v>
+      </c>
+      <c r="C145" t="s">
+        <v>1498</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B146" t="s">
+        <v>603</v>
+      </c>
+      <c r="C146" t="s">
+        <v>1499</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B147" t="s">
+        <v>1075</v>
+      </c>
+      <c r="C147" t="s">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B148" t="s">
+        <v>604</v>
+      </c>
+      <c r="C148" t="s">
+        <v>1399</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B149" t="s">
+        <v>605</v>
+      </c>
+      <c r="C149" t="s">
+        <v>1401</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B150" t="s">
+        <v>722</v>
+      </c>
+      <c r="C150" t="s">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B151" t="s">
+        <v>606</v>
+      </c>
+      <c r="C151" t="s">
+        <v>1503</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B152" t="s">
+        <v>607</v>
+      </c>
+      <c r="C152" t="s">
+        <v>1403</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B153" t="s">
+        <v>780</v>
+      </c>
+      <c r="C153" t="s">
+        <v>1402</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B154" t="s">
+        <v>608</v>
+      </c>
+      <c r="C154" t="s">
+        <v>1501</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B155" t="s">
+        <v>723</v>
+      </c>
+      <c r="C155" t="s">
+        <v>1404</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B156" t="s">
+        <v>724</v>
+      </c>
+      <c r="C156" t="s">
+        <v>1502</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B157" t="s">
+        <v>609</v>
+      </c>
+      <c r="C157" t="s">
+        <v>1508</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B158" t="s">
+        <v>726</v>
+      </c>
+      <c r="C158" t="s">
+        <v>1506</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B159" t="s">
+        <v>781</v>
+      </c>
+      <c r="C159" t="s">
+        <v>1504</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B160" t="s">
+        <v>725</v>
+      </c>
+      <c r="C160" t="s">
+        <v>1505</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B161" t="s">
+        <v>727</v>
+      </c>
+      <c r="C161" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B162" t="s">
+        <v>613</v>
+      </c>
+      <c r="C162" t="s">
+        <v>1409</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B163" t="s">
+        <v>610</v>
+      </c>
+      <c r="C163" t="s">
+        <v>1510</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B164" t="s">
+        <v>782</v>
+      </c>
+      <c r="C164" t="s">
+        <v>1509</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B165" t="s">
+        <v>611</v>
+      </c>
+      <c r="C165" t="s">
+        <v>1406</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B166" t="s">
+        <v>728</v>
+      </c>
+      <c r="C166" t="s">
+        <v>1405</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B167" t="s">
+        <v>612</v>
+      </c>
+      <c r="C167" t="s">
+        <v>1407</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B168" t="s">
+        <v>729</v>
+      </c>
+      <c r="C168" t="s">
+        <v>1408</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B169" t="s">
+        <v>614</v>
+      </c>
+      <c r="C169" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B170" t="s">
+        <v>730</v>
+      </c>
+      <c r="C170" t="s">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B171" t="s">
+        <v>615</v>
+      </c>
+      <c r="C171" t="s">
+        <v>1256</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B172" t="s">
+        <v>1070</v>
+      </c>
+      <c r="C172" t="s">
+        <v>1257</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B173" t="s">
+        <v>616</v>
+      </c>
+      <c r="C173" t="s">
+        <v>1258</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B174" t="s">
+        <v>617</v>
+      </c>
+      <c r="C174" t="s">
+        <v>1259</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B175" t="s">
+        <v>618</v>
+      </c>
+      <c r="C175" t="s">
+        <v>1260</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B176" t="s">
+        <v>619</v>
+      </c>
+      <c r="C176" t="s">
+        <v>1261</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B177" t="s">
+        <v>620</v>
+      </c>
+      <c r="C177" t="s">
+        <v>1262</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B178" t="s">
+        <v>621</v>
+      </c>
+      <c r="C178" t="s">
+        <v>1263</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B179" t="s">
+        <v>622</v>
+      </c>
+      <c r="C179" t="s">
+        <v>1264</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B180" t="s">
+        <v>623</v>
+      </c>
+      <c r="C180" t="s">
+        <v>1265</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B181" t="s">
+        <v>624</v>
+      </c>
+      <c r="C181" t="s">
+        <v>1266</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B182" t="s">
+        <v>731</v>
+      </c>
+      <c r="C182" t="s">
+        <v>1267</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B183" t="s">
+        <v>1230</v>
+      </c>
+      <c r="C183" t="s">
+        <v>1209</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B184" t="s">
+        <v>1223</v>
+      </c>
+      <c r="C184" t="s">
+        <v>1202</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B185" t="s">
+        <v>625</v>
+      </c>
+      <c r="C185" t="s">
+        <v>1269</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B186" t="s">
+        <v>732</v>
+      </c>
+      <c r="C186" t="s">
+        <v>1268</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B187" t="s">
+        <v>1231</v>
+      </c>
+      <c r="C187" t="s">
+        <v>1210</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B188" t="s">
+        <v>1232</v>
+      </c>
+      <c r="C188" t="s">
+        <v>1211</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B189" t="s">
+        <v>626</v>
+      </c>
+      <c r="C189" t="s">
+        <v>1275</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B190" t="s">
+        <v>733</v>
+      </c>
+      <c r="C190" t="s">
+        <v>1270</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B191" t="s">
+        <v>735</v>
+      </c>
+      <c r="C191" t="s">
+        <v>1272</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B192" t="s">
+        <v>734</v>
+      </c>
+      <c r="C192" t="s">
+        <v>1271</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B193" t="s">
+        <v>737</v>
+      </c>
+      <c r="C193" t="s">
+        <v>1274</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B194" t="s">
+        <v>736</v>
+      </c>
+      <c r="C194" t="s">
+        <v>1273</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B195" t="s">
+        <v>1216</v>
+      </c>
+      <c r="C195" t="s">
+        <v>1195</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B196" t="s">
+        <v>1225</v>
+      </c>
+      <c r="C196" t="s">
+        <v>1204</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B197" t="s">
+        <v>1215</v>
+      </c>
+      <c r="C197" t="s">
+        <v>1194</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B198" t="s">
+        <v>1233</v>
+      </c>
+      <c r="C198" t="s">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B199" t="s">
+        <v>738</v>
+      </c>
+      <c r="C199" t="s">
+        <v>1277</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B200" t="s">
+        <v>790</v>
+      </c>
+      <c r="C200" t="s">
+        <v>1276</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B201" t="s">
+        <v>760</v>
+      </c>
+      <c r="C201" t="s">
+        <v>1278</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B202" t="s">
+        <v>1229</v>
+      </c>
+      <c r="C202" t="s">
+        <v>1208</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B203" t="s">
+        <v>1222</v>
+      </c>
+      <c r="C203" t="s">
+        <v>1201</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B204" t="s">
+        <v>1084</v>
+      </c>
+      <c r="C204" t="s">
+        <v>1279</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B205" t="s">
+        <v>740</v>
+      </c>
+      <c r="C205" t="s">
+        <v>1281</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B206" t="s">
+        <v>739</v>
+      </c>
+      <c r="C206" t="s">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B207" t="s">
+        <v>1226</v>
+      </c>
+      <c r="C207" t="s">
+        <v>1205</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B208" t="s">
+        <v>1219</v>
+      </c>
+      <c r="C208" t="s">
+        <v>1198</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B209" t="s">
+        <v>763</v>
+      </c>
+      <c r="C209" t="s">
+        <v>1284</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A210" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B210" t="s">
+        <v>741</v>
+      </c>
+      <c r="C210" t="s">
+        <v>1283</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B211" t="s">
+        <v>748</v>
+      </c>
+      <c r="C211" t="s">
+        <v>1282</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B212" t="s">
+        <v>1072</v>
+      </c>
+      <c r="C212" t="s">
+        <v>1285</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B213" t="s">
+        <v>764</v>
+      </c>
+      <c r="C213" t="s">
+        <v>1290</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A214" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B214" t="s">
+        <v>629</v>
+      </c>
+      <c r="C214" t="s">
+        <v>1286</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B215" t="s">
+        <v>627</v>
+      </c>
+      <c r="C215" t="s">
+        <v>1287</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A216" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B216" t="s">
+        <v>630</v>
+      </c>
+      <c r="C216" t="s">
+        <v>1288</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A217" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B217" t="s">
+        <v>628</v>
+      </c>
+      <c r="C217" t="s">
+        <v>1289</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A218" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B218" t="s">
+        <v>1235</v>
+      </c>
+      <c r="C218" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A219" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B219" t="s">
+        <v>1074</v>
+      </c>
+      <c r="C219" t="s">
+        <v>1291</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A220" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B220" t="s">
+        <v>631</v>
+      </c>
+      <c r="C220" t="s">
+        <v>1293</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A221" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B221" t="s">
+        <v>1086</v>
+      </c>
+      <c r="C221" t="s">
+        <v>1292</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A222" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B222" t="s">
+        <v>633</v>
+      </c>
+      <c r="C222" t="s">
+        <v>1296</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A223" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B223" t="s">
+        <v>632</v>
+      </c>
+      <c r="C223" t="s">
+        <v>1295</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A224" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B224" t="s">
+        <v>750</v>
+      </c>
+      <c r="C224" t="s">
+        <v>1294</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A225" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B225" t="s">
+        <v>634</v>
+      </c>
+      <c r="C225" t="s">
+        <v>1302</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A226" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B226" t="s">
+        <v>635</v>
+      </c>
+      <c r="C226" t="s">
+        <v>1297</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A227" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B227" t="s">
+        <v>636</v>
+      </c>
+      <c r="C227" t="s">
+        <v>1299</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A228" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B228" t="s">
+        <v>751</v>
+      </c>
+      <c r="C228" t="s">
+        <v>1298</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A229" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B229" t="s">
+        <v>637</v>
+      </c>
+      <c r="C229" t="s">
+        <v>1301</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A230" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B230" t="s">
+        <v>753</v>
+      </c>
+      <c r="C230" t="s">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A231" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B231" t="s">
+        <v>638</v>
+      </c>
+      <c r="C231" t="s">
+        <v>1303</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A232" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B232" t="s">
+        <v>1076</v>
+      </c>
+      <c r="C232" t="s">
+        <v>1304</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A233" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B233" t="s">
+        <v>639</v>
+      </c>
+      <c r="C233" t="s">
+        <v>1305</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A234" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B234" t="s">
+        <v>1224</v>
+      </c>
+      <c r="C234" t="s">
+        <v>1203</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A235" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B235" t="s">
+        <v>640</v>
+      </c>
+      <c r="C235" t="s">
+        <v>1306</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A236" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B236" t="s">
+        <v>641</v>
+      </c>
+      <c r="C236" t="s">
+        <v>1307</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A237" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B237" t="s">
+        <v>642</v>
+      </c>
+      <c r="C237" t="s">
+        <v>1309</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A238" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B238" t="s">
+        <v>770</v>
+      </c>
+      <c r="C238" t="s">
+        <v>1308</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A239" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B239" t="s">
+        <v>757</v>
+      </c>
+      <c r="C239" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A240" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B240" t="s">
+        <v>643</v>
+      </c>
+      <c r="C240" t="s">
+        <v>1310</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A241" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B241" t="s">
+        <v>644</v>
+      </c>
+      <c r="C241" t="s">
+        <v>1311</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A242" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B242" t="s">
+        <v>645</v>
+      </c>
+      <c r="C242" t="s">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A243" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B243" t="s">
+        <v>758</v>
+      </c>
+      <c r="C243" t="s">
+        <v>1314</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A244" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B244" t="s">
+        <v>646</v>
+      </c>
+      <c r="C244" t="s">
+        <v>1316</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A245" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B245" t="s">
+        <v>792</v>
+      </c>
+      <c r="C245" t="s">
+        <v>1315</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A246" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B246" t="s">
+        <v>647</v>
+      </c>
+      <c r="C246" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A247" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B247" t="s">
+        <v>688</v>
+      </c>
+      <c r="C247" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A248" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B248" t="s">
+        <v>648</v>
+      </c>
+      <c r="C248" t="s">
+        <v>1320</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A249" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B249" t="s">
+        <v>761</v>
+      </c>
+      <c r="C249" t="s">
+        <v>1319</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A250" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B250" t="s">
+        <v>650</v>
+      </c>
+      <c r="C250" t="s">
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A251" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B251" t="s">
+        <v>649</v>
+      </c>
+      <c r="C251" t="s">
+        <v>1321</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A252" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B252" t="s">
+        <v>707</v>
+      </c>
+      <c r="C252" t="s">
+        <v>1324</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A253" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B253" t="s">
+        <v>762</v>
+      </c>
+      <c r="C253" t="s">
+        <v>1323</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A254" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B254" t="s">
+        <v>709</v>
+      </c>
+      <c r="C254" t="s">
+        <v>1326</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A255" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B255" t="s">
+        <v>710</v>
+      </c>
+      <c r="C255" t="s">
+        <v>1325</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A256" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B256" t="s">
+        <v>788</v>
+      </c>
+      <c r="C256" t="s">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A257" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B257" t="s">
+        <v>789</v>
+      </c>
+      <c r="C257" t="s">
+        <v>1327</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A258" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B258" t="s">
+        <v>711</v>
+      </c>
+      <c r="C258" t="s">
+        <v>1330</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A259" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B259" t="s">
+        <v>714</v>
+      </c>
+      <c r="C259" t="s">
+        <v>1329</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A260" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B260" t="s">
+        <v>651</v>
+      </c>
+      <c r="C260" t="s">
+        <v>1333</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A261" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B261" t="s">
+        <v>769</v>
+      </c>
+      <c r="C261" t="s">
+        <v>1331</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A262" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B262" t="s">
+        <v>689</v>
+      </c>
+      <c r="C262" t="s">
+        <v>1332</v>
+      </c>
+    </row>
+    <row r="263" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A263" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B263" t="s">
+        <v>652</v>
+      </c>
+      <c r="C263" t="s">
+        <v>1335</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A264" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B264" t="s">
+        <v>716</v>
+      </c>
+      <c r="C264" t="s">
+        <v>1334</v>
+      </c>
+    </row>
+    <row r="265" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A265" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B265" t="s">
+        <v>653</v>
+      </c>
+      <c r="C265" t="s">
+        <v>1337</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A266" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B266" t="s">
+        <v>708</v>
+      </c>
+      <c r="C266" t="s">
+        <v>1336</v>
+      </c>
+    </row>
+    <row r="267" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A267" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B267" t="s">
+        <v>1073</v>
+      </c>
+      <c r="C267" t="s">
+        <v>1339</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A268" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B268" t="s">
+        <v>1087</v>
+      </c>
+      <c r="C268" t="s">
+        <v>1338</v>
+      </c>
+    </row>
+    <row r="269" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A269" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B269" t="s">
+        <v>1218</v>
+      </c>
+      <c r="C269" t="s">
+        <v>1197</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A270" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B270" t="s">
+        <v>1217</v>
+      </c>
+      <c r="C270" t="s">
+        <v>1196</v>
+      </c>
+    </row>
+    <row r="271" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A271" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B271" t="s">
+        <v>744</v>
+      </c>
+      <c r="C271" t="s">
+        <v>1340</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A272" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B272" t="s">
+        <v>654</v>
+      </c>
+      <c r="C272" t="s">
+        <v>1341</v>
+      </c>
+    </row>
+    <row r="273" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A273" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B273" t="s">
+        <v>767</v>
+      </c>
+      <c r="C273" t="s">
+        <v>1342</v>
+      </c>
+    </row>
+    <row r="274" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A274" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B274" t="s">
+        <v>655</v>
+      </c>
+      <c r="C274" t="s">
+        <v>1344</v>
+      </c>
+    </row>
+    <row r="275" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A275" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B275" t="s">
+        <v>768</v>
+      </c>
+      <c r="C275" t="s">
+        <v>1343</v>
+      </c>
+    </row>
+    <row r="276" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A276" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B276" t="s">
+        <v>1078</v>
+      </c>
+      <c r="C276" t="s">
+        <v>1511</v>
+      </c>
+    </row>
+    <row r="277" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A277" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B277" t="s">
+        <v>1079</v>
+      </c>
+      <c r="C277" t="s">
+        <v>1346</v>
+      </c>
+    </row>
+    <row r="278" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A278" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B278" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C278" t="s">
+        <v>1345</v>
+      </c>
+    </row>
+    <row r="279" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A279" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B279" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C279" t="s">
+        <v>1347</v>
+      </c>
+    </row>
+    <row r="280" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A280" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B280" t="s">
+        <v>1067</v>
+      </c>
+      <c r="C280" t="s">
+        <v>1348</v>
+      </c>
+    </row>
+    <row r="281" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A281" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B281" t="s">
+        <v>1062</v>
+      </c>
+      <c r="C281" t="s">
+        <v>1350</v>
+      </c>
+    </row>
+    <row r="282" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A282" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B282" t="s">
+        <v>1081</v>
+      </c>
+      <c r="C282" t="s">
+        <v>1349</v>
+      </c>
+    </row>
+    <row r="283" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A283" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B283" t="s">
+        <v>657</v>
+      </c>
+      <c r="C283" t="s">
+        <v>1525</v>
+      </c>
+    </row>
+    <row r="284" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A284" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B284" t="s">
+        <v>656</v>
+      </c>
+      <c r="C284" t="s">
+        <v>1518</v>
+      </c>
+    </row>
+    <row r="285" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A285" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B285" t="s">
+        <v>658</v>
+      </c>
+      <c r="C285" t="s">
+        <v>1528</v>
+      </c>
+    </row>
+    <row r="286" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A286" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B286" t="s">
+        <v>659</v>
+      </c>
+      <c r="C286" t="s">
+        <v>1529</v>
+      </c>
+    </row>
+    <row r="287" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A287" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B287" t="s">
+        <v>660</v>
+      </c>
+      <c r="C287" t="s">
+        <v>1530</v>
+      </c>
+    </row>
+    <row r="288" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A288" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B288" t="s">
+        <v>771</v>
+      </c>
+      <c r="C288" t="s">
+        <v>1531</v>
+      </c>
+    </row>
+    <row r="289" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A289" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B289" t="s">
+        <v>661</v>
+      </c>
+      <c r="C289" t="s">
+        <v>1532</v>
+      </c>
+    </row>
+    <row r="290" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A290" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B290" t="s">
+        <v>662</v>
+      </c>
+      <c r="C290" t="s">
+        <v>1533</v>
+      </c>
+    </row>
+    <row r="291" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A291" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B291" t="s">
+        <v>663</v>
+      </c>
+      <c r="C291" t="s">
+        <v>1534</v>
+      </c>
+    </row>
+    <row r="292" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A292" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B292" t="s">
+        <v>664</v>
+      </c>
+      <c r="C292" t="s">
+        <v>1512</v>
+      </c>
+    </row>
+    <row r="293" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A293" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B293" t="s">
+        <v>665</v>
+      </c>
+      <c r="C293" t="s">
+        <v>1513</v>
+      </c>
+    </row>
+    <row r="294" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A294" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B294" t="s">
+        <v>667</v>
+      </c>
+      <c r="C294" t="s">
+        <v>1515</v>
+      </c>
+    </row>
+    <row r="295" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A295" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B295" t="s">
+        <v>666</v>
+      </c>
+      <c r="C295" t="s">
+        <v>1514</v>
+      </c>
+    </row>
+    <row r="296" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A296" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B296" t="s">
+        <v>669</v>
+      </c>
+      <c r="C296" t="s">
+        <v>1517</v>
+      </c>
+    </row>
+    <row r="297" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A297" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B297" t="s">
+        <v>668</v>
+      </c>
+      <c r="C297" t="s">
+        <v>1516</v>
+      </c>
+    </row>
+    <row r="298" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A298" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B298" t="s">
+        <v>670</v>
+      </c>
+      <c r="C298" t="s">
+        <v>1535</v>
+      </c>
+    </row>
+    <row r="299" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A299" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B299" t="s">
+        <v>671</v>
+      </c>
+      <c r="C299" t="s">
+        <v>1537</v>
+      </c>
+    </row>
+    <row r="300" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A300" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B300" t="s">
+        <v>1090</v>
+      </c>
+      <c r="C300" t="s">
+        <v>1536</v>
+      </c>
+    </row>
+    <row r="301" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A301" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B301" t="s">
+        <v>672</v>
+      </c>
+      <c r="C301" t="s">
+        <v>1538</v>
+      </c>
+    </row>
+    <row r="302" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A302" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B302" t="s">
+        <v>673</v>
+      </c>
+      <c r="C302" t="s">
+        <v>1539</v>
+      </c>
+    </row>
+    <row r="303" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A303" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B303" t="s">
+        <v>577</v>
+      </c>
+      <c r="C303" t="s">
+        <v>1540</v>
+      </c>
+    </row>
+    <row r="304" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A304" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B304" t="s">
+        <v>674</v>
+      </c>
+      <c r="C304" t="s">
+        <v>1541</v>
+      </c>
+    </row>
+    <row r="305" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A305" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B305" t="s">
+        <v>675</v>
+      </c>
+      <c r="C305" t="s">
+        <v>1542</v>
+      </c>
+    </row>
+    <row r="306" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A306" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B306" t="s">
+        <v>676</v>
+      </c>
+      <c r="C306" t="s">
+        <v>1543</v>
+      </c>
+    </row>
+    <row r="307" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A307" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B307" t="s">
+        <v>677</v>
+      </c>
+      <c r="C307" t="s">
+        <v>1544</v>
+      </c>
+    </row>
+    <row r="308" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A308" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B308" t="s">
+        <v>1063</v>
+      </c>
+      <c r="C308" t="s">
+        <v>1521</v>
+      </c>
+    </row>
+    <row r="309" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A309" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B309" t="s">
+        <v>1064</v>
+      </c>
+      <c r="C309" t="s">
+        <v>1519</v>
+      </c>
+    </row>
+    <row r="310" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A310" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B310" t="s">
+        <v>1065</v>
+      </c>
+      <c r="C310" t="s">
+        <v>1520</v>
+      </c>
+    </row>
+    <row r="311" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A311" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B311" t="s">
+        <v>678</v>
+      </c>
+      <c r="C311" t="s">
+        <v>1522</v>
+      </c>
+    </row>
+    <row r="312" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A312" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B312" t="s">
+        <v>679</v>
+      </c>
+      <c r="C312" t="s">
+        <v>1523</v>
+      </c>
+    </row>
+    <row r="313" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A313" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B313" t="s">
+        <v>1066</v>
+      </c>
+      <c r="C313" t="s">
+        <v>1524</v>
+      </c>
+    </row>
+    <row r="314" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A314" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B314" t="s">
+        <v>1091</v>
+      </c>
+      <c r="C314" t="s">
+        <v>1545</v>
+      </c>
+    </row>
+    <row r="315" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A315" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B315" t="s">
+        <v>680</v>
+      </c>
+      <c r="C315" t="s">
+        <v>1547</v>
+      </c>
+    </row>
+    <row r="316" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A316" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B316" t="s">
+        <v>681</v>
+      </c>
+      <c r="C316" t="s">
+        <v>1546</v>
+      </c>
+    </row>
+    <row r="317" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A317" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B317" t="s">
+        <v>742</v>
+      </c>
+      <c r="C317" t="s">
+        <v>1548</v>
+      </c>
+    </row>
+    <row r="318" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A318" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B318" t="s">
+        <v>684</v>
+      </c>
+      <c r="C318" t="s">
+        <v>1551</v>
+      </c>
+    </row>
+    <row r="319" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A319" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B319" t="s">
+        <v>682</v>
+      </c>
+      <c r="C319" t="s">
+        <v>1549</v>
+      </c>
+    </row>
+    <row r="320" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A320" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B320" t="s">
+        <v>683</v>
+      </c>
+      <c r="C320" t="s">
+        <v>1550</v>
+      </c>
+    </row>
+    <row r="321" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A321" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B321" t="s">
+        <v>685</v>
+      </c>
+      <c r="C321" t="s">
+        <v>1553</v>
+      </c>
+    </row>
+    <row r="322" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A322" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B322" t="s">
+        <v>1059</v>
+      </c>
+      <c r="C322" t="s">
+        <v>1552</v>
+      </c>
+    </row>
+    <row r="323" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A323" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B323" t="s">
+        <v>686</v>
+      </c>
+      <c r="C323" t="s">
+        <v>1527</v>
+      </c>
+    </row>
+    <row r="324" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A324" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B324" t="s">
+        <v>687</v>
+      </c>
+      <c r="C324" t="s">
+        <v>1554</v>
+      </c>
+    </row>
+    <row r="325" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A325" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B325" t="s">
+        <v>1234</v>
+      </c>
+      <c r="C325" t="s">
+        <v>1213</v>
+      </c>
+    </row>
+    <row r="326" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A326" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B326" t="s">
+        <v>765</v>
+      </c>
+      <c r="C326" t="s">
+        <v>1526</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="C1:D325">
+    <sortCondition ref="D1:D325"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>